<commit_message>
caseworker-bulkscan ccd role + user
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitinprabhu/hmcts/platform/bulk-scan-orchestrator/docker/ccd-definition-import/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C5F8DC-3D17-9E4B-89E2-C8D52072DA99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26820" windowHeight="13040" tabRatio="500" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="1340" windowWidth="26820" windowHeight="13040" tabRatio="500" firstSheet="16" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -33,8 +27,11 @@
     <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId18"/>
     <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -802,9 +799,6 @@
     <t>caseworker-sscs-systemupdate</t>
   </si>
   <si>
-    <t>caseworker-sscs</t>
-  </si>
-  <si>
     <t>caseworker-sscs-callagent</t>
   </si>
   <si>
@@ -847,18 +841,21 @@
     <t>Exception Records</t>
   </si>
   <si>
-    <t>SSCS</t>
+    <t>bulkscan</t>
+  </si>
+  <si>
+    <t>caseworker-bulkscan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1051,6 +1048,14 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1360,10 +1365,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1628,8 +1639,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1757,7 +1774,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1809,7 +1826,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2003,29 +2020,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="40.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2034,7 +2050,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="25.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2051,9 +2067,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2065,22 +2081,22 @@
         <v>43383</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="6"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="5"/>
       <c r="C6" s="2"/>
       <c r="D6" s="6"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="5"/>
       <c r="C7" s="2"/>
       <c r="D7" s="6"/>
@@ -2093,18 +2109,23 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048563"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
@@ -2119,7 +2140,7 @@
     <col min="28" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
         <v>215</v>
       </c>
@@ -2139,7 +2160,7 @@
       <c r="I1" s="48"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="C2" s="17" t="s">
         <v>12</v>
       </c>
@@ -2162,7 +2183,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -2209,13 +2230,13 @@
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" ht="12.75" customHeight="1">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>223</v>
@@ -2236,13 +2257,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" ht="12.75" customHeight="1">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>223</v>
@@ -2263,13 +2284,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>223</v>
@@ -2290,13 +2311,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27" ht="12.75" customHeight="1">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" s="33" t="s">
         <v>223</v>
@@ -2317,13 +2338,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" ht="12.75" customHeight="1">
       <c r="A8" s="15">
         <v>43101</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>223</v>
@@ -2344,13 +2365,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" ht="12.75" customHeight="1">
       <c r="A9" s="15">
         <v>43101</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>223</v>
@@ -2371,13 +2392,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" ht="12.75" customHeight="1">
       <c r="A10" s="15">
         <v>43101</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>223</v>
@@ -2398,13 +2419,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" ht="12.75" customHeight="1">
       <c r="A11" s="15">
         <v>43101</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>223</v>
@@ -2425,13 +2446,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27" ht="12.75" customHeight="1">
       <c r="A12" s="15">
         <v>43101</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>223</v>
@@ -2452,13 +2473,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27" ht="12.75" customHeight="1">
       <c r="A13" s="15">
         <v>43101</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>223</v>
@@ -2479,13 +2500,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" ht="12.75" customHeight="1">
       <c r="A14" s="15">
         <v>43101</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="33" t="s">
         <v>223</v>
@@ -2506,13 +2527,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:27" ht="12.75" customHeight="1">
       <c r="A15" s="15">
         <v>43101</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>223</v>
@@ -2533,13 +2554,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:27" ht="12.75" customHeight="1">
       <c r="A16" s="15">
         <v>43101</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D16" s="33" t="s">
         <v>223</v>
@@ -2560,13 +2581,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="12.75" customHeight="1">
       <c r="A17" s="15">
         <v>43101</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" s="33" t="s">
         <v>223</v>
@@ -2587,13 +2608,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="12.75" customHeight="1">
       <c r="A18" s="15">
         <v>43101</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="33" t="s">
         <v>223</v>
@@ -2614,13 +2635,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="12.75" customHeight="1">
       <c r="A19" s="15">
         <v>43101</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>223</v>
@@ -2641,33 +2662,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1048562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1048562" ht="12.75" customHeight="1"/>
+    <row r="1048563" ht="12.75" customHeight="1"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B19" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B19">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView topLeftCell="N2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="N2" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
@@ -2680,7 +2706,7 @@
     <col min="28" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
         <v>228</v>
       </c>
@@ -2700,7 +2726,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="19" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="19" customFormat="1" ht="37">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
@@ -2737,7 +2763,7 @@
       <c r="Z2" s="75"/>
       <c r="AA2" s="75"/>
     </row>
-    <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="14">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -2778,13 +2804,13 @@
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
     </row>
-    <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="14">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -2817,13 +2843,13 @@
       <c r="Z4" s="77"/>
       <c r="AA4" s="77"/>
     </row>
-    <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="14">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" t="s">
         <v>225</v>
@@ -2856,13 +2882,13 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>45</v>
@@ -2876,29 +2902,34 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B6">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -2910,7 +2941,7 @@
     <col min="28" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
         <v>231</v>
       </c>
@@ -2930,7 +2961,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="19" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="19" customFormat="1" ht="37">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
@@ -2967,7 +2998,7 @@
       <c r="Z2" s="75"/>
       <c r="AA2" s="75"/>
     </row>
-    <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="14">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -3008,13 +3039,13 @@
       <c r="Z3" s="78"/>
       <c r="AA3" s="78"/>
     </row>
-    <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="14">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -3047,13 +3078,13 @@
       <c r="Z4" s="78"/>
       <c r="AA4" s="78"/>
     </row>
-    <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="14">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" t="s">
         <v>225</v>
@@ -3086,13 +3117,13 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="14">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>45</v>
@@ -3125,13 +3156,13 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
@@ -3145,29 +3176,34 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B5:B7" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B5:B7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.1640625" style="28" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="79" customWidth="1"/>
@@ -3177,7 +3213,7 @@
     <col min="7" max="1025" width="7.1640625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" ht="18">
       <c r="A1" s="80" t="s">
         <v>233</v>
       </c>
@@ -4211,7 +4247,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" ht="48" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1024" ht="42">
       <c r="A2" s="85"/>
       <c r="B2" s="85"/>
       <c r="C2" s="86" t="s">
@@ -5245,7 +5281,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" ht="15" customHeight="1">
       <c r="A3" s="87" t="s">
         <v>15</v>
       </c>
@@ -6283,13 +6319,13 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1024" ht="15" customHeight="1">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -6301,13 +6337,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1024" ht="12">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" t="s">
         <v>225</v>
@@ -6319,13 +6355,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:1024" ht="13" customHeight="1">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>45</v>
@@ -6339,29 +6375,34 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B6">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.5" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
@@ -6374,7 +6415,7 @@
     <col min="28" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="25.5" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>237</v>
       </c>
@@ -6394,7 +6435,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="19" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="19" customFormat="1" ht="36">
       <c r="C2" s="17" t="s">
         <v>32</v>
       </c>
@@ -6408,7 +6449,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="14">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -6449,13 +6490,13 @@
       <c r="Z3" s="78"/>
       <c r="AA3" s="78"/>
     </row>
-    <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="14">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -6488,13 +6529,13 @@
       <c r="Z4" s="78"/>
       <c r="AA4" s="78"/>
     </row>
-    <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="14">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" t="s">
         <v>225</v>
@@ -6527,13 +6568,13 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="14">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>45</v>
@@ -6566,13 +6607,13 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
@@ -6586,29 +6627,34 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0D00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B5:B7" xr:uid="{00000000-0002-0000-0D00-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B5:B7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="30.83203125" customWidth="1"/>
@@ -6619,7 +6665,7 @@
     <col min="8" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="28" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="28" customFormat="1" ht="25.5" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>238</v>
       </c>
@@ -6640,11 +6686,11 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12">
       <c r="D2"/>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" s="28" customFormat="1">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -6664,25 +6710,25 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="89" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12">
       <c r="A5" s="15"/>
       <c r="B5" s="5"/>
       <c r="C5" s="89"/>
@@ -6690,7 +6736,7 @@
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12">
       <c r="A6" s="15"/>
       <c r="B6" s="5"/>
       <c r="C6" s="89"/>
@@ -6698,7 +6744,7 @@
       <c r="E6" s="33"/>
       <c r="F6" s="33"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12">
       <c r="A7" s="15"/>
       <c r="B7" s="5"/>
       <c r="C7" s="89"/>
@@ -6706,7 +6752,7 @@
       <c r="E7" s="33"/>
       <c r="F7" s="33"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12">
       <c r="A8" s="15"/>
       <c r="B8" s="5"/>
       <c r="C8" s="33"/>
@@ -6714,7 +6760,7 @@
       <c r="E8" s="33"/>
       <c r="F8" s="33"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12">
       <c r="A9" s="15"/>
       <c r="B9" s="5"/>
       <c r="C9" s="89"/>
@@ -6722,7 +6768,7 @@
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12">
       <c r="A10" s="15"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -6730,7 +6776,7 @@
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12">
       <c r="A11" s="15"/>
       <c r="B11" s="5"/>
       <c r="C11" s="33"/>
@@ -6738,7 +6784,7 @@
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12">
       <c r="A12" s="15"/>
       <c r="B12" s="5"/>
       <c r="C12" s="33"/>
@@ -6746,7 +6792,7 @@
       <c r="E12" s="33"/>
       <c r="F12" s="33"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12">
       <c r="A13" s="15"/>
       <c r="B13" s="5"/>
       <c r="C13" s="33"/>
@@ -6754,7 +6800,7 @@
       <c r="E13" s="33"/>
       <c r="F13" s="33"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12">
       <c r="A14" s="15"/>
       <c r="B14" s="5"/>
       <c r="C14" s="33"/>
@@ -6762,7 +6808,7 @@
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12">
       <c r="A15" s="15"/>
       <c r="B15" s="5"/>
       <c r="C15" s="33"/>
@@ -6770,7 +6816,7 @@
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12">
       <c r="A16" s="15"/>
       <c r="B16" s="5"/>
       <c r="C16" s="89"/>
@@ -6778,7 +6824,7 @@
       <c r="E16" s="33"/>
       <c r="F16" s="33"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6">
       <c r="A17" s="15"/>
       <c r="B17" s="5"/>
       <c r="C17" s="33"/>
@@ -6786,7 +6832,7 @@
       <c r="E17" s="33"/>
       <c r="F17" s="33"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6">
       <c r="A18" s="15"/>
       <c r="B18" s="5"/>
       <c r="C18" s="33"/>
@@ -6794,63 +6840,63 @@
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6">
       <c r="A19" s="15"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6">
       <c r="A20" s="15"/>
       <c r="C20" s="5"/>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="33"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6">
       <c r="A21" s="15"/>
       <c r="C21" s="5"/>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="33"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6">
       <c r="A22" s="15"/>
       <c r="C22" s="5"/>
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
       <c r="F22" s="33"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6">
       <c r="A23" s="15"/>
       <c r="C23" s="5"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
       <c r="F23" s="33"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6">
       <c r="A24" s="15"/>
       <c r="C24" s="5"/>
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6">
       <c r="A25" s="15"/>
       <c r="C25" s="5"/>
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="33"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6">
       <c r="A26" s="15"/>
       <c r="C26" s="5"/>
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="33"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6">
       <c r="A27" s="15"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -6858,7 +6904,7 @@
       <c r="E27" s="33"/>
       <c r="F27" s="33"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6">
       <c r="A28" s="15"/>
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
@@ -6867,18 +6913,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
@@ -6888,7 +6939,7 @@
     <col min="6" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" s="7" t="s">
         <v>243</v>
       </c>
@@ -6908,7 +6959,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="19" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="19" customFormat="1" ht="72">
       <c r="C2" s="17" t="s">
         <v>12</v>
       </c>
@@ -6919,7 +6970,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10">
       <c r="A3" s="66" t="s">
         <v>15</v>
       </c>
@@ -6936,13 +6987,13 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>248</v>
@@ -6952,32 +7003,32 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="E5" s="28" t="s">
         <v>247</v>
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10">
       <c r="A6" s="15">
         <v>43102</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>247</v>
@@ -6985,25 +7036,30 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0F00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C51"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
@@ -7014,9 +7070,9 @@
     <col min="7" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>9</v>
@@ -7033,7 +7089,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="60">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
@@ -7070,7 +7126,7 @@
       <c r="Z2" s="12"/>
       <c r="AA2" s="12"/>
     </row>
-    <row r="3" spans="1:27" s="66" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" s="66" customFormat="1">
       <c r="A3" s="66" t="s">
         <v>15</v>
       </c>
@@ -7090,13 +7146,13 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27">
       <c r="A4" s="90">
         <v>43101</v>
       </c>
       <c r="B4" s="91"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="93" t="s">
         <v>45</v>
@@ -7108,12 +7164,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27">
       <c r="A5" s="96">
         <v>43101</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>47</v>
@@ -7125,12 +7181,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27">
       <c r="A6" s="96">
         <v>43101</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>50</v>
@@ -7142,12 +7198,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27">
       <c r="A7" s="96">
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>52</v>
@@ -7159,12 +7215,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27">
       <c r="A8" s="96">
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>54</v>
@@ -7176,12 +7232,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27">
       <c r="A9" s="96">
         <v>43101</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>56</v>
@@ -7193,12 +7249,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27">
       <c r="A10" s="96">
         <v>43101</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>58</v>
@@ -7210,12 +7266,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27">
       <c r="A11" s="96">
         <v>43101</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>60</v>
@@ -7227,12 +7283,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27">
       <c r="A12" s="96">
         <v>43101</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>61</v>
@@ -7244,12 +7300,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27">
       <c r="A13" s="96">
         <v>43101</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>64</v>
@@ -7261,12 +7317,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27">
       <c r="A14" s="96">
         <v>43101</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>66</v>
@@ -7278,12 +7334,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:27">
       <c r="A15" s="96">
         <v>43101</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>68</v>
@@ -7295,12 +7351,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:27">
       <c r="A16" s="96">
         <v>43101</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>70</v>
@@ -7312,12 +7368,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6">
       <c r="A17" s="96">
         <v>43101</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>72</v>
@@ -7329,12 +7385,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6">
       <c r="A18" s="96">
         <v>43101</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>75</v>
@@ -7346,12 +7402,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6">
       <c r="A19" s="96">
         <v>43101</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>78</v>
@@ -7363,548 +7419,548 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6">
       <c r="A20" s="90">
         <v>43101</v>
       </c>
       <c r="B20" s="91"/>
       <c r="C20" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D20" s="93" t="s">
         <v>45</v>
       </c>
       <c r="E20" s="92" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F20" s="95" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6">
       <c r="A21" s="96">
         <v>43101</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F21" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6">
       <c r="A22" s="96">
         <v>43101</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>50</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F22" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6">
       <c r="A23" s="96">
         <v>43101</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>52</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F23" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6">
       <c r="A24" s="96">
         <v>43101</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>54</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F24" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6">
       <c r="A25" s="96">
         <v>43101</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F25" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6">
       <c r="A26" s="96">
         <v>43101</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D26" s="26" t="s">
         <v>58</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F26" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6">
       <c r="A27" s="96">
         <v>43101</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>60</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F27" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6">
       <c r="A28" s="96">
         <v>43101</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F28" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6">
       <c r="A29" s="96">
         <v>43101</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>64</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F29" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6">
       <c r="A30" s="96">
         <v>43101</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F30" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6">
       <c r="A31" s="96">
         <v>43101</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>68</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F31" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6">
       <c r="A32" s="96">
         <v>43101</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>70</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F32" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6">
       <c r="A33" s="96">
         <v>43101</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>72</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F33" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6">
       <c r="A34" s="96">
         <v>43101</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D34" s="25" t="s">
         <v>75</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F34" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6">
       <c r="A35" s="96">
         <v>43101</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D35" s="25" t="s">
         <v>78</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F35" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6">
       <c r="A36" s="90">
         <v>43101</v>
       </c>
       <c r="B36" s="91"/>
       <c r="C36" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D36" s="93" t="s">
         <v>45</v>
       </c>
       <c r="E36" s="92" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="F36" s="95" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6">
       <c r="A37" s="96">
         <v>43101</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>249</v>
+      <c r="E37" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F37" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6">
       <c r="A38" s="96">
         <v>43101</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>249</v>
+      <c r="E38" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F38" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6">
       <c r="A39" s="96">
         <v>43101</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D39" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>249</v>
+      <c r="E39" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F39" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6">
       <c r="A40" s="96">
         <v>43101</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>249</v>
+      <c r="E40" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F40" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6">
       <c r="A41" s="96">
         <v>43101</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D41" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>249</v>
+      <c r="E41" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F41" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6">
       <c r="A42" s="96">
         <v>43101</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D42" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>249</v>
+      <c r="E42" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F42" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6">
       <c r="A43" s="96">
         <v>43101</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D43" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>249</v>
+      <c r="E43" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F43" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6">
       <c r="A44" s="96">
         <v>43101</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D44" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>249</v>
+      <c r="E44" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F44" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6">
       <c r="A45" s="96">
         <v>43101</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>249</v>
+      <c r="E45" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F45" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6">
       <c r="A46" s="96">
         <v>43101</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D46" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>249</v>
+      <c r="E46" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F46" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6">
       <c r="A47" s="96">
         <v>43101</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D47" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E47" s="5" t="s">
-        <v>249</v>
+      <c r="E47" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F47" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6">
       <c r="A48" s="96">
         <v>43101</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>249</v>
+      <c r="E48" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F48" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6">
       <c r="A49" s="96">
         <v>43101</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>249</v>
+      <c r="E49" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F49" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6">
       <c r="A50" s="96">
         <v>43101</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>249</v>
+      <c r="E50" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F50" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6">
       <c r="A51" s="98">
         <v>43101</v>
       </c>
       <c r="B51" s="99"/>
       <c r="C51" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D51" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="E51" s="100" t="s">
-        <v>249</v>
+      <c r="E51" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F51" s="102" t="s">
         <v>247</v>
@@ -7912,25 +7968,30 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A51" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A51">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E4:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -7941,9 +8002,9 @@
     <col min="7" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="107" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="107" customFormat="1" ht="34">
       <c r="A1" s="103" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="104" t="s">
         <v>9</v>
@@ -7961,7 +8022,7 @@
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
     </row>
-    <row r="2" spans="1:27" s="19" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="19" customFormat="1" ht="36">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
@@ -7971,7 +8032,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>245</v>
@@ -7998,7 +8059,7 @@
       <c r="Z2" s="18"/>
       <c r="AA2" s="18"/>
     </row>
-    <row r="3" spans="1:27" s="66" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" s="66" customFormat="1">
       <c r="A3" s="66" t="s">
         <v>15</v>
       </c>
@@ -8018,103 +8079,103 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27">
       <c r="A4" s="90">
         <v>43101</v>
       </c>
       <c r="B4" s="91"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="108" t="s">
         <v>179</v>
       </c>
-      <c r="E4" s="94" t="s">
-        <v>249</v>
+      <c r="E4" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F4" s="95" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27">
       <c r="A5" s="96">
         <v>43101</v>
       </c>
       <c r="B5" s="109"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="E5" s="110" t="s">
-        <v>249</v>
+      <c r="E5" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F5" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27">
       <c r="A6" s="96">
         <v>43101</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>249</v>
+      <c r="E6" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F6" s="111" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27">
       <c r="A7" s="96">
         <v>43101</v>
       </c>
       <c r="B7" s="110"/>
       <c r="C7" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" s="54" t="s">
         <v>187</v>
       </c>
-      <c r="E7" s="110" t="s">
-        <v>249</v>
+      <c r="E7" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F7" s="97" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27">
       <c r="A8" s="98">
         <v>43101</v>
       </c>
       <c r="B8" s="112"/>
       <c r="C8" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="113" t="s">
         <v>189</v>
       </c>
-      <c r="E8" s="112" t="s">
-        <v>249</v>
+      <c r="E8" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F8" s="102" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27">
       <c r="A9" s="90">
         <v>43101</v>
       </c>
       <c r="B9" s="92"/>
       <c r="C9" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" s="114" t="s">
         <v>182</v>
@@ -8126,13 +8187,13 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27">
       <c r="A10" s="96">
         <v>43101</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="53" t="s">
         <v>185</v>
@@ -8144,13 +8205,13 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27">
       <c r="A11" s="98">
         <v>43101</v>
       </c>
       <c r="B11" s="112"/>
       <c r="C11" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" s="116" t="s">
         <v>187</v>
@@ -8162,55 +8223,55 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27">
       <c r="A12" s="90">
         <v>43101</v>
       </c>
       <c r="B12" s="94"/>
       <c r="C12" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="114" t="s">
         <v>182</v>
       </c>
       <c r="E12" s="92" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F12" s="95" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27">
       <c r="A13" s="96">
         <v>43101</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="53" t="s">
         <v>185</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F13" s="111" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27">
       <c r="A14" s="98">
         <v>43101</v>
       </c>
       <c r="B14" s="112"/>
       <c r="C14" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="116" t="s">
         <v>187</v>
       </c>
       <c r="E14" s="100" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F14" s="117" t="s">
         <v>247</v>
@@ -8218,25 +8279,30 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-1100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.1640625" style="118" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="118" customWidth="1"/>
@@ -8248,9 +8314,9 @@
     <col min="256" max="1025" width="7.1640625" style="118" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="129" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:255" s="129" customFormat="1" ht="34">
       <c r="A1" s="120" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="121" t="s">
         <v>9</v>
@@ -8513,7 +8579,7 @@
       <c r="IT1" s="127"/>
       <c r="IU1" s="128"/>
     </row>
-    <row r="2" spans="1:255" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:255" ht="24">
       <c r="A2" s="130"/>
       <c r="B2" s="130"/>
       <c r="C2" s="131" t="s">
@@ -8523,7 +8589,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="131" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F2" s="132" t="s">
         <v>245</v>
@@ -8778,7 +8844,7 @@
       <c r="IT2" s="134"/>
       <c r="IU2" s="135"/>
     </row>
-    <row r="3" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:255">
       <c r="A3" s="136" t="s">
         <v>15</v>
       </c>
@@ -8789,7 +8855,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="137" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E3" s="137" t="s">
         <v>246</v>
@@ -9047,67 +9113,67 @@
       <c r="IT3" s="141"/>
       <c r="IU3" s="142"/>
     </row>
-    <row r="4" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:255">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="143" t="s">
         <v>156</v>
       </c>
-      <c r="E4" s="94" t="s">
-        <v>249</v>
+      <c r="E4" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F4" s="144" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:255">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="145" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>249</v>
+      <c r="E5" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F5" s="146" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:255">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="147" t="s">
         <v>160</v>
       </c>
-      <c r="E6" s="112" t="s">
-        <v>249</v>
+      <c r="E6" s="92" t="s">
+        <v>264</v>
       </c>
       <c r="F6" s="148" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:255">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" s="143" t="s">
         <v>156</v>
@@ -9119,13 +9185,13 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:255">
       <c r="A8" s="15">
         <v>43101</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="145" t="s">
         <v>158</v>
@@ -9137,13 +9203,13 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:255">
       <c r="A9" s="15">
         <v>43101</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" s="147" t="s">
         <v>160</v>
@@ -9155,55 +9221,55 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:255">
       <c r="A10" s="15">
         <v>43101</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="143" t="s">
         <v>156</v>
       </c>
       <c r="E10" s="92" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F10" s="144" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:255">
       <c r="A11" s="15">
         <v>43101</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" s="145" t="s">
         <v>158</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F11" s="146" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:255" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:255">
       <c r="A12" s="15">
         <v>43101</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="147" t="s">
         <v>160</v>
       </c>
       <c r="E12" s="100" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F12" s="148" t="s">
         <v>247</v>
@@ -9211,25 +9277,30 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12" xr:uid="{00000000-0002-0000-1200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -9240,7 +9311,7 @@
     <col min="28" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -9260,7 +9331,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="12.75" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
@@ -9295,7 +9366,7 @@
       <c r="Z2" s="12"/>
       <c r="AA2" s="12"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -9334,46 +9405,51 @@
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" ht="12.75" customHeight="1">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
@@ -9387,7 +9463,7 @@
     <col min="10" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -9407,7 +9483,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="19" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="19" customFormat="1" ht="60">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
@@ -9450,7 +9526,7 @@
       <c r="Z2" s="18"/>
       <c r="AA2" s="18"/>
     </row>
-    <row r="3" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -9497,21 +9573,21 @@
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="C4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>259</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -9521,25 +9597,30 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
@@ -9555,7 +9636,7 @@
     <col min="27" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="17">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -9574,7 +9655,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:26" s="19" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" s="19" customFormat="1" ht="51.75" customHeight="1">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
@@ -9618,7 +9699,7 @@
       <c r="Y2" s="18"/>
       <c r="Z2" s="18"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -9670,13 +9751,13 @@
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>45</v>
@@ -9693,13 +9774,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>47</v>
@@ -9716,13 +9797,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>50</v>
@@ -9739,13 +9820,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>52</v>
@@ -9762,13 +9843,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="A8" s="15">
         <v>43101</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>54</v>
@@ -9785,13 +9866,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" ht="12.75" customHeight="1">
       <c r="A9" s="15">
         <v>43101</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>56</v>
@@ -9808,13 +9889,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" ht="12.75" customHeight="1">
       <c r="A10" s="15">
         <v>43101</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>58</v>
@@ -9831,13 +9912,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="A11" s="15">
         <v>43101</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>60</v>
@@ -9854,13 +9935,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" ht="12.75" customHeight="1">
       <c r="A12" s="15">
         <v>43101</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>61</v>
@@ -9877,13 +9958,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" ht="12.75" customHeight="1">
       <c r="A13" s="15">
         <v>43101</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>64</v>
@@ -9900,13 +9981,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" ht="12.75" customHeight="1">
       <c r="A14" s="15">
         <v>43101</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>66</v>
@@ -9923,13 +10004,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" ht="12.75" customHeight="1">
       <c r="A15" s="15">
         <v>43101</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>68</v>
@@ -9946,13 +10027,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" ht="12.75" customHeight="1">
       <c r="A16" s="15">
         <v>43101</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>70</v>
@@ -9969,13 +10050,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="12.75" customHeight="1">
       <c r="A17" s="15">
         <v>43101</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>72</v>
@@ -9992,13 +10073,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="12.75" customHeight="1">
       <c r="A18" s="15">
         <v>43101</v>
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>75</v>
@@ -10017,13 +10098,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="12.75" customHeight="1">
       <c r="A19" s="15">
         <v>43101</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>78</v>
@@ -10042,32 +10123,37 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="1:10" ht="12.75" customHeight="1"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B19" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B19">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -10085,7 +10171,7 @@
     <col min="29" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="17">
       <c r="A1" s="7" t="s">
         <v>81</v>
       </c>
@@ -10106,7 +10192,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" ht="51.75" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
@@ -10156,7 +10242,7 @@
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
     </row>
-    <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -10214,7 +10300,7 @@
       <c r="AA3" s="13"/>
       <c r="AB3" s="13"/>
     </row>
-    <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" ht="12.75" customHeight="1">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
@@ -10246,7 +10332,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="12.75" customHeight="1">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
@@ -10277,7 +10363,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="12.75" customHeight="1">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
@@ -10310,7 +10396,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="12.75" customHeight="1">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
@@ -10341,7 +10427,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="12.75" customHeight="1">
       <c r="A8" s="15">
         <v>43101</v>
       </c>
@@ -10372,7 +10458,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" ht="12.75" customHeight="1">
       <c r="A9" s="15">
         <v>43101</v>
       </c>
@@ -10403,7 +10489,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="12.75" customHeight="1">
       <c r="A10" s="15">
         <v>43101</v>
       </c>
@@ -10434,7 +10520,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" ht="12.75" customHeight="1">
       <c r="A11" s="15">
         <v>43101</v>
       </c>
@@ -10467,25 +10553,30 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -10495,7 +10586,7 @@
     <col min="28" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
         <v>106</v>
       </c>
@@ -10515,7 +10606,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
@@ -10550,7 +10641,7 @@
       <c r="Z2" s="18"/>
       <c r="AA2" s="18"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -10589,7 +10680,7 @@
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" ht="12.75" customHeight="1">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
@@ -10616,7 +10707,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" ht="12.75" customHeight="1">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
@@ -10643,7 +10734,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
@@ -10670,7 +10761,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27" ht="12.75" customHeight="1">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
@@ -10697,7 +10788,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" ht="12.75" customHeight="1">
       <c r="A8" s="15">
         <v>43101</v>
       </c>
@@ -10724,7 +10815,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" ht="12.75" customHeight="1">
       <c r="A9" s="15">
         <v>43101</v>
       </c>
@@ -10751,7 +10842,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" ht="12.75" customHeight="1">
       <c r="A10" s="15">
         <v>43101</v>
       </c>
@@ -10778,7 +10869,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" ht="12.75" customHeight="1">
       <c r="A11" s="15">
         <v>43101</v>
       </c>
@@ -10805,7 +10896,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27" ht="12.75" customHeight="1">
       <c r="A12" s="15">
         <v>43101</v>
       </c>
@@ -10832,7 +10923,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27" ht="12.75" customHeight="1">
       <c r="A13" s="15">
         <v>43101</v>
       </c>
@@ -10859,7 +10950,7 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
     </row>
-    <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" ht="12.75" customHeight="1">
       <c r="A14" s="15">
         <v>43101</v>
       </c>
@@ -10886,7 +10977,7 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
     </row>
-    <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:27" ht="12.75" customHeight="1">
       <c r="A15" s="15">
         <v>43101</v>
       </c>
@@ -10913,7 +11004,7 @@
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
     </row>
-    <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:27" ht="12.75" customHeight="1">
       <c r="A16" s="15">
         <v>43101</v>
       </c>
@@ -10940,7 +11031,7 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
     </row>
-    <row r="17" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" ht="12.75" customHeight="1">
       <c r="A17" s="15">
         <v>43101</v>
       </c>
@@ -10967,7 +11058,7 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
     </row>
-    <row r="18" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" ht="12.75" customHeight="1">
       <c r="A18" s="15">
         <v>43101</v>
       </c>
@@ -10994,7 +11085,7 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
     </row>
-    <row r="19" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" ht="12.75" customHeight="1">
       <c r="A19" s="15">
         <v>43101</v>
       </c>
@@ -11021,7 +11112,7 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="20" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" ht="12.75" customHeight="1">
       <c r="A20" s="15">
         <v>43101</v>
       </c>
@@ -11048,7 +11139,7 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
     </row>
-    <row r="21" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" ht="12.75" customHeight="1">
       <c r="A21" s="15">
         <v>43101</v>
       </c>
@@ -11075,7 +11166,7 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" ht="12.75" customHeight="1">
       <c r="A22" s="15">
         <v>43101</v>
       </c>
@@ -11102,7 +11193,7 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
     </row>
-    <row r="23" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" ht="12.75" customHeight="1">
       <c r="A23" s="15">
         <v>43101</v>
       </c>
@@ -11129,7 +11220,7 @@
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
     </row>
-    <row r="24" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" ht="12.75" customHeight="1">
       <c r="A24" s="15">
         <v>43101</v>
       </c>
@@ -11156,7 +11247,7 @@
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
     </row>
-    <row r="25" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" ht="12.75" customHeight="1">
       <c r="A25" s="15">
         <v>43101</v>
       </c>
@@ -11185,25 +11276,30 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -11216,7 +11312,7 @@
     <col min="28" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
         <v>153</v>
       </c>
@@ -11236,7 +11332,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="61" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="61" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -11269,7 +11365,7 @@
       <c r="Z2" s="12"/>
       <c r="AA2" s="12"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" ht="12.75" customHeight="1">
       <c r="A3" s="40" t="s">
         <v>15</v>
       </c>
@@ -11292,13 +11388,13 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" ht="12.75" customHeight="1">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>156</v>
@@ -11313,13 +11409,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" ht="12.75" customHeight="1">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>158</v>
@@ -11334,12 +11430,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>160</v>
@@ -11356,33 +11452,38 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B5">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G6" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G6">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
@@ -11406,7 +11507,7 @@
     <col min="30" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="17">
       <c r="A1" s="7" t="s">
         <v>162</v>
       </c>
@@ -11433,7 +11534,7 @@
       <c r="R1" s="44"/>
       <c r="S1" s="44"/>
     </row>
-    <row r="2" spans="1:29" ht="98" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" ht="84">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
@@ -11494,7 +11595,7 @@
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
     </row>
-    <row r="3" spans="1:29" ht="45" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" ht="39">
       <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
@@ -11563,13 +11664,13 @@
       <c r="AB3" s="13"/>
       <c r="AC3" s="13"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="47" t="s">
         <v>179</v>
@@ -11595,13 +11696,13 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="51" t="s">
         <v>182</v>
@@ -11636,13 +11737,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>185</v>
@@ -11677,13 +11778,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" s="54" t="s">
         <v>187</v>
@@ -11718,13 +11819,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29">
       <c r="A8" s="15">
         <v>43466</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="55" t="s">
         <v>189</v>
@@ -11756,33 +11857,38 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B8">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G8" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G8">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -11802,7 +11908,7 @@
     <col min="29" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="17">
       <c r="A1" s="7" t="s">
         <v>192</v>
       </c>
@@ -11824,7 +11930,7 @@
       <c r="K1"/>
       <c r="M1"/>
     </row>
-    <row r="2" spans="1:28" s="58" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" s="58" customFormat="1" ht="54.75" customHeight="1">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39" t="s">
@@ -11878,7 +11984,7 @@
       <c r="AA2" s="29"/>
       <c r="AB2" s="29"/>
     </row>
-    <row r="3" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" ht="21.75" customHeight="1">
       <c r="A3" s="59" t="s">
         <v>15</v>
       </c>
@@ -11922,13 +12028,13 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28">
       <c r="A4" s="15">
         <v>43101</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="47" t="s">
         <v>179</v>
@@ -11956,13 +12062,13 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="12.75" customHeight="1">
       <c r="A5" s="15">
         <v>43101</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" s="47" t="s">
         <v>179</v>
@@ -11991,13 +12097,13 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="12.75" customHeight="1">
       <c r="A6" s="15">
         <v>43101</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="47" t="s">
         <v>179</v>
@@ -12026,13 +12132,13 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="12.75" customHeight="1">
       <c r="A7" s="15">
         <v>43101</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" s="47" t="s">
         <v>179</v>
@@ -12061,13 +12167,13 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="12.75" customHeight="1">
       <c r="A8" s="15">
         <v>43101</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="47" t="s">
         <v>179</v>
@@ -12096,13 +12202,13 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" ht="12.75" customHeight="1">
       <c r="A9" s="15">
         <v>43101</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" s="47" t="s">
         <v>179</v>
@@ -12131,13 +12237,13 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="12.75" customHeight="1">
       <c r="A10" s="15">
         <v>43101</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="47" t="s">
         <v>179</v>
@@ -12166,13 +12272,13 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" ht="12.75" customHeight="1">
       <c r="A11" s="15">
         <v>43101</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>179</v>
@@ -12201,13 +12307,13 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" ht="12.75" customHeight="1">
       <c r="A12" s="15">
         <v>43101</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>179</v>
@@ -12236,13 +12342,13 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" ht="12.75" customHeight="1">
       <c r="A13" s="15">
         <v>43101</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="47" t="s">
         <v>179</v>
@@ -12271,13 +12377,13 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" ht="12.75" customHeight="1">
       <c r="A14" s="15">
         <v>43101</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="47" t="s">
         <v>179</v>
@@ -12306,13 +12412,13 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" ht="12.75" customHeight="1">
       <c r="A15" s="15">
         <v>43101</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D15" s="47" t="s">
         <v>179</v>
@@ -12341,13 +12447,13 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" ht="12.75" customHeight="1">
       <c r="A16" s="15">
         <v>43101</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D16" s="47" t="s">
         <v>179</v>
@@ -12376,13 +12482,13 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" ht="12.75" customHeight="1">
       <c r="A17" s="15">
         <v>43101</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" s="51" t="s">
         <v>182</v>
@@ -12411,13 +12517,13 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" ht="12.75" customHeight="1">
       <c r="A18" s="15">
         <v>43101</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="51" t="s">
         <v>182</v>
@@ -12446,13 +12552,13 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" ht="12.75" customHeight="1">
       <c r="A19" s="15">
         <v>43101</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D19" s="51" t="s">
         <v>182</v>
@@ -12481,13 +12587,13 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" ht="12.75" customHeight="1">
       <c r="A20" s="15">
         <v>43101</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>182</v>
@@ -12516,13 +12622,13 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" ht="12.75" customHeight="1">
       <c r="A21" s="15">
         <v>43101</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D21" s="51" t="s">
         <v>182</v>
@@ -12551,13 +12657,13 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" ht="12.75" customHeight="1">
       <c r="A22" s="15">
         <v>43101</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D22" s="53" t="s">
         <v>185</v>
@@ -12586,13 +12692,13 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" ht="12.75" customHeight="1">
       <c r="A23" s="15">
         <v>43101</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D23" s="53" t="s">
         <v>185</v>
@@ -12621,13 +12727,13 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" ht="12.75" customHeight="1">
       <c r="A24" s="15">
         <v>43101</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D24" s="53" t="s">
         <v>185</v>
@@ -12656,13 +12762,13 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15">
       <c r="A25" s="15">
         <v>43101</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D25" s="54" t="s">
         <v>187</v>
@@ -12690,13 +12796,13 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" ht="12.75" customHeight="1">
       <c r="A26" s="15">
         <v>43101</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D26" s="54" t="s">
         <v>187</v>
@@ -12725,13 +12831,13 @@
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
     </row>
-    <row r="27" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" ht="12.75" customHeight="1">
       <c r="A27" s="15">
         <v>43101</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D27" s="54" t="s">
         <v>187</v>
@@ -12760,13 +12866,13 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
     </row>
-    <row r="28" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" ht="12.75" customHeight="1">
       <c r="A28" s="15">
         <v>43101</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D28" s="54" t="s">
         <v>187</v>
@@ -12795,13 +12901,13 @@
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" ht="12.75" customHeight="1">
       <c r="A29" s="15">
         <v>43101</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D29" s="54" t="s">
         <v>187</v>
@@ -12830,13 +12936,13 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15">
       <c r="A30" s="15">
         <v>43466</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D30" s="55" t="s">
         <v>189</v>
@@ -12860,13 +12966,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15">
       <c r="A31" s="15">
         <v>43466</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D31" s="55" t="s">
         <v>189</v>
@@ -12890,13 +12996,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15">
       <c r="A32" s="15">
         <v>43466</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D32" s="55" t="s">
         <v>189</v>
@@ -12920,13 +13026,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11">
       <c r="A33" s="15">
         <v>43466</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D33" s="55" t="s">
         <v>189</v>
@@ -12950,13 +13056,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11">
       <c r="A34" s="15">
         <v>43466</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D34" s="55" t="s">
         <v>189</v>
@@ -12982,12 +13088,17 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A34" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A34">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove extra sscs roles
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="1340" windowWidth="26820" windowHeight="13040" tabRatio="500" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="260" yWindow="1340" windowWidth="26820" windowHeight="13040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="263">
   <si>
     <t>Change History</t>
   </si>
@@ -794,12 +794,6 @@
   </si>
   <si>
     <t>CRUD</t>
-  </si>
-  <si>
-    <t>caseworker-sscs-systemupdate</t>
-  </si>
-  <si>
-    <t>caseworker-sscs-callagent</t>
   </si>
   <si>
     <t>AuthorisationCaseField</t>
@@ -1376,7 +1370,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1531,13 +1525,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1561,10 +1553,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2020,7 +2008,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2069,7 +2057,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2081,7 +2069,7 @@
         <v>43383</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2236,7 +2224,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>223</v>
@@ -2263,7 +2251,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>223</v>
@@ -2290,7 +2278,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>223</v>
@@ -2317,7 +2305,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7" s="33" t="s">
         <v>223</v>
@@ -2344,7 +2332,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>223</v>
@@ -2371,7 +2359,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>223</v>
@@ -2398,7 +2386,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>223</v>
@@ -2425,7 +2413,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>223</v>
@@ -2452,7 +2440,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>223</v>
@@ -2479,7 +2467,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>223</v>
@@ -2506,7 +2494,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D14" s="33" t="s">
         <v>223</v>
@@ -2533,7 +2521,7 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>223</v>
@@ -2560,7 +2548,7 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D16" s="33" t="s">
         <v>223</v>
@@ -2587,7 +2575,7 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D17" s="33" t="s">
         <v>223</v>
@@ -2614,7 +2602,7 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D18" s="33" t="s">
         <v>223</v>
@@ -2641,7 +2629,7 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>223</v>
@@ -2810,7 +2798,7 @@
       </c>
       <c r="B4" s="33"/>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -2849,7 +2837,7 @@
       </c>
       <c r="B5" s="33"/>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
         <v>225</v>
@@ -2888,7 +2876,7 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>45</v>
@@ -3045,7 +3033,7 @@
       </c>
       <c r="B4" s="33"/>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -3084,7 +3072,7 @@
       </c>
       <c r="B5" s="33"/>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
         <v>225</v>
@@ -3123,7 +3111,7 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>45</v>
@@ -3162,7 +3150,7 @@
       </c>
       <c r="B7" s="33"/>
       <c r="C7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
@@ -6325,7 +6313,7 @@
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -6343,7 +6331,7 @@
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
         <v>225</v>
@@ -6361,7 +6349,7 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>45</v>
@@ -6496,7 +6484,7 @@
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -6535,7 +6523,7 @@
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
         <v>225</v>
@@ -6574,7 +6562,7 @@
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>45</v>
@@ -6613,7 +6601,7 @@
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
@@ -6716,13 +6704,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="89" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>156</v>
@@ -6923,10 +6911,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6991,52 +6979,21 @@
       <c r="A4" s="15">
         <v>43101</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>248</v>
+        <v>254</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>247</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="15">
-        <v>43102</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>247</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7053,10 +7010,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA51"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7072,7 +7029,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="17">
       <c r="A1" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>9</v>
@@ -7152,823 +7109,277 @@
       </c>
       <c r="B4" s="91"/>
       <c r="C4" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="94" t="s">
-        <v>248</v>
-      </c>
-      <c r="F4" s="95" t="s">
+      <c r="E4" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="94" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="96">
+      <c r="A5" s="95">
         <v>43101</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F5" s="97" t="s">
+      <c r="E5" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="96">
+      <c r="A6" s="95">
         <v>43101</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F6" s="97" t="s">
+      <c r="E6" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="96">
+      <c r="A7" s="95">
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F7" s="97" t="s">
+      <c r="E7" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F7" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="96">
+      <c r="A8" s="95">
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F8" s="97" t="s">
+      <c r="E8" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F8" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="96">
+      <c r="A9" s="95">
         <v>43101</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" s="97" t="s">
+      <c r="E9" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F9" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="96">
+      <c r="A10" s="95">
         <v>43101</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F10" s="97" t="s">
+      <c r="E10" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F10" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="96">
+      <c r="A11" s="95">
         <v>43101</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F11" s="97" t="s">
+      <c r="E11" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F11" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="96">
+      <c r="A12" s="95">
         <v>43101</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F12" s="97" t="s">
+      <c r="E12" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F12" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="96">
+      <c r="A13" s="95">
         <v>43101</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F13" s="97" t="s">
+      <c r="E13" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F13" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="96">
+      <c r="A14" s="95">
         <v>43101</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F14" s="97" t="s">
+      <c r="E14" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F14" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="96">
+      <c r="A15" s="95">
         <v>43101</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F15" s="97" t="s">
+      <c r="E15" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F15" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="96">
+      <c r="A16" s="95">
         <v>43101</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F16" s="97" t="s">
+      <c r="E16" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F16" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="96">
+      <c r="A17" s="95">
         <v>43101</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F17" s="97" t="s">
+      <c r="E17" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F17" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="96">
+      <c r="A18" s="95">
         <v>43101</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F18" s="97" t="s">
+      <c r="E18" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F18" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="96">
-        <v>43101</v>
-      </c>
+      <c r="A19" s="97">
+        <v>43101</v>
+      </c>
+      <c r="B19" s="98"/>
       <c r="C19" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D19" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="D19" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F19" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="90">
-        <v>43101</v>
-      </c>
-      <c r="B20" s="91"/>
-      <c r="C20" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D20" s="93" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="92" t="s">
-        <v>249</v>
-      </c>
-      <c r="F20" s="95" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F21" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F22" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F23" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F24" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F25" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F26" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F27" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F28" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F29" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F30" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F31" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F32" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F33" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F34" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F35" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="90">
-        <v>43101</v>
-      </c>
-      <c r="B36" s="91"/>
-      <c r="C36" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D36" s="93" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F36" s="95" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F37" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F38" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F39" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F40" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D41" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F41" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D42" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E42" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F42" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E43" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F43" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D44" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E44" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F44" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D45" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E45" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F45" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E46" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F46" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D47" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E47" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F47" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E48" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F48" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E49" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F49" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="96">
-        <v>43101</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E50" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F50" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="98">
-        <v>43101</v>
-      </c>
-      <c r="B51" s="99"/>
-      <c r="C51" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D51" s="101" t="s">
-        <v>78</v>
-      </c>
-      <c r="E51" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F51" s="102" t="s">
+      <c r="E19" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="F19" s="100" t="s">
         <v>247</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A51">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7985,10 +7396,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E4:E8"/>
+      <selection activeCell="A9" sqref="A9:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -8002,17 +7413,17 @@
     <col min="7" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="107" customFormat="1" ht="34">
-      <c r="A1" s="103" t="s">
-        <v>251</v>
-      </c>
-      <c r="B1" s="104" t="s">
+    <row r="1" spans="1:27" s="105" customFormat="1" ht="34">
+      <c r="A1" s="101" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="105" t="s">
+      <c r="C1" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="104" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="19"/>
@@ -8032,7 +7443,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>245</v>
@@ -8085,201 +7496,93 @@
       </c>
       <c r="B4" s="91"/>
       <c r="C4" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" s="108" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="106" t="s">
         <v>179</v>
       </c>
       <c r="E4" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F4" s="95" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="94" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="96">
-        <v>43101</v>
-      </c>
-      <c r="B5" s="109"/>
+      <c r="A5" s="95">
+        <v>43101</v>
+      </c>
+      <c r="B5" s="107"/>
       <c r="C5" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" s="51" t="s">
         <v>182</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F5" s="97" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="96">
+      <c r="A6" s="95">
         <v>43101</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>185</v>
       </c>
       <c r="E6" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F6" s="111" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="109" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="96">
-        <v>43101</v>
-      </c>
-      <c r="B7" s="110"/>
+      <c r="A7" s="95">
+        <v>43101</v>
+      </c>
+      <c r="B7" s="108"/>
       <c r="C7" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7" s="54" t="s">
         <v>187</v>
       </c>
       <c r="E7" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F7" s="97" t="s">
+        <v>262</v>
+      </c>
+      <c r="F7" s="96" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="98">
-        <v>43101</v>
-      </c>
-      <c r="B8" s="112"/>
+      <c r="A8" s="97">
+        <v>43101</v>
+      </c>
+      <c r="B8" s="110"/>
       <c r="C8" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D8" s="113" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="111" t="s">
         <v>189</v>
       </c>
       <c r="E8" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F8" s="102" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27">
-      <c r="A9" s="90">
-        <v>43101</v>
-      </c>
-      <c r="B9" s="92"/>
-      <c r="C9" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D9" s="114" t="s">
-        <v>182</v>
-      </c>
-      <c r="E9" s="94" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" s="115" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27">
-      <c r="A10" s="96">
-        <v>43101</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F10" s="97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27">
-      <c r="A11" s="98">
-        <v>43101</v>
-      </c>
-      <c r="B11" s="112"/>
-      <c r="C11" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D11" s="116" t="s">
-        <v>187</v>
-      </c>
-      <c r="E11" s="112" t="s">
-        <v>248</v>
-      </c>
-      <c r="F11" s="117" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27">
-      <c r="A12" s="90">
-        <v>43101</v>
-      </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D12" s="114" t="s">
-        <v>182</v>
-      </c>
-      <c r="E12" s="92" t="s">
-        <v>249</v>
-      </c>
-      <c r="F12" s="95" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27">
-      <c r="A13" s="96">
-        <v>43101</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D13" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F13" s="111" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27">
-      <c r="A14" s="98">
-        <v>43101</v>
-      </c>
-      <c r="B14" s="112"/>
-      <c r="C14" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D14" s="116" t="s">
-        <v>187</v>
-      </c>
-      <c r="E14" s="100" t="s">
-        <v>249</v>
-      </c>
-      <c r="F14" s="117" t="s">
+        <v>262</v>
+      </c>
+      <c r="F8" s="100" t="s">
         <v>247</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8296,822 +7599,822 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK12"/>
+  <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="118" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="118" customWidth="1"/>
-    <col min="3" max="3" width="23.5" style="118" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" style="118" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" style="118" customWidth="1"/>
-    <col min="6" max="6" width="36" style="119" customWidth="1"/>
-    <col min="7" max="255" width="12.5" style="118" customWidth="1"/>
-    <col min="256" max="1025" width="7.1640625" style="118" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" style="112" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="112" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="112" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" style="112" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" style="112" customWidth="1"/>
+    <col min="6" max="6" width="36" style="113" customWidth="1"/>
+    <col min="7" max="255" width="12.5" style="112" customWidth="1"/>
+    <col min="256" max="1025" width="7.1640625" style="112" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="129" customFormat="1" ht="34">
-      <c r="A1" s="120" t="s">
-        <v>253</v>
-      </c>
-      <c r="B1" s="121" t="s">
+    <row r="1" spans="1:255" s="123" customFormat="1" ht="34">
+      <c r="A1" s="114" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="124"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-      <c r="O1" s="127"/>
-      <c r="P1" s="127"/>
-      <c r="Q1" s="127"/>
-      <c r="R1" s="127"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="127"/>
-      <c r="V1" s="127"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="127"/>
-      <c r="Z1" s="127"/>
-      <c r="AA1" s="127"/>
-      <c r="AB1" s="127"/>
-      <c r="AC1" s="127"/>
-      <c r="AD1" s="127"/>
-      <c r="AE1" s="127"/>
-      <c r="AF1" s="127"/>
-      <c r="AG1" s="127"/>
-      <c r="AH1" s="127"/>
-      <c r="AI1" s="127"/>
-      <c r="AJ1" s="127"/>
-      <c r="AK1" s="127"/>
-      <c r="AL1" s="127"/>
-      <c r="AM1" s="127"/>
-      <c r="AN1" s="127"/>
-      <c r="AO1" s="127"/>
-      <c r="AP1" s="127"/>
-      <c r="AQ1" s="127"/>
-      <c r="AR1" s="127"/>
-      <c r="AS1" s="127"/>
-      <c r="AT1" s="127"/>
-      <c r="AU1" s="127"/>
-      <c r="AV1" s="127"/>
-      <c r="AW1" s="127"/>
-      <c r="AX1" s="127"/>
-      <c r="AY1" s="127"/>
-      <c r="AZ1" s="127"/>
-      <c r="BA1" s="127"/>
-      <c r="BB1" s="127"/>
-      <c r="BC1" s="127"/>
-      <c r="BD1" s="127"/>
-      <c r="BE1" s="127"/>
-      <c r="BF1" s="127"/>
-      <c r="BG1" s="127"/>
-      <c r="BH1" s="127"/>
-      <c r="BI1" s="127"/>
-      <c r="BJ1" s="127"/>
-      <c r="BK1" s="127"/>
-      <c r="BL1" s="127"/>
-      <c r="BM1" s="127"/>
-      <c r="BN1" s="127"/>
-      <c r="BO1" s="127"/>
-      <c r="BP1" s="127"/>
-      <c r="BQ1" s="127"/>
-      <c r="BR1" s="127"/>
-      <c r="BS1" s="127"/>
-      <c r="BT1" s="127"/>
-      <c r="BU1" s="127"/>
-      <c r="BV1" s="127"/>
-      <c r="BW1" s="127"/>
-      <c r="BX1" s="127"/>
-      <c r="BY1" s="127"/>
-      <c r="BZ1" s="127"/>
-      <c r="CA1" s="127"/>
-      <c r="CB1" s="127"/>
-      <c r="CC1" s="127"/>
-      <c r="CD1" s="127"/>
-      <c r="CE1" s="127"/>
-      <c r="CF1" s="127"/>
-      <c r="CG1" s="127"/>
-      <c r="CH1" s="127"/>
-      <c r="CI1" s="127"/>
-      <c r="CJ1" s="127"/>
-      <c r="CK1" s="127"/>
-      <c r="CL1" s="127"/>
-      <c r="CM1" s="127"/>
-      <c r="CN1" s="127"/>
-      <c r="CO1" s="127"/>
-      <c r="CP1" s="127"/>
-      <c r="CQ1" s="127"/>
-      <c r="CR1" s="127"/>
-      <c r="CS1" s="127"/>
-      <c r="CT1" s="127"/>
-      <c r="CU1" s="127"/>
-      <c r="CV1" s="127"/>
-      <c r="CW1" s="127"/>
-      <c r="CX1" s="127"/>
-      <c r="CY1" s="127"/>
-      <c r="CZ1" s="127"/>
-      <c r="DA1" s="127"/>
-      <c r="DB1" s="127"/>
-      <c r="DC1" s="127"/>
-      <c r="DD1" s="127"/>
-      <c r="DE1" s="127"/>
-      <c r="DF1" s="127"/>
-      <c r="DG1" s="127"/>
-      <c r="DH1" s="127"/>
-      <c r="DI1" s="127"/>
-      <c r="DJ1" s="127"/>
-      <c r="DK1" s="127"/>
-      <c r="DL1" s="127"/>
-      <c r="DM1" s="127"/>
-      <c r="DN1" s="127"/>
-      <c r="DO1" s="127"/>
-      <c r="DP1" s="127"/>
-      <c r="DQ1" s="127"/>
-      <c r="DR1" s="127"/>
-      <c r="DS1" s="127"/>
-      <c r="DT1" s="127"/>
-      <c r="DU1" s="127"/>
-      <c r="DV1" s="127"/>
-      <c r="DW1" s="127"/>
-      <c r="DX1" s="127"/>
-      <c r="DY1" s="127"/>
-      <c r="DZ1" s="127"/>
-      <c r="EA1" s="127"/>
-      <c r="EB1" s="127"/>
-      <c r="EC1" s="127"/>
-      <c r="ED1" s="127"/>
-      <c r="EE1" s="127"/>
-      <c r="EF1" s="127"/>
-      <c r="EG1" s="127"/>
-      <c r="EH1" s="127"/>
-      <c r="EI1" s="127"/>
-      <c r="EJ1" s="127"/>
-      <c r="EK1" s="127"/>
-      <c r="EL1" s="127"/>
-      <c r="EM1" s="127"/>
-      <c r="EN1" s="127"/>
-      <c r="EO1" s="127"/>
-      <c r="EP1" s="127"/>
-      <c r="EQ1" s="127"/>
-      <c r="ER1" s="127"/>
-      <c r="ES1" s="127"/>
-      <c r="ET1" s="127"/>
-      <c r="EU1" s="127"/>
-      <c r="EV1" s="127"/>
-      <c r="EW1" s="127"/>
-      <c r="EX1" s="127"/>
-      <c r="EY1" s="127"/>
-      <c r="EZ1" s="127"/>
-      <c r="FA1" s="127"/>
-      <c r="FB1" s="127"/>
-      <c r="FC1" s="127"/>
-      <c r="FD1" s="127"/>
-      <c r="FE1" s="127"/>
-      <c r="FF1" s="127"/>
-      <c r="FG1" s="127"/>
-      <c r="FH1" s="127"/>
-      <c r="FI1" s="127"/>
-      <c r="FJ1" s="127"/>
-      <c r="FK1" s="127"/>
-      <c r="FL1" s="127"/>
-      <c r="FM1" s="127"/>
-      <c r="FN1" s="127"/>
-      <c r="FO1" s="127"/>
-      <c r="FP1" s="127"/>
-      <c r="FQ1" s="127"/>
-      <c r="FR1" s="127"/>
-      <c r="FS1" s="127"/>
-      <c r="FT1" s="127"/>
-      <c r="FU1" s="127"/>
-      <c r="FV1" s="127"/>
-      <c r="FW1" s="127"/>
-      <c r="FX1" s="127"/>
-      <c r="FY1" s="127"/>
-      <c r="FZ1" s="127"/>
-      <c r="GA1" s="127"/>
-      <c r="GB1" s="127"/>
-      <c r="GC1" s="127"/>
-      <c r="GD1" s="127"/>
-      <c r="GE1" s="127"/>
-      <c r="GF1" s="127"/>
-      <c r="GG1" s="127"/>
-      <c r="GH1" s="127"/>
-      <c r="GI1" s="127"/>
-      <c r="GJ1" s="127"/>
-      <c r="GK1" s="127"/>
-      <c r="GL1" s="127"/>
-      <c r="GM1" s="127"/>
-      <c r="GN1" s="127"/>
-      <c r="GO1" s="127"/>
-      <c r="GP1" s="127"/>
-      <c r="GQ1" s="127"/>
-      <c r="GR1" s="127"/>
-      <c r="GS1" s="127"/>
-      <c r="GT1" s="127"/>
-      <c r="GU1" s="127"/>
-      <c r="GV1" s="127"/>
-      <c r="GW1" s="127"/>
-      <c r="GX1" s="127"/>
-      <c r="GY1" s="127"/>
-      <c r="GZ1" s="127"/>
-      <c r="HA1" s="127"/>
-      <c r="HB1" s="127"/>
-      <c r="HC1" s="127"/>
-      <c r="HD1" s="127"/>
-      <c r="HE1" s="127"/>
-      <c r="HF1" s="127"/>
-      <c r="HG1" s="127"/>
-      <c r="HH1" s="127"/>
-      <c r="HI1" s="127"/>
-      <c r="HJ1" s="127"/>
-      <c r="HK1" s="127"/>
-      <c r="HL1" s="127"/>
-      <c r="HM1" s="127"/>
-      <c r="HN1" s="127"/>
-      <c r="HO1" s="127"/>
-      <c r="HP1" s="127"/>
-      <c r="HQ1" s="127"/>
-      <c r="HR1" s="127"/>
-      <c r="HS1" s="127"/>
-      <c r="HT1" s="127"/>
-      <c r="HU1" s="127"/>
-      <c r="HV1" s="127"/>
-      <c r="HW1" s="127"/>
-      <c r="HX1" s="127"/>
-      <c r="HY1" s="127"/>
-      <c r="HZ1" s="127"/>
-      <c r="IA1" s="127"/>
-      <c r="IB1" s="127"/>
-      <c r="IC1" s="127"/>
-      <c r="ID1" s="127"/>
-      <c r="IE1" s="127"/>
-      <c r="IF1" s="127"/>
-      <c r="IG1" s="127"/>
-      <c r="IH1" s="127"/>
-      <c r="II1" s="127"/>
-      <c r="IJ1" s="127"/>
-      <c r="IK1" s="127"/>
-      <c r="IL1" s="127"/>
-      <c r="IM1" s="127"/>
-      <c r="IN1" s="127"/>
-      <c r="IO1" s="127"/>
-      <c r="IP1" s="127"/>
-      <c r="IQ1" s="127"/>
-      <c r="IR1" s="127"/>
-      <c r="IS1" s="127"/>
-      <c r="IT1" s="127"/>
-      <c r="IU1" s="128"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="121"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
+      <c r="T1" s="121"/>
+      <c r="U1" s="121"/>
+      <c r="V1" s="121"/>
+      <c r="W1" s="121"/>
+      <c r="X1" s="121"/>
+      <c r="Y1" s="121"/>
+      <c r="Z1" s="121"/>
+      <c r="AA1" s="121"/>
+      <c r="AB1" s="121"/>
+      <c r="AC1" s="121"/>
+      <c r="AD1" s="121"/>
+      <c r="AE1" s="121"/>
+      <c r="AF1" s="121"/>
+      <c r="AG1" s="121"/>
+      <c r="AH1" s="121"/>
+      <c r="AI1" s="121"/>
+      <c r="AJ1" s="121"/>
+      <c r="AK1" s="121"/>
+      <c r="AL1" s="121"/>
+      <c r="AM1" s="121"/>
+      <c r="AN1" s="121"/>
+      <c r="AO1" s="121"/>
+      <c r="AP1" s="121"/>
+      <c r="AQ1" s="121"/>
+      <c r="AR1" s="121"/>
+      <c r="AS1" s="121"/>
+      <c r="AT1" s="121"/>
+      <c r="AU1" s="121"/>
+      <c r="AV1" s="121"/>
+      <c r="AW1" s="121"/>
+      <c r="AX1" s="121"/>
+      <c r="AY1" s="121"/>
+      <c r="AZ1" s="121"/>
+      <c r="BA1" s="121"/>
+      <c r="BB1" s="121"/>
+      <c r="BC1" s="121"/>
+      <c r="BD1" s="121"/>
+      <c r="BE1" s="121"/>
+      <c r="BF1" s="121"/>
+      <c r="BG1" s="121"/>
+      <c r="BH1" s="121"/>
+      <c r="BI1" s="121"/>
+      <c r="BJ1" s="121"/>
+      <c r="BK1" s="121"/>
+      <c r="BL1" s="121"/>
+      <c r="BM1" s="121"/>
+      <c r="BN1" s="121"/>
+      <c r="BO1" s="121"/>
+      <c r="BP1" s="121"/>
+      <c r="BQ1" s="121"/>
+      <c r="BR1" s="121"/>
+      <c r="BS1" s="121"/>
+      <c r="BT1" s="121"/>
+      <c r="BU1" s="121"/>
+      <c r="BV1" s="121"/>
+      <c r="BW1" s="121"/>
+      <c r="BX1" s="121"/>
+      <c r="BY1" s="121"/>
+      <c r="BZ1" s="121"/>
+      <c r="CA1" s="121"/>
+      <c r="CB1" s="121"/>
+      <c r="CC1" s="121"/>
+      <c r="CD1" s="121"/>
+      <c r="CE1" s="121"/>
+      <c r="CF1" s="121"/>
+      <c r="CG1" s="121"/>
+      <c r="CH1" s="121"/>
+      <c r="CI1" s="121"/>
+      <c r="CJ1" s="121"/>
+      <c r="CK1" s="121"/>
+      <c r="CL1" s="121"/>
+      <c r="CM1" s="121"/>
+      <c r="CN1" s="121"/>
+      <c r="CO1" s="121"/>
+      <c r="CP1" s="121"/>
+      <c r="CQ1" s="121"/>
+      <c r="CR1" s="121"/>
+      <c r="CS1" s="121"/>
+      <c r="CT1" s="121"/>
+      <c r="CU1" s="121"/>
+      <c r="CV1" s="121"/>
+      <c r="CW1" s="121"/>
+      <c r="CX1" s="121"/>
+      <c r="CY1" s="121"/>
+      <c r="CZ1" s="121"/>
+      <c r="DA1" s="121"/>
+      <c r="DB1" s="121"/>
+      <c r="DC1" s="121"/>
+      <c r="DD1" s="121"/>
+      <c r="DE1" s="121"/>
+      <c r="DF1" s="121"/>
+      <c r="DG1" s="121"/>
+      <c r="DH1" s="121"/>
+      <c r="DI1" s="121"/>
+      <c r="DJ1" s="121"/>
+      <c r="DK1" s="121"/>
+      <c r="DL1" s="121"/>
+      <c r="DM1" s="121"/>
+      <c r="DN1" s="121"/>
+      <c r="DO1" s="121"/>
+      <c r="DP1" s="121"/>
+      <c r="DQ1" s="121"/>
+      <c r="DR1" s="121"/>
+      <c r="DS1" s="121"/>
+      <c r="DT1" s="121"/>
+      <c r="DU1" s="121"/>
+      <c r="DV1" s="121"/>
+      <c r="DW1" s="121"/>
+      <c r="DX1" s="121"/>
+      <c r="DY1" s="121"/>
+      <c r="DZ1" s="121"/>
+      <c r="EA1" s="121"/>
+      <c r="EB1" s="121"/>
+      <c r="EC1" s="121"/>
+      <c r="ED1" s="121"/>
+      <c r="EE1" s="121"/>
+      <c r="EF1" s="121"/>
+      <c r="EG1" s="121"/>
+      <c r="EH1" s="121"/>
+      <c r="EI1" s="121"/>
+      <c r="EJ1" s="121"/>
+      <c r="EK1" s="121"/>
+      <c r="EL1" s="121"/>
+      <c r="EM1" s="121"/>
+      <c r="EN1" s="121"/>
+      <c r="EO1" s="121"/>
+      <c r="EP1" s="121"/>
+      <c r="EQ1" s="121"/>
+      <c r="ER1" s="121"/>
+      <c r="ES1" s="121"/>
+      <c r="ET1" s="121"/>
+      <c r="EU1" s="121"/>
+      <c r="EV1" s="121"/>
+      <c r="EW1" s="121"/>
+      <c r="EX1" s="121"/>
+      <c r="EY1" s="121"/>
+      <c r="EZ1" s="121"/>
+      <c r="FA1" s="121"/>
+      <c r="FB1" s="121"/>
+      <c r="FC1" s="121"/>
+      <c r="FD1" s="121"/>
+      <c r="FE1" s="121"/>
+      <c r="FF1" s="121"/>
+      <c r="FG1" s="121"/>
+      <c r="FH1" s="121"/>
+      <c r="FI1" s="121"/>
+      <c r="FJ1" s="121"/>
+      <c r="FK1" s="121"/>
+      <c r="FL1" s="121"/>
+      <c r="FM1" s="121"/>
+      <c r="FN1" s="121"/>
+      <c r="FO1" s="121"/>
+      <c r="FP1" s="121"/>
+      <c r="FQ1" s="121"/>
+      <c r="FR1" s="121"/>
+      <c r="FS1" s="121"/>
+      <c r="FT1" s="121"/>
+      <c r="FU1" s="121"/>
+      <c r="FV1" s="121"/>
+      <c r="FW1" s="121"/>
+      <c r="FX1" s="121"/>
+      <c r="FY1" s="121"/>
+      <c r="FZ1" s="121"/>
+      <c r="GA1" s="121"/>
+      <c r="GB1" s="121"/>
+      <c r="GC1" s="121"/>
+      <c r="GD1" s="121"/>
+      <c r="GE1" s="121"/>
+      <c r="GF1" s="121"/>
+      <c r="GG1" s="121"/>
+      <c r="GH1" s="121"/>
+      <c r="GI1" s="121"/>
+      <c r="GJ1" s="121"/>
+      <c r="GK1" s="121"/>
+      <c r="GL1" s="121"/>
+      <c r="GM1" s="121"/>
+      <c r="GN1" s="121"/>
+      <c r="GO1" s="121"/>
+      <c r="GP1" s="121"/>
+      <c r="GQ1" s="121"/>
+      <c r="GR1" s="121"/>
+      <c r="GS1" s="121"/>
+      <c r="GT1" s="121"/>
+      <c r="GU1" s="121"/>
+      <c r="GV1" s="121"/>
+      <c r="GW1" s="121"/>
+      <c r="GX1" s="121"/>
+      <c r="GY1" s="121"/>
+      <c r="GZ1" s="121"/>
+      <c r="HA1" s="121"/>
+      <c r="HB1" s="121"/>
+      <c r="HC1" s="121"/>
+      <c r="HD1" s="121"/>
+      <c r="HE1" s="121"/>
+      <c r="HF1" s="121"/>
+      <c r="HG1" s="121"/>
+      <c r="HH1" s="121"/>
+      <c r="HI1" s="121"/>
+      <c r="HJ1" s="121"/>
+      <c r="HK1" s="121"/>
+      <c r="HL1" s="121"/>
+      <c r="HM1" s="121"/>
+      <c r="HN1" s="121"/>
+      <c r="HO1" s="121"/>
+      <c r="HP1" s="121"/>
+      <c r="HQ1" s="121"/>
+      <c r="HR1" s="121"/>
+      <c r="HS1" s="121"/>
+      <c r="HT1" s="121"/>
+      <c r="HU1" s="121"/>
+      <c r="HV1" s="121"/>
+      <c r="HW1" s="121"/>
+      <c r="HX1" s="121"/>
+      <c r="HY1" s="121"/>
+      <c r="HZ1" s="121"/>
+      <c r="IA1" s="121"/>
+      <c r="IB1" s="121"/>
+      <c r="IC1" s="121"/>
+      <c r="ID1" s="121"/>
+      <c r="IE1" s="121"/>
+      <c r="IF1" s="121"/>
+      <c r="IG1" s="121"/>
+      <c r="IH1" s="121"/>
+      <c r="II1" s="121"/>
+      <c r="IJ1" s="121"/>
+      <c r="IK1" s="121"/>
+      <c r="IL1" s="121"/>
+      <c r="IM1" s="121"/>
+      <c r="IN1" s="121"/>
+      <c r="IO1" s="121"/>
+      <c r="IP1" s="121"/>
+      <c r="IQ1" s="121"/>
+      <c r="IR1" s="121"/>
+      <c r="IS1" s="121"/>
+      <c r="IT1" s="121"/>
+      <c r="IU1" s="122"/>
     </row>
     <row r="2" spans="1:255" ht="24">
-      <c r="A2" s="130"/>
-      <c r="B2" s="130"/>
-      <c r="C2" s="131" t="s">
+      <c r="A2" s="124"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="131" t="s">
+      <c r="D2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="131" t="s">
+      <c r="E2" s="125" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="126" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
+      <c r="P2" s="128"/>
+      <c r="Q2" s="128"/>
+      <c r="R2" s="128"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="128"/>
+      <c r="V2" s="128"/>
+      <c r="W2" s="128"/>
+      <c r="X2" s="128"/>
+      <c r="Y2" s="128"/>
+      <c r="Z2" s="128"/>
+      <c r="AA2" s="128"/>
+      <c r="AB2" s="128"/>
+      <c r="AC2" s="128"/>
+      <c r="AD2" s="128"/>
+      <c r="AE2" s="128"/>
+      <c r="AF2" s="128"/>
+      <c r="AG2" s="128"/>
+      <c r="AH2" s="128"/>
+      <c r="AI2" s="128"/>
+      <c r="AJ2" s="128"/>
+      <c r="AK2" s="128"/>
+      <c r="AL2" s="128"/>
+      <c r="AM2" s="128"/>
+      <c r="AN2" s="128"/>
+      <c r="AO2" s="128"/>
+      <c r="AP2" s="128"/>
+      <c r="AQ2" s="128"/>
+      <c r="AR2" s="128"/>
+      <c r="AS2" s="128"/>
+      <c r="AT2" s="128"/>
+      <c r="AU2" s="128"/>
+      <c r="AV2" s="128"/>
+      <c r="AW2" s="128"/>
+      <c r="AX2" s="128"/>
+      <c r="AY2" s="128"/>
+      <c r="AZ2" s="128"/>
+      <c r="BA2" s="128"/>
+      <c r="BB2" s="128"/>
+      <c r="BC2" s="128"/>
+      <c r="BD2" s="128"/>
+      <c r="BE2" s="128"/>
+      <c r="BF2" s="128"/>
+      <c r="BG2" s="128"/>
+      <c r="BH2" s="128"/>
+      <c r="BI2" s="128"/>
+      <c r="BJ2" s="128"/>
+      <c r="BK2" s="128"/>
+      <c r="BL2" s="128"/>
+      <c r="BM2" s="128"/>
+      <c r="BN2" s="128"/>
+      <c r="BO2" s="128"/>
+      <c r="BP2" s="128"/>
+      <c r="BQ2" s="128"/>
+      <c r="BR2" s="128"/>
+      <c r="BS2" s="128"/>
+      <c r="BT2" s="128"/>
+      <c r="BU2" s="128"/>
+      <c r="BV2" s="128"/>
+      <c r="BW2" s="128"/>
+      <c r="BX2" s="128"/>
+      <c r="BY2" s="128"/>
+      <c r="BZ2" s="128"/>
+      <c r="CA2" s="128"/>
+      <c r="CB2" s="128"/>
+      <c r="CC2" s="128"/>
+      <c r="CD2" s="128"/>
+      <c r="CE2" s="128"/>
+      <c r="CF2" s="128"/>
+      <c r="CG2" s="128"/>
+      <c r="CH2" s="128"/>
+      <c r="CI2" s="128"/>
+      <c r="CJ2" s="128"/>
+      <c r="CK2" s="128"/>
+      <c r="CL2" s="128"/>
+      <c r="CM2" s="128"/>
+      <c r="CN2" s="128"/>
+      <c r="CO2" s="128"/>
+      <c r="CP2" s="128"/>
+      <c r="CQ2" s="128"/>
+      <c r="CR2" s="128"/>
+      <c r="CS2" s="128"/>
+      <c r="CT2" s="128"/>
+      <c r="CU2" s="128"/>
+      <c r="CV2" s="128"/>
+      <c r="CW2" s="128"/>
+      <c r="CX2" s="128"/>
+      <c r="CY2" s="128"/>
+      <c r="CZ2" s="128"/>
+      <c r="DA2" s="128"/>
+      <c r="DB2" s="128"/>
+      <c r="DC2" s="128"/>
+      <c r="DD2" s="128"/>
+      <c r="DE2" s="128"/>
+      <c r="DF2" s="128"/>
+      <c r="DG2" s="128"/>
+      <c r="DH2" s="128"/>
+      <c r="DI2" s="128"/>
+      <c r="DJ2" s="128"/>
+      <c r="DK2" s="128"/>
+      <c r="DL2" s="128"/>
+      <c r="DM2" s="128"/>
+      <c r="DN2" s="128"/>
+      <c r="DO2" s="128"/>
+      <c r="DP2" s="128"/>
+      <c r="DQ2" s="128"/>
+      <c r="DR2" s="128"/>
+      <c r="DS2" s="128"/>
+      <c r="DT2" s="128"/>
+      <c r="DU2" s="128"/>
+      <c r="DV2" s="128"/>
+      <c r="DW2" s="128"/>
+      <c r="DX2" s="128"/>
+      <c r="DY2" s="128"/>
+      <c r="DZ2" s="128"/>
+      <c r="EA2" s="128"/>
+      <c r="EB2" s="128"/>
+      <c r="EC2" s="128"/>
+      <c r="ED2" s="128"/>
+      <c r="EE2" s="128"/>
+      <c r="EF2" s="128"/>
+      <c r="EG2" s="128"/>
+      <c r="EH2" s="128"/>
+      <c r="EI2" s="128"/>
+      <c r="EJ2" s="128"/>
+      <c r="EK2" s="128"/>
+      <c r="EL2" s="128"/>
+      <c r="EM2" s="128"/>
+      <c r="EN2" s="128"/>
+      <c r="EO2" s="128"/>
+      <c r="EP2" s="128"/>
+      <c r="EQ2" s="128"/>
+      <c r="ER2" s="128"/>
+      <c r="ES2" s="128"/>
+      <c r="ET2" s="128"/>
+      <c r="EU2" s="128"/>
+      <c r="EV2" s="128"/>
+      <c r="EW2" s="128"/>
+      <c r="EX2" s="128"/>
+      <c r="EY2" s="128"/>
+      <c r="EZ2" s="128"/>
+      <c r="FA2" s="128"/>
+      <c r="FB2" s="128"/>
+      <c r="FC2" s="128"/>
+      <c r="FD2" s="128"/>
+      <c r="FE2" s="128"/>
+      <c r="FF2" s="128"/>
+      <c r="FG2" s="128"/>
+      <c r="FH2" s="128"/>
+      <c r="FI2" s="128"/>
+      <c r="FJ2" s="128"/>
+      <c r="FK2" s="128"/>
+      <c r="FL2" s="128"/>
+      <c r="FM2" s="128"/>
+      <c r="FN2" s="128"/>
+      <c r="FO2" s="128"/>
+      <c r="FP2" s="128"/>
+      <c r="FQ2" s="128"/>
+      <c r="FR2" s="128"/>
+      <c r="FS2" s="128"/>
+      <c r="FT2" s="128"/>
+      <c r="FU2" s="128"/>
+      <c r="FV2" s="128"/>
+      <c r="FW2" s="128"/>
+      <c r="FX2" s="128"/>
+      <c r="FY2" s="128"/>
+      <c r="FZ2" s="128"/>
+      <c r="GA2" s="128"/>
+      <c r="GB2" s="128"/>
+      <c r="GC2" s="128"/>
+      <c r="GD2" s="128"/>
+      <c r="GE2" s="128"/>
+      <c r="GF2" s="128"/>
+      <c r="GG2" s="128"/>
+      <c r="GH2" s="128"/>
+      <c r="GI2" s="128"/>
+      <c r="GJ2" s="128"/>
+      <c r="GK2" s="128"/>
+      <c r="GL2" s="128"/>
+      <c r="GM2" s="128"/>
+      <c r="GN2" s="128"/>
+      <c r="GO2" s="128"/>
+      <c r="GP2" s="128"/>
+      <c r="GQ2" s="128"/>
+      <c r="GR2" s="128"/>
+      <c r="GS2" s="128"/>
+      <c r="GT2" s="128"/>
+      <c r="GU2" s="128"/>
+      <c r="GV2" s="128"/>
+      <c r="GW2" s="128"/>
+      <c r="GX2" s="128"/>
+      <c r="GY2" s="128"/>
+      <c r="GZ2" s="128"/>
+      <c r="HA2" s="128"/>
+      <c r="HB2" s="128"/>
+      <c r="HC2" s="128"/>
+      <c r="HD2" s="128"/>
+      <c r="HE2" s="128"/>
+      <c r="HF2" s="128"/>
+      <c r="HG2" s="128"/>
+      <c r="HH2" s="128"/>
+      <c r="HI2" s="128"/>
+      <c r="HJ2" s="128"/>
+      <c r="HK2" s="128"/>
+      <c r="HL2" s="128"/>
+      <c r="HM2" s="128"/>
+      <c r="HN2" s="128"/>
+      <c r="HO2" s="128"/>
+      <c r="HP2" s="128"/>
+      <c r="HQ2" s="128"/>
+      <c r="HR2" s="128"/>
+      <c r="HS2" s="128"/>
+      <c r="HT2" s="128"/>
+      <c r="HU2" s="128"/>
+      <c r="HV2" s="128"/>
+      <c r="HW2" s="128"/>
+      <c r="HX2" s="128"/>
+      <c r="HY2" s="128"/>
+      <c r="HZ2" s="128"/>
+      <c r="IA2" s="128"/>
+      <c r="IB2" s="128"/>
+      <c r="IC2" s="128"/>
+      <c r="ID2" s="128"/>
+      <c r="IE2" s="128"/>
+      <c r="IF2" s="128"/>
+      <c r="IG2" s="128"/>
+      <c r="IH2" s="128"/>
+      <c r="II2" s="128"/>
+      <c r="IJ2" s="128"/>
+      <c r="IK2" s="128"/>
+      <c r="IL2" s="128"/>
+      <c r="IM2" s="128"/>
+      <c r="IN2" s="128"/>
+      <c r="IO2" s="128"/>
+      <c r="IP2" s="128"/>
+      <c r="IQ2" s="128"/>
+      <c r="IR2" s="128"/>
+      <c r="IS2" s="128"/>
+      <c r="IT2" s="128"/>
+      <c r="IU2" s="129"/>
+    </row>
+    <row r="3" spans="1:255">
+      <c r="A3" s="130" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="130" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="131" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="131" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="132" t="s">
-        <v>245</v>
-      </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="130"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="134"/>
-      <c r="S2" s="134"/>
-      <c r="T2" s="134"/>
-      <c r="U2" s="134"/>
-      <c r="V2" s="134"/>
-      <c r="W2" s="134"/>
-      <c r="X2" s="134"/>
-      <c r="Y2" s="134"/>
-      <c r="Z2" s="134"/>
-      <c r="AA2" s="134"/>
-      <c r="AB2" s="134"/>
-      <c r="AC2" s="134"/>
-      <c r="AD2" s="134"/>
-      <c r="AE2" s="134"/>
-      <c r="AF2" s="134"/>
-      <c r="AG2" s="134"/>
-      <c r="AH2" s="134"/>
-      <c r="AI2" s="134"/>
-      <c r="AJ2" s="134"/>
-      <c r="AK2" s="134"/>
-      <c r="AL2" s="134"/>
-      <c r="AM2" s="134"/>
-      <c r="AN2" s="134"/>
-      <c r="AO2" s="134"/>
-      <c r="AP2" s="134"/>
-      <c r="AQ2" s="134"/>
-      <c r="AR2" s="134"/>
-      <c r="AS2" s="134"/>
-      <c r="AT2" s="134"/>
-      <c r="AU2" s="134"/>
-      <c r="AV2" s="134"/>
-      <c r="AW2" s="134"/>
-      <c r="AX2" s="134"/>
-      <c r="AY2" s="134"/>
-      <c r="AZ2" s="134"/>
-      <c r="BA2" s="134"/>
-      <c r="BB2" s="134"/>
-      <c r="BC2" s="134"/>
-      <c r="BD2" s="134"/>
-      <c r="BE2" s="134"/>
-      <c r="BF2" s="134"/>
-      <c r="BG2" s="134"/>
-      <c r="BH2" s="134"/>
-      <c r="BI2" s="134"/>
-      <c r="BJ2" s="134"/>
-      <c r="BK2" s="134"/>
-      <c r="BL2" s="134"/>
-      <c r="BM2" s="134"/>
-      <c r="BN2" s="134"/>
-      <c r="BO2" s="134"/>
-      <c r="BP2" s="134"/>
-      <c r="BQ2" s="134"/>
-      <c r="BR2" s="134"/>
-      <c r="BS2" s="134"/>
-      <c r="BT2" s="134"/>
-      <c r="BU2" s="134"/>
-      <c r="BV2" s="134"/>
-      <c r="BW2" s="134"/>
-      <c r="BX2" s="134"/>
-      <c r="BY2" s="134"/>
-      <c r="BZ2" s="134"/>
-      <c r="CA2" s="134"/>
-      <c r="CB2" s="134"/>
-      <c r="CC2" s="134"/>
-      <c r="CD2" s="134"/>
-      <c r="CE2" s="134"/>
-      <c r="CF2" s="134"/>
-      <c r="CG2" s="134"/>
-      <c r="CH2" s="134"/>
-      <c r="CI2" s="134"/>
-      <c r="CJ2" s="134"/>
-      <c r="CK2" s="134"/>
-      <c r="CL2" s="134"/>
-      <c r="CM2" s="134"/>
-      <c r="CN2" s="134"/>
-      <c r="CO2" s="134"/>
-      <c r="CP2" s="134"/>
-      <c r="CQ2" s="134"/>
-      <c r="CR2" s="134"/>
-      <c r="CS2" s="134"/>
-      <c r="CT2" s="134"/>
-      <c r="CU2" s="134"/>
-      <c r="CV2" s="134"/>
-      <c r="CW2" s="134"/>
-      <c r="CX2" s="134"/>
-      <c r="CY2" s="134"/>
-      <c r="CZ2" s="134"/>
-      <c r="DA2" s="134"/>
-      <c r="DB2" s="134"/>
-      <c r="DC2" s="134"/>
-      <c r="DD2" s="134"/>
-      <c r="DE2" s="134"/>
-      <c r="DF2" s="134"/>
-      <c r="DG2" s="134"/>
-      <c r="DH2" s="134"/>
-      <c r="DI2" s="134"/>
-      <c r="DJ2" s="134"/>
-      <c r="DK2" s="134"/>
-      <c r="DL2" s="134"/>
-      <c r="DM2" s="134"/>
-      <c r="DN2" s="134"/>
-      <c r="DO2" s="134"/>
-      <c r="DP2" s="134"/>
-      <c r="DQ2" s="134"/>
-      <c r="DR2" s="134"/>
-      <c r="DS2" s="134"/>
-      <c r="DT2" s="134"/>
-      <c r="DU2" s="134"/>
-      <c r="DV2" s="134"/>
-      <c r="DW2" s="134"/>
-      <c r="DX2" s="134"/>
-      <c r="DY2" s="134"/>
-      <c r="DZ2" s="134"/>
-      <c r="EA2" s="134"/>
-      <c r="EB2" s="134"/>
-      <c r="EC2" s="134"/>
-      <c r="ED2" s="134"/>
-      <c r="EE2" s="134"/>
-      <c r="EF2" s="134"/>
-      <c r="EG2" s="134"/>
-      <c r="EH2" s="134"/>
-      <c r="EI2" s="134"/>
-      <c r="EJ2" s="134"/>
-      <c r="EK2" s="134"/>
-      <c r="EL2" s="134"/>
-      <c r="EM2" s="134"/>
-      <c r="EN2" s="134"/>
-      <c r="EO2" s="134"/>
-      <c r="EP2" s="134"/>
-      <c r="EQ2" s="134"/>
-      <c r="ER2" s="134"/>
-      <c r="ES2" s="134"/>
-      <c r="ET2" s="134"/>
-      <c r="EU2" s="134"/>
-      <c r="EV2" s="134"/>
-      <c r="EW2" s="134"/>
-      <c r="EX2" s="134"/>
-      <c r="EY2" s="134"/>
-      <c r="EZ2" s="134"/>
-      <c r="FA2" s="134"/>
-      <c r="FB2" s="134"/>
-      <c r="FC2" s="134"/>
-      <c r="FD2" s="134"/>
-      <c r="FE2" s="134"/>
-      <c r="FF2" s="134"/>
-      <c r="FG2" s="134"/>
-      <c r="FH2" s="134"/>
-      <c r="FI2" s="134"/>
-      <c r="FJ2" s="134"/>
-      <c r="FK2" s="134"/>
-      <c r="FL2" s="134"/>
-      <c r="FM2" s="134"/>
-      <c r="FN2" s="134"/>
-      <c r="FO2" s="134"/>
-      <c r="FP2" s="134"/>
-      <c r="FQ2" s="134"/>
-      <c r="FR2" s="134"/>
-      <c r="FS2" s="134"/>
-      <c r="FT2" s="134"/>
-      <c r="FU2" s="134"/>
-      <c r="FV2" s="134"/>
-      <c r="FW2" s="134"/>
-      <c r="FX2" s="134"/>
-      <c r="FY2" s="134"/>
-      <c r="FZ2" s="134"/>
-      <c r="GA2" s="134"/>
-      <c r="GB2" s="134"/>
-      <c r="GC2" s="134"/>
-      <c r="GD2" s="134"/>
-      <c r="GE2" s="134"/>
-      <c r="GF2" s="134"/>
-      <c r="GG2" s="134"/>
-      <c r="GH2" s="134"/>
-      <c r="GI2" s="134"/>
-      <c r="GJ2" s="134"/>
-      <c r="GK2" s="134"/>
-      <c r="GL2" s="134"/>
-      <c r="GM2" s="134"/>
-      <c r="GN2" s="134"/>
-      <c r="GO2" s="134"/>
-      <c r="GP2" s="134"/>
-      <c r="GQ2" s="134"/>
-      <c r="GR2" s="134"/>
-      <c r="GS2" s="134"/>
-      <c r="GT2" s="134"/>
-      <c r="GU2" s="134"/>
-      <c r="GV2" s="134"/>
-      <c r="GW2" s="134"/>
-      <c r="GX2" s="134"/>
-      <c r="GY2" s="134"/>
-      <c r="GZ2" s="134"/>
-      <c r="HA2" s="134"/>
-      <c r="HB2" s="134"/>
-      <c r="HC2" s="134"/>
-      <c r="HD2" s="134"/>
-      <c r="HE2" s="134"/>
-      <c r="HF2" s="134"/>
-      <c r="HG2" s="134"/>
-      <c r="HH2" s="134"/>
-      <c r="HI2" s="134"/>
-      <c r="HJ2" s="134"/>
-      <c r="HK2" s="134"/>
-      <c r="HL2" s="134"/>
-      <c r="HM2" s="134"/>
-      <c r="HN2" s="134"/>
-      <c r="HO2" s="134"/>
-      <c r="HP2" s="134"/>
-      <c r="HQ2" s="134"/>
-      <c r="HR2" s="134"/>
-      <c r="HS2" s="134"/>
-      <c r="HT2" s="134"/>
-      <c r="HU2" s="134"/>
-      <c r="HV2" s="134"/>
-      <c r="HW2" s="134"/>
-      <c r="HX2" s="134"/>
-      <c r="HY2" s="134"/>
-      <c r="HZ2" s="134"/>
-      <c r="IA2" s="134"/>
-      <c r="IB2" s="134"/>
-      <c r="IC2" s="134"/>
-      <c r="ID2" s="134"/>
-      <c r="IE2" s="134"/>
-      <c r="IF2" s="134"/>
-      <c r="IG2" s="134"/>
-      <c r="IH2" s="134"/>
-      <c r="II2" s="134"/>
-      <c r="IJ2" s="134"/>
-      <c r="IK2" s="134"/>
-      <c r="IL2" s="134"/>
-      <c r="IM2" s="134"/>
-      <c r="IN2" s="134"/>
-      <c r="IO2" s="134"/>
-      <c r="IP2" s="134"/>
-      <c r="IQ2" s="134"/>
-      <c r="IR2" s="134"/>
-      <c r="IS2" s="134"/>
-      <c r="IT2" s="134"/>
-      <c r="IU2" s="135"/>
-    </row>
-    <row r="3" spans="1:255">
-      <c r="A3" s="136" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="136" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="137" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="137" t="s">
-        <v>254</v>
-      </c>
-      <c r="E3" s="137" t="s">
+      <c r="E3" s="131" t="s">
         <v>246</v>
       </c>
-      <c r="F3" s="138" t="s">
+      <c r="F3" s="132" t="s">
         <v>247</v>
       </c>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="139"/>
-      <c r="K3" s="139"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="141"/>
-      <c r="N3" s="141"/>
-      <c r="O3" s="141"/>
-      <c r="P3" s="141"/>
-      <c r="Q3" s="141"/>
-      <c r="R3" s="141"/>
-      <c r="S3" s="141"/>
-      <c r="T3" s="141"/>
-      <c r="U3" s="141"/>
-      <c r="V3" s="141"/>
-      <c r="W3" s="141"/>
-      <c r="X3" s="141"/>
-      <c r="Y3" s="141"/>
-      <c r="Z3" s="141"/>
-      <c r="AA3" s="141"/>
-      <c r="AB3" s="141"/>
-      <c r="AC3" s="141"/>
-      <c r="AD3" s="141"/>
-      <c r="AE3" s="141"/>
-      <c r="AF3" s="141"/>
-      <c r="AG3" s="141"/>
-      <c r="AH3" s="141"/>
-      <c r="AI3" s="141"/>
-      <c r="AJ3" s="141"/>
-      <c r="AK3" s="141"/>
-      <c r="AL3" s="141"/>
-      <c r="AM3" s="141"/>
-      <c r="AN3" s="141"/>
-      <c r="AO3" s="141"/>
-      <c r="AP3" s="141"/>
-      <c r="AQ3" s="141"/>
-      <c r="AR3" s="141"/>
-      <c r="AS3" s="141"/>
-      <c r="AT3" s="141"/>
-      <c r="AU3" s="141"/>
-      <c r="AV3" s="141"/>
-      <c r="AW3" s="141"/>
-      <c r="AX3" s="141"/>
-      <c r="AY3" s="141"/>
-      <c r="AZ3" s="141"/>
-      <c r="BA3" s="141"/>
-      <c r="BB3" s="141"/>
-      <c r="BC3" s="141"/>
-      <c r="BD3" s="141"/>
-      <c r="BE3" s="141"/>
-      <c r="BF3" s="141"/>
-      <c r="BG3" s="141"/>
-      <c r="BH3" s="141"/>
-      <c r="BI3" s="141"/>
-      <c r="BJ3" s="141"/>
-      <c r="BK3" s="141"/>
-      <c r="BL3" s="141"/>
-      <c r="BM3" s="141"/>
-      <c r="BN3" s="141"/>
-      <c r="BO3" s="141"/>
-      <c r="BP3" s="141"/>
-      <c r="BQ3" s="141"/>
-      <c r="BR3" s="141"/>
-      <c r="BS3" s="141"/>
-      <c r="BT3" s="141"/>
-      <c r="BU3" s="141"/>
-      <c r="BV3" s="141"/>
-      <c r="BW3" s="141"/>
-      <c r="BX3" s="141"/>
-      <c r="BY3" s="141"/>
-      <c r="BZ3" s="141"/>
-      <c r="CA3" s="141"/>
-      <c r="CB3" s="141"/>
-      <c r="CC3" s="141"/>
-      <c r="CD3" s="141"/>
-      <c r="CE3" s="141"/>
-      <c r="CF3" s="141"/>
-      <c r="CG3" s="141"/>
-      <c r="CH3" s="141"/>
-      <c r="CI3" s="141"/>
-      <c r="CJ3" s="141"/>
-      <c r="CK3" s="141"/>
-      <c r="CL3" s="141"/>
-      <c r="CM3" s="141"/>
-      <c r="CN3" s="141"/>
-      <c r="CO3" s="141"/>
-      <c r="CP3" s="141"/>
-      <c r="CQ3" s="141"/>
-      <c r="CR3" s="141"/>
-      <c r="CS3" s="141"/>
-      <c r="CT3" s="141"/>
-      <c r="CU3" s="141"/>
-      <c r="CV3" s="141"/>
-      <c r="CW3" s="141"/>
-      <c r="CX3" s="141"/>
-      <c r="CY3" s="141"/>
-      <c r="CZ3" s="141"/>
-      <c r="DA3" s="141"/>
-      <c r="DB3" s="141"/>
-      <c r="DC3" s="141"/>
-      <c r="DD3" s="141"/>
-      <c r="DE3" s="141"/>
-      <c r="DF3" s="141"/>
-      <c r="DG3" s="141"/>
-      <c r="DH3" s="141"/>
-      <c r="DI3" s="141"/>
-      <c r="DJ3" s="141"/>
-      <c r="DK3" s="141"/>
-      <c r="DL3" s="141"/>
-      <c r="DM3" s="141"/>
-      <c r="DN3" s="141"/>
-      <c r="DO3" s="141"/>
-      <c r="DP3" s="141"/>
-      <c r="DQ3" s="141"/>
-      <c r="DR3" s="141"/>
-      <c r="DS3" s="141"/>
-      <c r="DT3" s="141"/>
-      <c r="DU3" s="141"/>
-      <c r="DV3" s="141"/>
-      <c r="DW3" s="141"/>
-      <c r="DX3" s="141"/>
-      <c r="DY3" s="141"/>
-      <c r="DZ3" s="141"/>
-      <c r="EA3" s="141"/>
-      <c r="EB3" s="141"/>
-      <c r="EC3" s="141"/>
-      <c r="ED3" s="141"/>
-      <c r="EE3" s="141"/>
-      <c r="EF3" s="141"/>
-      <c r="EG3" s="141"/>
-      <c r="EH3" s="141"/>
-      <c r="EI3" s="141"/>
-      <c r="EJ3" s="141"/>
-      <c r="EK3" s="141"/>
-      <c r="EL3" s="141"/>
-      <c r="EM3" s="141"/>
-      <c r="EN3" s="141"/>
-      <c r="EO3" s="141"/>
-      <c r="EP3" s="141"/>
-      <c r="EQ3" s="141"/>
-      <c r="ER3" s="141"/>
-      <c r="ES3" s="141"/>
-      <c r="ET3" s="141"/>
-      <c r="EU3" s="141"/>
-      <c r="EV3" s="141"/>
-      <c r="EW3" s="141"/>
-      <c r="EX3" s="141"/>
-      <c r="EY3" s="141"/>
-      <c r="EZ3" s="141"/>
-      <c r="FA3" s="141"/>
-      <c r="FB3" s="141"/>
-      <c r="FC3" s="141"/>
-      <c r="FD3" s="141"/>
-      <c r="FE3" s="141"/>
-      <c r="FF3" s="141"/>
-      <c r="FG3" s="141"/>
-      <c r="FH3" s="141"/>
-      <c r="FI3" s="141"/>
-      <c r="FJ3" s="141"/>
-      <c r="FK3" s="141"/>
-      <c r="FL3" s="141"/>
-      <c r="FM3" s="141"/>
-      <c r="FN3" s="141"/>
-      <c r="FO3" s="141"/>
-      <c r="FP3" s="141"/>
-      <c r="FQ3" s="141"/>
-      <c r="FR3" s="141"/>
-      <c r="FS3" s="141"/>
-      <c r="FT3" s="141"/>
-      <c r="FU3" s="141"/>
-      <c r="FV3" s="141"/>
-      <c r="FW3" s="141"/>
-      <c r="FX3" s="141"/>
-      <c r="FY3" s="141"/>
-      <c r="FZ3" s="141"/>
-      <c r="GA3" s="141"/>
-      <c r="GB3" s="141"/>
-      <c r="GC3" s="141"/>
-      <c r="GD3" s="141"/>
-      <c r="GE3" s="141"/>
-      <c r="GF3" s="141"/>
-      <c r="GG3" s="141"/>
-      <c r="GH3" s="141"/>
-      <c r="GI3" s="141"/>
-      <c r="GJ3" s="141"/>
-      <c r="GK3" s="141"/>
-      <c r="GL3" s="141"/>
-      <c r="GM3" s="141"/>
-      <c r="GN3" s="141"/>
-      <c r="GO3" s="141"/>
-      <c r="GP3" s="141"/>
-      <c r="GQ3" s="141"/>
-      <c r="GR3" s="141"/>
-      <c r="GS3" s="141"/>
-      <c r="GT3" s="141"/>
-      <c r="GU3" s="141"/>
-      <c r="GV3" s="141"/>
-      <c r="GW3" s="141"/>
-      <c r="GX3" s="141"/>
-      <c r="GY3" s="141"/>
-      <c r="GZ3" s="141"/>
-      <c r="HA3" s="141"/>
-      <c r="HB3" s="141"/>
-      <c r="HC3" s="141"/>
-      <c r="HD3" s="141"/>
-      <c r="HE3" s="141"/>
-      <c r="HF3" s="141"/>
-      <c r="HG3" s="141"/>
-      <c r="HH3" s="141"/>
-      <c r="HI3" s="141"/>
-      <c r="HJ3" s="141"/>
-      <c r="HK3" s="141"/>
-      <c r="HL3" s="141"/>
-      <c r="HM3" s="141"/>
-      <c r="HN3" s="141"/>
-      <c r="HO3" s="141"/>
-      <c r="HP3" s="141"/>
-      <c r="HQ3" s="141"/>
-      <c r="HR3" s="141"/>
-      <c r="HS3" s="141"/>
-      <c r="HT3" s="141"/>
-      <c r="HU3" s="141"/>
-      <c r="HV3" s="141"/>
-      <c r="HW3" s="141"/>
-      <c r="HX3" s="141"/>
-      <c r="HY3" s="141"/>
-      <c r="HZ3" s="141"/>
-      <c r="IA3" s="141"/>
-      <c r="IB3" s="141"/>
-      <c r="IC3" s="141"/>
-      <c r="ID3" s="141"/>
-      <c r="IE3" s="141"/>
-      <c r="IF3" s="141"/>
-      <c r="IG3" s="141"/>
-      <c r="IH3" s="141"/>
-      <c r="II3" s="141"/>
-      <c r="IJ3" s="141"/>
-      <c r="IK3" s="141"/>
-      <c r="IL3" s="141"/>
-      <c r="IM3" s="141"/>
-      <c r="IN3" s="141"/>
-      <c r="IO3" s="141"/>
-      <c r="IP3" s="141"/>
-      <c r="IQ3" s="141"/>
-      <c r="IR3" s="141"/>
-      <c r="IS3" s="141"/>
-      <c r="IT3" s="141"/>
-      <c r="IU3" s="142"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="135"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="135"/>
+      <c r="T3" s="135"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="135"/>
+      <c r="X3" s="135"/>
+      <c r="Y3" s="135"/>
+      <c r="Z3" s="135"/>
+      <c r="AA3" s="135"/>
+      <c r="AB3" s="135"/>
+      <c r="AC3" s="135"/>
+      <c r="AD3" s="135"/>
+      <c r="AE3" s="135"/>
+      <c r="AF3" s="135"/>
+      <c r="AG3" s="135"/>
+      <c r="AH3" s="135"/>
+      <c r="AI3" s="135"/>
+      <c r="AJ3" s="135"/>
+      <c r="AK3" s="135"/>
+      <c r="AL3" s="135"/>
+      <c r="AM3" s="135"/>
+      <c r="AN3" s="135"/>
+      <c r="AO3" s="135"/>
+      <c r="AP3" s="135"/>
+      <c r="AQ3" s="135"/>
+      <c r="AR3" s="135"/>
+      <c r="AS3" s="135"/>
+      <c r="AT3" s="135"/>
+      <c r="AU3" s="135"/>
+      <c r="AV3" s="135"/>
+      <c r="AW3" s="135"/>
+      <c r="AX3" s="135"/>
+      <c r="AY3" s="135"/>
+      <c r="AZ3" s="135"/>
+      <c r="BA3" s="135"/>
+      <c r="BB3" s="135"/>
+      <c r="BC3" s="135"/>
+      <c r="BD3" s="135"/>
+      <c r="BE3" s="135"/>
+      <c r="BF3" s="135"/>
+      <c r="BG3" s="135"/>
+      <c r="BH3" s="135"/>
+      <c r="BI3" s="135"/>
+      <c r="BJ3" s="135"/>
+      <c r="BK3" s="135"/>
+      <c r="BL3" s="135"/>
+      <c r="BM3" s="135"/>
+      <c r="BN3" s="135"/>
+      <c r="BO3" s="135"/>
+      <c r="BP3" s="135"/>
+      <c r="BQ3" s="135"/>
+      <c r="BR3" s="135"/>
+      <c r="BS3" s="135"/>
+      <c r="BT3" s="135"/>
+      <c r="BU3" s="135"/>
+      <c r="BV3" s="135"/>
+      <c r="BW3" s="135"/>
+      <c r="BX3" s="135"/>
+      <c r="BY3" s="135"/>
+      <c r="BZ3" s="135"/>
+      <c r="CA3" s="135"/>
+      <c r="CB3" s="135"/>
+      <c r="CC3" s="135"/>
+      <c r="CD3" s="135"/>
+      <c r="CE3" s="135"/>
+      <c r="CF3" s="135"/>
+      <c r="CG3" s="135"/>
+      <c r="CH3" s="135"/>
+      <c r="CI3" s="135"/>
+      <c r="CJ3" s="135"/>
+      <c r="CK3" s="135"/>
+      <c r="CL3" s="135"/>
+      <c r="CM3" s="135"/>
+      <c r="CN3" s="135"/>
+      <c r="CO3" s="135"/>
+      <c r="CP3" s="135"/>
+      <c r="CQ3" s="135"/>
+      <c r="CR3" s="135"/>
+      <c r="CS3" s="135"/>
+      <c r="CT3" s="135"/>
+      <c r="CU3" s="135"/>
+      <c r="CV3" s="135"/>
+      <c r="CW3" s="135"/>
+      <c r="CX3" s="135"/>
+      <c r="CY3" s="135"/>
+      <c r="CZ3" s="135"/>
+      <c r="DA3" s="135"/>
+      <c r="DB3" s="135"/>
+      <c r="DC3" s="135"/>
+      <c r="DD3" s="135"/>
+      <c r="DE3" s="135"/>
+      <c r="DF3" s="135"/>
+      <c r="DG3" s="135"/>
+      <c r="DH3" s="135"/>
+      <c r="DI3" s="135"/>
+      <c r="DJ3" s="135"/>
+      <c r="DK3" s="135"/>
+      <c r="DL3" s="135"/>
+      <c r="DM3" s="135"/>
+      <c r="DN3" s="135"/>
+      <c r="DO3" s="135"/>
+      <c r="DP3" s="135"/>
+      <c r="DQ3" s="135"/>
+      <c r="DR3" s="135"/>
+      <c r="DS3" s="135"/>
+      <c r="DT3" s="135"/>
+      <c r="DU3" s="135"/>
+      <c r="DV3" s="135"/>
+      <c r="DW3" s="135"/>
+      <c r="DX3" s="135"/>
+      <c r="DY3" s="135"/>
+      <c r="DZ3" s="135"/>
+      <c r="EA3" s="135"/>
+      <c r="EB3" s="135"/>
+      <c r="EC3" s="135"/>
+      <c r="ED3" s="135"/>
+      <c r="EE3" s="135"/>
+      <c r="EF3" s="135"/>
+      <c r="EG3" s="135"/>
+      <c r="EH3" s="135"/>
+      <c r="EI3" s="135"/>
+      <c r="EJ3" s="135"/>
+      <c r="EK3" s="135"/>
+      <c r="EL3" s="135"/>
+      <c r="EM3" s="135"/>
+      <c r="EN3" s="135"/>
+      <c r="EO3" s="135"/>
+      <c r="EP3" s="135"/>
+      <c r="EQ3" s="135"/>
+      <c r="ER3" s="135"/>
+      <c r="ES3" s="135"/>
+      <c r="ET3" s="135"/>
+      <c r="EU3" s="135"/>
+      <c r="EV3" s="135"/>
+      <c r="EW3" s="135"/>
+      <c r="EX3" s="135"/>
+      <c r="EY3" s="135"/>
+      <c r="EZ3" s="135"/>
+      <c r="FA3" s="135"/>
+      <c r="FB3" s="135"/>
+      <c r="FC3" s="135"/>
+      <c r="FD3" s="135"/>
+      <c r="FE3" s="135"/>
+      <c r="FF3" s="135"/>
+      <c r="FG3" s="135"/>
+      <c r="FH3" s="135"/>
+      <c r="FI3" s="135"/>
+      <c r="FJ3" s="135"/>
+      <c r="FK3" s="135"/>
+      <c r="FL3" s="135"/>
+      <c r="FM3" s="135"/>
+      <c r="FN3" s="135"/>
+      <c r="FO3" s="135"/>
+      <c r="FP3" s="135"/>
+      <c r="FQ3" s="135"/>
+      <c r="FR3" s="135"/>
+      <c r="FS3" s="135"/>
+      <c r="FT3" s="135"/>
+      <c r="FU3" s="135"/>
+      <c r="FV3" s="135"/>
+      <c r="FW3" s="135"/>
+      <c r="FX3" s="135"/>
+      <c r="FY3" s="135"/>
+      <c r="FZ3" s="135"/>
+      <c r="GA3" s="135"/>
+      <c r="GB3" s="135"/>
+      <c r="GC3" s="135"/>
+      <c r="GD3" s="135"/>
+      <c r="GE3" s="135"/>
+      <c r="GF3" s="135"/>
+      <c r="GG3" s="135"/>
+      <c r="GH3" s="135"/>
+      <c r="GI3" s="135"/>
+      <c r="GJ3" s="135"/>
+      <c r="GK3" s="135"/>
+      <c r="GL3" s="135"/>
+      <c r="GM3" s="135"/>
+      <c r="GN3" s="135"/>
+      <c r="GO3" s="135"/>
+      <c r="GP3" s="135"/>
+      <c r="GQ3" s="135"/>
+      <c r="GR3" s="135"/>
+      <c r="GS3" s="135"/>
+      <c r="GT3" s="135"/>
+      <c r="GU3" s="135"/>
+      <c r="GV3" s="135"/>
+      <c r="GW3" s="135"/>
+      <c r="GX3" s="135"/>
+      <c r="GY3" s="135"/>
+      <c r="GZ3" s="135"/>
+      <c r="HA3" s="135"/>
+      <c r="HB3" s="135"/>
+      <c r="HC3" s="135"/>
+      <c r="HD3" s="135"/>
+      <c r="HE3" s="135"/>
+      <c r="HF3" s="135"/>
+      <c r="HG3" s="135"/>
+      <c r="HH3" s="135"/>
+      <c r="HI3" s="135"/>
+      <c r="HJ3" s="135"/>
+      <c r="HK3" s="135"/>
+      <c r="HL3" s="135"/>
+      <c r="HM3" s="135"/>
+      <c r="HN3" s="135"/>
+      <c r="HO3" s="135"/>
+      <c r="HP3" s="135"/>
+      <c r="HQ3" s="135"/>
+      <c r="HR3" s="135"/>
+      <c r="HS3" s="135"/>
+      <c r="HT3" s="135"/>
+      <c r="HU3" s="135"/>
+      <c r="HV3" s="135"/>
+      <c r="HW3" s="135"/>
+      <c r="HX3" s="135"/>
+      <c r="HY3" s="135"/>
+      <c r="HZ3" s="135"/>
+      <c r="IA3" s="135"/>
+      <c r="IB3" s="135"/>
+      <c r="IC3" s="135"/>
+      <c r="ID3" s="135"/>
+      <c r="IE3" s="135"/>
+      <c r="IF3" s="135"/>
+      <c r="IG3" s="135"/>
+      <c r="IH3" s="135"/>
+      <c r="II3" s="135"/>
+      <c r="IJ3" s="135"/>
+      <c r="IK3" s="135"/>
+      <c r="IL3" s="135"/>
+      <c r="IM3" s="135"/>
+      <c r="IN3" s="135"/>
+      <c r="IO3" s="135"/>
+      <c r="IP3" s="135"/>
+      <c r="IQ3" s="135"/>
+      <c r="IR3" s="135"/>
+      <c r="IS3" s="135"/>
+      <c r="IT3" s="135"/>
+      <c r="IU3" s="136"/>
     </row>
     <row r="4" spans="1:255">
       <c r="A4" s="15">
@@ -9119,15 +8422,15 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" s="143" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="137" t="s">
         <v>156</v>
       </c>
       <c r="E4" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F4" s="144" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="138" t="s">
         <v>247</v>
       </c>
     </row>
@@ -9137,15 +8440,15 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" s="145" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="139" t="s">
         <v>158</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F5" s="146" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="140" t="s">
         <v>247</v>
       </c>
     </row>
@@ -9155,129 +8458,21 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="147" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="141" t="s">
         <v>160</v>
       </c>
       <c r="E6" s="92" t="s">
-        <v>264</v>
-      </c>
-      <c r="F6" s="148" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:255">
-      <c r="A7" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D7" s="143" t="s">
-        <v>156</v>
-      </c>
-      <c r="E7" s="94" t="s">
-        <v>248</v>
-      </c>
-      <c r="F7" s="144" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" spans="1:255">
-      <c r="A8" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D8" s="145" t="s">
-        <v>158</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F8" s="146" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:255">
-      <c r="A9" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D9" s="147" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" s="112" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" s="148" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:255">
-      <c r="A10" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D10" s="143" t="s">
-        <v>156</v>
-      </c>
-      <c r="E10" s="92" t="s">
-        <v>249</v>
-      </c>
-      <c r="F10" s="144" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="11" spans="1:255">
-      <c r="A11" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D11" s="145" t="s">
-        <v>158</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F11" s="146" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="12" spans="1:255">
-      <c r="A12" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D12" s="147" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="100" t="s">
-        <v>249</v>
-      </c>
-      <c r="F12" s="148" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="142" t="s">
         <v>247</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9296,7 +8491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -9411,13 +8606,13 @@
       </c>
       <c r="B4" s="16"/>
       <c r="C4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -9578,16 +8773,16 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>258</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -9757,7 +8952,7 @@
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>45</v>
@@ -9780,7 +8975,7 @@
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>47</v>
@@ -9803,7 +8998,7 @@
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>50</v>
@@ -9826,7 +9021,7 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>52</v>
@@ -9849,7 +9044,7 @@
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>54</v>
@@ -9872,7 +9067,7 @@
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>56</v>
@@ -9895,7 +9090,7 @@
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>58</v>
@@ -9918,7 +9113,7 @@
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>60</v>
@@ -9941,7 +9136,7 @@
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>61</v>
@@ -9964,7 +9159,7 @@
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>64</v>
@@ -9987,7 +9182,7 @@
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>66</v>
@@ -10010,7 +9205,7 @@
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>68</v>
@@ -10033,7 +9228,7 @@
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>70</v>
@@ -10056,7 +9251,7 @@
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>72</v>
@@ -10079,7 +9274,7 @@
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>75</v>
@@ -10104,7 +9299,7 @@
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>78</v>
@@ -11394,7 +10589,7 @@
       </c>
       <c r="B4" s="43"/>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>156</v>
@@ -11415,7 +10610,7 @@
       </c>
       <c r="B5" s="43"/>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>158</v>
@@ -11435,7 +10630,7 @@
         <v>43101</v>
       </c>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>160</v>
@@ -11479,7 +10674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -11670,7 +10865,7 @@
       </c>
       <c r="B4" s="43"/>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="47" t="s">
         <v>179</v>
@@ -11702,7 +10897,7 @@
       </c>
       <c r="B5" s="43"/>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" s="51" t="s">
         <v>182</v>
@@ -11743,7 +10938,7 @@
       </c>
       <c r="B6" s="43"/>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>185</v>
@@ -11784,7 +10979,7 @@
       </c>
       <c r="B7" s="43"/>
       <c r="C7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7" s="54" t="s">
         <v>187</v>
@@ -11825,7 +11020,7 @@
       </c>
       <c r="B8" s="43"/>
       <c r="C8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D8" s="55" t="s">
         <v>189</v>
@@ -11884,7 +11079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -12034,7 +11229,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D4" s="47" t="s">
         <v>179</v>
@@ -12068,7 +11263,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D5" s="47" t="s">
         <v>179</v>
@@ -12103,7 +11298,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="47" t="s">
         <v>179</v>
@@ -12138,7 +11333,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D7" s="47" t="s">
         <v>179</v>
@@ -12173,7 +11368,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D8" s="47" t="s">
         <v>179</v>
@@ -12208,7 +11403,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D9" s="47" t="s">
         <v>179</v>
@@ -12243,7 +11438,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D10" s="47" t="s">
         <v>179</v>
@@ -12278,7 +11473,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>179</v>
@@ -12313,7 +11508,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>179</v>
@@ -12348,7 +11543,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D13" s="47" t="s">
         <v>179</v>
@@ -12383,7 +11578,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D14" s="47" t="s">
         <v>179</v>
@@ -12418,7 +11613,7 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D15" s="47" t="s">
         <v>179</v>
@@ -12453,7 +11648,7 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D16" s="47" t="s">
         <v>179</v>
@@ -12488,7 +11683,7 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D17" s="51" t="s">
         <v>182</v>
@@ -12523,7 +11718,7 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D18" s="51" t="s">
         <v>182</v>
@@ -12558,7 +11753,7 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D19" s="51" t="s">
         <v>182</v>
@@ -12593,7 +11788,7 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>182</v>
@@ -12628,7 +11823,7 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D21" s="51" t="s">
         <v>182</v>
@@ -12663,7 +11858,7 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D22" s="53" t="s">
         <v>185</v>
@@ -12698,7 +11893,7 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D23" s="53" t="s">
         <v>185</v>
@@ -12733,7 +11928,7 @@
       </c>
       <c r="B24" s="5"/>
       <c r="C24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D24" s="53" t="s">
         <v>185</v>
@@ -12768,7 +11963,7 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D25" s="54" t="s">
         <v>187</v>
@@ -12802,7 +11997,7 @@
       </c>
       <c r="B26" s="5"/>
       <c r="C26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D26" s="54" t="s">
         <v>187</v>
@@ -12837,7 +12032,7 @@
       </c>
       <c r="B27" s="5"/>
       <c r="C27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D27" s="54" t="s">
         <v>187</v>
@@ -12872,7 +12067,7 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D28" s="54" t="s">
         <v>187</v>
@@ -12907,7 +12102,7 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D29" s="54" t="s">
         <v>187</v>
@@ -12942,7 +12137,7 @@
       </c>
       <c r="B30" s="5"/>
       <c r="C30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D30" s="55" t="s">
         <v>189</v>
@@ -12972,7 +12167,7 @@
       </c>
       <c r="B31" s="5"/>
       <c r="C31" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D31" s="55" t="s">
         <v>189</v>
@@ -13002,7 +12197,7 @@
       </c>
       <c r="B32" s="5"/>
       <c r="C32" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D32" s="55" t="s">
         <v>189</v>
@@ -13032,7 +12227,7 @@
       </c>
       <c r="B33" s="5"/>
       <c r="C33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D33" s="55" t="s">
         <v>189</v>
@@ -13062,7 +12257,7 @@
       </c>
       <c r="B34" s="5"/>
       <c r="C34" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D34" s="55" t="s">
         <v>189</v>

</xml_diff>

<commit_message>
Update spreadsheet change history
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B951313C-4E3E-F44F-8B11-4DEFB546B88E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF96C10-B100-D647-AEBD-6294E75D4244}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1340" windowWidth="25600" windowHeight="13040" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1340" windowWidth="25600" windowHeight="13040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$L$18</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="233">
   <si>
     <t>Change History</t>
   </si>
@@ -734,6 +735,30 @@
   </si>
   <si>
     <t>Cherished</t>
+  </si>
+  <si>
+    <t>Leszek Gonczar</t>
+  </si>
+  <si>
+    <t>Added attachScannedDocs case event</t>
+  </si>
+  <si>
+    <t>Removed scanDocument1 field from case</t>
+  </si>
+  <si>
+    <t>Renamed scanDocument2 field to scannedDocuments</t>
+  </si>
+  <si>
+    <t>Renamed ServiceDocument complex type to ScannedDocument</t>
+  </si>
+  <si>
+    <t>Changed the field set in ScannedDocument complex type</t>
+  </si>
+  <si>
+    <t>Luigi Bitonti</t>
+  </si>
+  <si>
+    <t>Set jurisdiction to BULKSCAN</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1296,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1532,6 +1557,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -1668,7 +1694,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1720,7 +1746,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1922,17 +1948,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+    <col min="2" max="2" width="50.5" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1972,29 +2000,113 @@
         <v>7</v>
       </c>
       <c r="D4" s="6">
-        <v>43383</v>
+        <v>43353</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="2"/>
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6">
+        <v>43376</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43382</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="5"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="2"/>
+      <c r="A7" s="146">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6">
+        <v>43382</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="146">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6">
+        <v>43382</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="146">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>43382</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="146">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6">
+        <v>43382</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -9230,7 +9342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix the version of the first change in spreadsheet's change history
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF96C10-B100-D647-AEBD-6294E75D4244}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A75DB9-76DD-694D-B4EF-5DC0EB4B969A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1340" windowWidth="25600" windowHeight="13040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$L$18</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="232">
   <si>
     <t>Change History</t>
   </si>
@@ -660,9 +659,6 @@
   </si>
   <si>
     <t>bulkscan+ccd@gmail.com</t>
-  </si>
-  <si>
-    <t>Scanned Corespondance</t>
   </si>
   <si>
     <t>Nitin Prabhu</t>
@@ -1951,7 +1947,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1990,8 +1986,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>200</v>
+      <c r="A4" s="5">
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2003,7 +1999,7 @@
         <v>43353</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2011,7 +2007,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -2020,7 +2016,7 @@
         <v>43376</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2028,7 +2024,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -2037,7 +2033,7 @@
         <v>43382</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -2045,7 +2041,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -2054,7 +2050,7 @@
         <v>43382</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2062,7 +2058,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -2071,7 +2067,7 @@
         <v>43382</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -2079,7 +2075,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -2088,7 +2084,7 @@
         <v>43382</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -2096,7 +2092,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -2105,7 +2101,7 @@
         <v>43382</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2338,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I7" s="74">
         <v>4</v>
@@ -2635,7 +2631,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I18" s="74">
         <v>2</v>
@@ -6725,7 +6721,7 @@
         <v>199</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>196</v>
@@ -7002,7 +6998,7 @@
         <v>196</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>189</v>
@@ -7133,7 +7129,7 @@
         <v>45</v>
       </c>
       <c r="E4" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F4" s="94" t="s">
         <v>189</v>
@@ -7150,7 +7146,7 @@
         <v>47</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F5" s="96" t="s">
         <v>189</v>
@@ -7167,7 +7163,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F6" s="96" t="s">
         <v>189</v>
@@ -7184,7 +7180,7 @@
         <v>52</v>
       </c>
       <c r="E7" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F7" s="96" t="s">
         <v>189</v>
@@ -7201,7 +7197,7 @@
         <v>54</v>
       </c>
       <c r="E8" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F8" s="96" t="s">
         <v>189</v>
@@ -7218,7 +7214,7 @@
         <v>56</v>
       </c>
       <c r="E9" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F9" s="96" t="s">
         <v>189</v>
@@ -7235,7 +7231,7 @@
         <v>58</v>
       </c>
       <c r="E10" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F10" s="96" t="s">
         <v>189</v>
@@ -7252,7 +7248,7 @@
         <v>60</v>
       </c>
       <c r="E11" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F11" s="96" t="s">
         <v>189</v>
@@ -7269,7 +7265,7 @@
         <v>61</v>
       </c>
       <c r="E12" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F12" s="96" t="s">
         <v>189</v>
@@ -7286,7 +7282,7 @@
         <v>64</v>
       </c>
       <c r="E13" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F13" s="96" t="s">
         <v>189</v>
@@ -7303,7 +7299,7 @@
         <v>66</v>
       </c>
       <c r="E14" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F14" s="96" t="s">
         <v>189</v>
@@ -7320,7 +7316,7 @@
         <v>68</v>
       </c>
       <c r="E15" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F15" s="96" t="s">
         <v>189</v>
@@ -7337,7 +7333,7 @@
         <v>70</v>
       </c>
       <c r="E16" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F16" s="96" t="s">
         <v>189</v>
@@ -7351,10 +7347,10 @@
         <v>196</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E17" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F17" s="96" t="s">
         <v>189</v>
@@ -7372,7 +7368,7 @@
         <v>75</v>
       </c>
       <c r="E18" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F18" s="100" t="s">
         <v>189</v>
@@ -7503,7 +7499,7 @@
         <v>121</v>
       </c>
       <c r="E4" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F4" s="94" t="s">
         <v>189</v>
@@ -7521,7 +7517,7 @@
         <v>124</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F5" s="96" t="s">
         <v>189</v>
@@ -7539,7 +7535,7 @@
         <v>127</v>
       </c>
       <c r="E6" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F6" s="109" t="s">
         <v>189</v>
@@ -7557,7 +7553,7 @@
         <v>129</v>
       </c>
       <c r="E7" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F7" s="96" t="s">
         <v>189</v>
@@ -7575,7 +7571,7 @@
         <v>131</v>
       </c>
       <c r="E8" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F8" s="100" t="s">
         <v>189</v>
@@ -7590,10 +7586,10 @@
         <v>196</v>
       </c>
       <c r="D9" s="144" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E9" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F9" s="100" t="s">
         <v>189</v>
@@ -8447,7 +8443,7 @@
         <v>98</v>
       </c>
       <c r="E4" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F4" s="138" t="s">
         <v>189</v>
@@ -8465,7 +8461,7 @@
         <v>100</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F5" s="140" t="s">
         <v>189</v>
@@ -8483,7 +8479,7 @@
         <v>102</v>
       </c>
       <c r="E6" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F6" s="142" t="s">
         <v>189</v>
@@ -8625,10 +8621,10 @@
       </c>
       <c r="B4" s="16"/>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>195</v>
@@ -8801,7 +8797,7 @@
         <v>198</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -9273,7 +9269,7 @@
         <v>196</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>72</v>
@@ -9283,7 +9279,7 @@
         <v>74</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>30</v>
@@ -9562,16 +9558,16 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>49</v>
       </c>
       <c r="F6" s="145" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="33"/>
@@ -9593,16 +9589,16 @@
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="33"/>
@@ -9624,21 +9620,21 @@
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E8" s="33" t="s">
         <v>89</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="33"/>
       <c r="J8" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="33" t="s">
@@ -9657,16 +9653,16 @@
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="33"/>
@@ -9688,16 +9684,16 @@
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="33" t="s">
         <v>73</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="33"/>
@@ -9719,16 +9715,16 @@
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E11" s="35" t="s">
         <v>49</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="33"/>
@@ -9879,13 +9875,13 @@
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="E4" s="32" t="s">
         <v>223</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>224</v>
       </c>
       <c r="F4" s="33"/>
       <c r="H4" s="5"/>
@@ -9906,7 +9902,7 @@
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>93</v>
@@ -10897,22 +10893,22 @@
         <v>196</v>
       </c>
       <c r="D9" s="143" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" t="s">
         <v>205</v>
       </c>
-      <c r="E9" t="s">
-        <v>206</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G9" s="48">
         <v>6</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P9" s="28" t="s">
         <v>123</v>
@@ -11528,7 +11524,7 @@
         <v>121</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F16" s="48">
         <v>13</v>
@@ -11703,7 +11699,7 @@
         <v>124</v>
       </c>
       <c r="E21" s="68" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F21" s="48">
         <v>5</v>
@@ -11808,7 +11804,7 @@
         <v>127</v>
       </c>
       <c r="E24" s="69" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F24" s="48">
         <v>3</v>
@@ -11982,7 +11978,7 @@
         <v>129</v>
       </c>
       <c r="E29" s="67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F29" s="48">
         <v>5</v>
@@ -12107,7 +12103,7 @@
         <v>131</v>
       </c>
       <c r="E33" s="71" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F33" s="48">
         <v>4</v>

</xml_diff>

<commit_message>
got the callbacks on a defined address working.
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/projects/moj/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A75DB9-76DD-694D-B4EF-5DC0EB4B969A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41216C0-F2A5-294A-8C32-CBC674609658}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1340" windowWidth="25600" windowHeight="13040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="238">
   <si>
     <t>Change History</t>
   </si>
@@ -755,6 +755,24 @@
   </si>
   <si>
     <t>Set jurisdiction to BULKSCAN</t>
+  </si>
+  <si>
+    <t>http://host.docker.internal:60000/event/ccd/CREATE_EXCEPTION</t>
+  </si>
+  <si>
+    <t>http://host.docker.internal:60000/event/ccd/ATTACH_RECORD</t>
+  </si>
+  <si>
+    <t>http://host.docker.internal:60000/event/ccd/CREATE_NEW</t>
+  </si>
+  <si>
+    <t>http://host.docker.internal:60000/event/ccd/REJECT_RECORD</t>
+  </si>
+  <si>
+    <t>http://host.docker.internal:60000/event/ccd/UPDATED_MANUALLY</t>
+  </si>
+  <si>
+    <t>http://host.docker.internal:60000/event/ccd/ATTACH_SCANNED_DOC</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1388,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1554,6 +1571,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -1946,7 +1964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2037,7 +2055,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="146">
+      <c r="A7" s="145">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -2054,7 +2072,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="146">
+      <c r="A8" s="145">
         <v>5</v>
       </c>
       <c r="B8" t="s">
@@ -2071,7 +2089,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="146">
+      <c r="A9" s="145">
         <v>6</v>
       </c>
       <c r="B9" t="s">
@@ -2088,7 +2106,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="146">
+      <c r="A10" s="145">
         <v>7</v>
       </c>
       <c r="B10" t="s">
@@ -2175,13 +2193,13 @@
       <c r="F2" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="71" t="s">
         <v>159</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="I2" s="71" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2204,13 +2222,13 @@
       <c r="F3" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="G3" s="73" t="s">
+      <c r="G3" s="72" t="s">
         <v>163</v>
       </c>
       <c r="H3" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="72" t="s">
         <v>164</v>
       </c>
       <c r="J3" s="13"/>
@@ -2249,13 +2267,13 @@
       <c r="F4" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="74">
+      <c r="G4" s="73">
         <v>1</v>
       </c>
       <c r="H4" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="74">
+      <c r="I4" s="73">
         <v>1</v>
       </c>
     </row>
@@ -2276,13 +2294,13 @@
       <c r="F5" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G5" s="74">
+      <c r="G5" s="73">
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="I5" s="74">
+      <c r="I5" s="73">
         <v>2</v>
       </c>
     </row>
@@ -2303,13 +2321,13 @@
       <c r="F6" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="73">
         <v>1</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="74">
+      <c r="I6" s="73">
         <v>3</v>
       </c>
     </row>
@@ -2330,13 +2348,13 @@
       <c r="F7" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="74">
+      <c r="G7" s="73">
         <v>1</v>
       </c>
       <c r="H7" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="I7" s="74">
+      <c r="I7" s="73">
         <v>4</v>
       </c>
     </row>
@@ -2357,13 +2375,13 @@
       <c r="F8" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G8" s="74">
+      <c r="G8" s="73">
         <v>1</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="74">
+      <c r="I8" s="73">
         <v>5</v>
       </c>
     </row>
@@ -2384,13 +2402,13 @@
       <c r="F9" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G9" s="74">
+      <c r="G9" s="73">
         <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="74">
+      <c r="I9" s="73">
         <v>6</v>
       </c>
     </row>
@@ -2411,13 +2429,13 @@
       <c r="F10" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G10" s="74">
+      <c r="G10" s="73">
         <v>1</v>
       </c>
       <c r="H10" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="74">
+      <c r="I10" s="73">
         <v>7</v>
       </c>
     </row>
@@ -2438,13 +2456,13 @@
       <c r="F11" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G11" s="74">
+      <c r="G11" s="73">
         <v>1</v>
       </c>
       <c r="H11" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="74">
+      <c r="I11" s="73">
         <v>8</v>
       </c>
     </row>
@@ -2465,13 +2483,13 @@
       <c r="F12" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G12" s="74">
+      <c r="G12" s="73">
         <v>1</v>
       </c>
       <c r="H12" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="74">
+      <c r="I12" s="73">
         <v>9</v>
       </c>
     </row>
@@ -2492,13 +2510,13 @@
       <c r="F13" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G13" s="74">
+      <c r="G13" s="73">
         <v>1</v>
       </c>
       <c r="H13" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="74">
+      <c r="I13" s="73">
         <v>10</v>
       </c>
     </row>
@@ -2519,13 +2537,13 @@
       <c r="F14" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G14" s="74">
+      <c r="G14" s="73">
         <v>1</v>
       </c>
       <c r="H14" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="74">
+      <c r="I14" s="73">
         <v>11</v>
       </c>
     </row>
@@ -2546,13 +2564,13 @@
       <c r="F15" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G15" s="74">
+      <c r="G15" s="73">
         <v>1</v>
       </c>
       <c r="H15" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="74">
+      <c r="I15" s="73">
         <v>12</v>
       </c>
     </row>
@@ -2573,13 +2591,13 @@
       <c r="F16" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G16" s="74">
+      <c r="G16" s="73">
         <v>1</v>
       </c>
       <c r="H16" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="74">
+      <c r="I16" s="73">
         <v>13</v>
       </c>
     </row>
@@ -2600,13 +2618,13 @@
       <c r="F17" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="G17" s="74">
+      <c r="G17" s="73">
         <v>2</v>
       </c>
       <c r="H17" t="s">
         <v>70</v>
       </c>
-      <c r="I17" s="74">
+      <c r="I17" s="73">
         <v>1</v>
       </c>
     </row>
@@ -2627,13 +2645,13 @@
       <c r="F18" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="G18" s="74">
+      <c r="G18" s="73">
         <v>2</v>
       </c>
       <c r="H18" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="I18" s="74">
+      <c r="I18" s="73">
         <v>2</v>
       </c>
     </row>
@@ -2654,13 +2672,13 @@
       <c r="F19" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="74">
+      <c r="G19" s="73">
         <v>2</v>
       </c>
       <c r="H19" t="s">
         <v>75</v>
       </c>
-      <c r="I19" s="74">
+      <c r="I19" s="73">
         <v>3</v>
       </c>
     </row>
@@ -2743,27 +2761,27 @@
       <c r="F2" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="75"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="74"/>
+      <c r="AA2" s="74"/>
     </row>
     <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -2772,10 +2790,10 @@
       <c r="B3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="75" t="s">
         <v>145</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -2784,27 +2802,27 @@
       <c r="F3" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="77"/>
-      <c r="Y3" s="77"/>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="77"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
@@ -2823,27 +2841,27 @@
       <c r="F4" s="5">
         <v>1</v>
       </c>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="77"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="77"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
     </row>
     <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
@@ -2862,27 +2880,27 @@
       <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="77"/>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="76"/>
+      <c r="S5" s="76"/>
+      <c r="T5" s="76"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="76"/>
+      <c r="W5" s="76"/>
+      <c r="X5" s="76"/>
+      <c r="Y5" s="76"/>
+      <c r="Z5" s="76"/>
+      <c r="AA5" s="76"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A6" s="15">
@@ -2978,27 +2996,27 @@
       <c r="F2" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="75"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="74"/>
+      <c r="AA2" s="74"/>
     </row>
     <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -3007,10 +3025,10 @@
       <c r="B3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="75" t="s">
         <v>145</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -3019,27 +3037,27 @@
       <c r="F3" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="77"/>
+      <c r="X3" s="77"/>
+      <c r="Y3" s="77"/>
+      <c r="Z3" s="77"/>
+      <c r="AA3" s="77"/>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
@@ -3058,27 +3076,27 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="77"/>
     </row>
     <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
@@ -3097,27 +3115,27 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="77"/>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="76"/>
+      <c r="S5" s="76"/>
+      <c r="T5" s="76"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="76"/>
+      <c r="W5" s="76"/>
+      <c r="X5" s="76"/>
+      <c r="Y5" s="76"/>
+      <c r="Z5" s="76"/>
+      <c r="AA5" s="76"/>
     </row>
     <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
@@ -3136,27 +3154,27 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="77"/>
-      <c r="X6" s="77"/>
-      <c r="Y6" s="77"/>
-      <c r="Z6" s="77"/>
-      <c r="AA6" s="77"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="76"/>
+      <c r="V6" s="76"/>
+      <c r="W6" s="76"/>
+      <c r="X6" s="76"/>
+      <c r="Y6" s="76"/>
+      <c r="Z6" s="76"/>
+      <c r="AA6" s="76"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A7" s="15">
@@ -3208,28 +3226,28 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="32.1640625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="79" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="79" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="79" customWidth="1"/>
-    <col min="5" max="6" width="15.1640625" style="79" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="78" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="78" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="78" customWidth="1"/>
+    <col min="5" max="6" width="15.1640625" style="78" customWidth="1"/>
     <col min="7" max="1025" width="7.1640625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -4250,18 +4268,18 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024" ht="48" x14ac:dyDescent="0.15">
-      <c r="A2" s="85"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="86" t="s">
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="85" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="85" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="85" t="s">
         <v>178</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="85" t="s">
         <v>106</v>
       </c>
       <c r="G2"/>
@@ -5284,22 +5302,22 @@
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="86" t="s">
         <v>97</v>
       </c>
       <c r="G3"/>
@@ -6458,10 +6476,10 @@
       <c r="B3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="75" t="s">
         <v>145</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -6470,27 +6488,27 @@
       <c r="F3" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="77"/>
+      <c r="X3" s="77"/>
+      <c r="Y3" s="77"/>
+      <c r="Z3" s="77"/>
+      <c r="AA3" s="77"/>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
@@ -6509,27 +6527,27 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="77"/>
     </row>
     <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
@@ -6548,27 +6566,27 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="77"/>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="76"/>
+      <c r="S5" s="76"/>
+      <c r="T5" s="76"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="76"/>
+      <c r="W5" s="76"/>
+      <c r="X5" s="76"/>
+      <c r="Y5" s="76"/>
+      <c r="Z5" s="76"/>
+      <c r="AA5" s="76"/>
     </row>
     <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
@@ -6587,27 +6605,27 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="77"/>
-      <c r="X6" s="77"/>
-      <c r="Y6" s="77"/>
-      <c r="Z6" s="77"/>
-      <c r="AA6" s="77"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="76"/>
+      <c r="V6" s="76"/>
+      <c r="W6" s="76"/>
+      <c r="X6" s="76"/>
+      <c r="Y6" s="76"/>
+      <c r="Z6" s="76"/>
+      <c r="AA6" s="76"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A7" s="15">
@@ -6702,13 +6720,13 @@
       <c r="C3" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="87" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="87" t="s">
         <v>184</v>
       </c>
     </row>
@@ -6717,7 +6735,7 @@
         <v>43101</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="88" t="s">
         <v>199</v>
       </c>
       <c r="D4" s="33" t="s">
@@ -6733,7 +6751,7 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="15"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="89"/>
+      <c r="C5" s="88"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
@@ -6741,7 +6759,7 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="15"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="89"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
       <c r="F6" s="33"/>
@@ -6749,7 +6767,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="15"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="89"/>
+      <c r="C7" s="88"/>
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
       <c r="F7" s="33"/>
@@ -6765,7 +6783,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="15"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="89"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
@@ -6821,7 +6839,7 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="15"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="89"/>
+      <c r="C16" s="88"/>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
       <c r="F16" s="33"/>
@@ -6973,10 +6991,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="65" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="20" t="s">
@@ -6985,7 +7003,7 @@
       <c r="D3" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="65" t="s">
         <v>189</v>
       </c>
     </row>
@@ -7097,11 +7115,11 @@
       <c r="Z2" s="12"/>
       <c r="AA2" s="12"/>
     </row>
-    <row r="3" spans="1:27" s="66" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="66" t="s">
+    <row r="3" spans="1:27" s="65" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="65" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="20" t="s">
@@ -7113,30 +7131,30 @@
       <c r="E3" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="F3" s="65" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A4" s="90">
+      <c r="A4" s="89">
         <v>43101</v>
       </c>
-      <c r="B4" s="91"/>
+      <c r="B4" s="90"/>
       <c r="C4" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="93" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A5" s="95">
+      <c r="A5" s="94">
         <v>43101</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -7145,15 +7163,15 @@
       <c r="D5" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F5" s="96" t="s">
+      <c r="F5" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A6" s="95">
+      <c r="A6" s="94">
         <v>43101</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -7162,15 +7180,15 @@
       <c r="D6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F6" s="96" t="s">
+      <c r="F6" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A7" s="95">
+      <c r="A7" s="94">
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -7179,15 +7197,15 @@
       <c r="D7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A8" s="95">
+      <c r="A8" s="94">
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -7196,15 +7214,15 @@
       <c r="D8" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="92" t="s">
+      <c r="E8" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="96" t="s">
+      <c r="F8" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A9" s="95">
+      <c r="A9" s="94">
         <v>43101</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -7213,15 +7231,15 @@
       <c r="D9" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="92" t="s">
+      <c r="E9" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F9" s="96" t="s">
+      <c r="F9" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A10" s="95">
+      <c r="A10" s="94">
         <v>43101</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -7230,15 +7248,15 @@
       <c r="D10" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="92" t="s">
+      <c r="E10" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F10" s="96" t="s">
+      <c r="F10" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A11" s="95">
+      <c r="A11" s="94">
         <v>43101</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -7247,15 +7265,15 @@
       <c r="D11" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="92" t="s">
+      <c r="E11" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F11" s="96" t="s">
+      <c r="F11" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A12" s="95">
+      <c r="A12" s="94">
         <v>43101</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -7264,15 +7282,15 @@
       <c r="D12" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="92" t="s">
+      <c r="E12" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F12" s="96" t="s">
+      <c r="F12" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A13" s="95">
+      <c r="A13" s="94">
         <v>43101</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -7281,15 +7299,15 @@
       <c r="D13" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="92" t="s">
+      <c r="E13" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F13" s="96" t="s">
+      <c r="F13" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A14" s="95">
+      <c r="A14" s="94">
         <v>43101</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -7298,15 +7316,15 @@
       <c r="D14" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="92" t="s">
+      <c r="E14" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F14" s="96" t="s">
+      <c r="F14" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A15" s="95">
+      <c r="A15" s="94">
         <v>43101</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -7315,15 +7333,15 @@
       <c r="D15" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="92" t="s">
+      <c r="E15" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F15" s="96" t="s">
+      <c r="F15" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A16" s="95">
+      <c r="A16" s="94">
         <v>43101</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -7332,15 +7350,15 @@
       <c r="D16" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="92" t="s">
+      <c r="E16" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F16" s="96" t="s">
+      <c r="F16" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="95">
+      <c r="A17" s="94">
         <v>43101</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -7349,28 +7367,28 @@
       <c r="D17" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="E17" s="92" t="s">
+      <c r="E17" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F17" s="96" t="s">
+      <c r="F17" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="97">
+      <c r="A18" s="96">
         <v>43101</v>
       </c>
-      <c r="B18" s="98"/>
+      <c r="B18" s="97"/>
       <c r="C18" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D18" s="99" t="s">
+      <c r="D18" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="92" t="s">
+      <c r="E18" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F18" s="100" t="s">
+      <c r="F18" s="99" t="s">
         <v>189</v>
       </c>
     </row>
@@ -7410,17 +7428,17 @@
     <col min="7" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="105" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+    <row r="1" spans="1:27" s="104" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A1" s="100" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="104" t="s">
+      <c r="D1" s="103" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="19"/>
@@ -7467,11 +7485,11 @@
       <c r="Z2" s="18"/>
       <c r="AA2" s="18"/>
     </row>
-    <row r="3" spans="1:27" s="66" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="66" t="s">
+    <row r="3" spans="1:27" s="65" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="65" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="20" t="s">
@@ -7483,115 +7501,115 @@
       <c r="E3" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="F3" s="65" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A4" s="90">
+      <c r="A4" s="89">
         <v>43101</v>
       </c>
-      <c r="B4" s="91"/>
+      <c r="B4" s="90"/>
       <c r="C4" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="105" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="93" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A5" s="95">
+      <c r="A5" s="94">
         <v>43101</v>
       </c>
-      <c r="B5" s="107"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F5" s="96" t="s">
+      <c r="F5" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A6" s="95">
+      <c r="A6" s="94">
         <v>43101</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F6" s="109" t="s">
+      <c r="F6" s="108" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A7" s="95">
+      <c r="A7" s="94">
         <v>43101</v>
       </c>
-      <c r="B7" s="108"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="95" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A8" s="97">
+      <c r="A8" s="96">
         <v>43101</v>
       </c>
-      <c r="B8" s="110"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D8" s="111" t="s">
+      <c r="D8" s="110" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="92" t="s">
+      <c r="E8" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="100" t="s">
+      <c r="F8" s="99" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A9" s="97">
+      <c r="A9" s="96">
         <v>43101</v>
       </c>
-      <c r="B9" s="110"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="144" t="s">
+      <c r="D9" s="143" t="s">
         <v>204</v>
       </c>
-      <c r="E9" s="92" t="s">
+      <c r="E9" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F9" s="100" t="s">
+      <c r="F9" s="99" t="s">
         <v>189</v>
       </c>
     </row>
@@ -7622,814 +7640,814 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="112" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="112" customWidth="1"/>
-    <col min="3" max="3" width="23.5" style="112" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" style="112" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" style="112" customWidth="1"/>
-    <col min="6" max="6" width="36" style="113" customWidth="1"/>
-    <col min="7" max="255" width="12.5" style="112" customWidth="1"/>
-    <col min="256" max="1025" width="7.1640625" style="112" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" style="111" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="111" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="111" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" style="111" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" style="111" customWidth="1"/>
+    <col min="6" max="6" width="36" style="112" customWidth="1"/>
+    <col min="7" max="255" width="12.5" style="111" customWidth="1"/>
+    <col min="256" max="1025" width="7.1640625" style="111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="123" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:255" s="122" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A1" s="113" t="s">
         <v>193</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="118"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="121"/>
-      <c r="T1" s="121"/>
-      <c r="U1" s="121"/>
-      <c r="V1" s="121"/>
-      <c r="W1" s="121"/>
-      <c r="X1" s="121"/>
-      <c r="Y1" s="121"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="121"/>
-      <c r="AB1" s="121"/>
-      <c r="AC1" s="121"/>
-      <c r="AD1" s="121"/>
-      <c r="AE1" s="121"/>
-      <c r="AF1" s="121"/>
-      <c r="AG1" s="121"/>
-      <c r="AH1" s="121"/>
-      <c r="AI1" s="121"/>
-      <c r="AJ1" s="121"/>
-      <c r="AK1" s="121"/>
-      <c r="AL1" s="121"/>
-      <c r="AM1" s="121"/>
-      <c r="AN1" s="121"/>
-      <c r="AO1" s="121"/>
-      <c r="AP1" s="121"/>
-      <c r="AQ1" s="121"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="121"/>
-      <c r="AT1" s="121"/>
-      <c r="AU1" s="121"/>
-      <c r="AV1" s="121"/>
-      <c r="AW1" s="121"/>
-      <c r="AX1" s="121"/>
-      <c r="AY1" s="121"/>
-      <c r="AZ1" s="121"/>
-      <c r="BA1" s="121"/>
-      <c r="BB1" s="121"/>
-      <c r="BC1" s="121"/>
-      <c r="BD1" s="121"/>
-      <c r="BE1" s="121"/>
-      <c r="BF1" s="121"/>
-      <c r="BG1" s="121"/>
-      <c r="BH1" s="121"/>
-      <c r="BI1" s="121"/>
-      <c r="BJ1" s="121"/>
-      <c r="BK1" s="121"/>
-      <c r="BL1" s="121"/>
-      <c r="BM1" s="121"/>
-      <c r="BN1" s="121"/>
-      <c r="BO1" s="121"/>
-      <c r="BP1" s="121"/>
-      <c r="BQ1" s="121"/>
-      <c r="BR1" s="121"/>
-      <c r="BS1" s="121"/>
-      <c r="BT1" s="121"/>
-      <c r="BU1" s="121"/>
-      <c r="BV1" s="121"/>
-      <c r="BW1" s="121"/>
-      <c r="BX1" s="121"/>
-      <c r="BY1" s="121"/>
-      <c r="BZ1" s="121"/>
-      <c r="CA1" s="121"/>
-      <c r="CB1" s="121"/>
-      <c r="CC1" s="121"/>
-      <c r="CD1" s="121"/>
-      <c r="CE1" s="121"/>
-      <c r="CF1" s="121"/>
-      <c r="CG1" s="121"/>
-      <c r="CH1" s="121"/>
-      <c r="CI1" s="121"/>
-      <c r="CJ1" s="121"/>
-      <c r="CK1" s="121"/>
-      <c r="CL1" s="121"/>
-      <c r="CM1" s="121"/>
-      <c r="CN1" s="121"/>
-      <c r="CO1" s="121"/>
-      <c r="CP1" s="121"/>
-      <c r="CQ1" s="121"/>
-      <c r="CR1" s="121"/>
-      <c r="CS1" s="121"/>
-      <c r="CT1" s="121"/>
-      <c r="CU1" s="121"/>
-      <c r="CV1" s="121"/>
-      <c r="CW1" s="121"/>
-      <c r="CX1" s="121"/>
-      <c r="CY1" s="121"/>
-      <c r="CZ1" s="121"/>
-      <c r="DA1" s="121"/>
-      <c r="DB1" s="121"/>
-      <c r="DC1" s="121"/>
-      <c r="DD1" s="121"/>
-      <c r="DE1" s="121"/>
-      <c r="DF1" s="121"/>
-      <c r="DG1" s="121"/>
-      <c r="DH1" s="121"/>
-      <c r="DI1" s="121"/>
-      <c r="DJ1" s="121"/>
-      <c r="DK1" s="121"/>
-      <c r="DL1" s="121"/>
-      <c r="DM1" s="121"/>
-      <c r="DN1" s="121"/>
-      <c r="DO1" s="121"/>
-      <c r="DP1" s="121"/>
-      <c r="DQ1" s="121"/>
-      <c r="DR1" s="121"/>
-      <c r="DS1" s="121"/>
-      <c r="DT1" s="121"/>
-      <c r="DU1" s="121"/>
-      <c r="DV1" s="121"/>
-      <c r="DW1" s="121"/>
-      <c r="DX1" s="121"/>
-      <c r="DY1" s="121"/>
-      <c r="DZ1" s="121"/>
-      <c r="EA1" s="121"/>
-      <c r="EB1" s="121"/>
-      <c r="EC1" s="121"/>
-      <c r="ED1" s="121"/>
-      <c r="EE1" s="121"/>
-      <c r="EF1" s="121"/>
-      <c r="EG1" s="121"/>
-      <c r="EH1" s="121"/>
-      <c r="EI1" s="121"/>
-      <c r="EJ1" s="121"/>
-      <c r="EK1" s="121"/>
-      <c r="EL1" s="121"/>
-      <c r="EM1" s="121"/>
-      <c r="EN1" s="121"/>
-      <c r="EO1" s="121"/>
-      <c r="EP1" s="121"/>
-      <c r="EQ1" s="121"/>
-      <c r="ER1" s="121"/>
-      <c r="ES1" s="121"/>
-      <c r="ET1" s="121"/>
-      <c r="EU1" s="121"/>
-      <c r="EV1" s="121"/>
-      <c r="EW1" s="121"/>
-      <c r="EX1" s="121"/>
-      <c r="EY1" s="121"/>
-      <c r="EZ1" s="121"/>
-      <c r="FA1" s="121"/>
-      <c r="FB1" s="121"/>
-      <c r="FC1" s="121"/>
-      <c r="FD1" s="121"/>
-      <c r="FE1" s="121"/>
-      <c r="FF1" s="121"/>
-      <c r="FG1" s="121"/>
-      <c r="FH1" s="121"/>
-      <c r="FI1" s="121"/>
-      <c r="FJ1" s="121"/>
-      <c r="FK1" s="121"/>
-      <c r="FL1" s="121"/>
-      <c r="FM1" s="121"/>
-      <c r="FN1" s="121"/>
-      <c r="FO1" s="121"/>
-      <c r="FP1" s="121"/>
-      <c r="FQ1" s="121"/>
-      <c r="FR1" s="121"/>
-      <c r="FS1" s="121"/>
-      <c r="FT1" s="121"/>
-      <c r="FU1" s="121"/>
-      <c r="FV1" s="121"/>
-      <c r="FW1" s="121"/>
-      <c r="FX1" s="121"/>
-      <c r="FY1" s="121"/>
-      <c r="FZ1" s="121"/>
-      <c r="GA1" s="121"/>
-      <c r="GB1" s="121"/>
-      <c r="GC1" s="121"/>
-      <c r="GD1" s="121"/>
-      <c r="GE1" s="121"/>
-      <c r="GF1" s="121"/>
-      <c r="GG1" s="121"/>
-      <c r="GH1" s="121"/>
-      <c r="GI1" s="121"/>
-      <c r="GJ1" s="121"/>
-      <c r="GK1" s="121"/>
-      <c r="GL1" s="121"/>
-      <c r="GM1" s="121"/>
-      <c r="GN1" s="121"/>
-      <c r="GO1" s="121"/>
-      <c r="GP1" s="121"/>
-      <c r="GQ1" s="121"/>
-      <c r="GR1" s="121"/>
-      <c r="GS1" s="121"/>
-      <c r="GT1" s="121"/>
-      <c r="GU1" s="121"/>
-      <c r="GV1" s="121"/>
-      <c r="GW1" s="121"/>
-      <c r="GX1" s="121"/>
-      <c r="GY1" s="121"/>
-      <c r="GZ1" s="121"/>
-      <c r="HA1" s="121"/>
-      <c r="HB1" s="121"/>
-      <c r="HC1" s="121"/>
-      <c r="HD1" s="121"/>
-      <c r="HE1" s="121"/>
-      <c r="HF1" s="121"/>
-      <c r="HG1" s="121"/>
-      <c r="HH1" s="121"/>
-      <c r="HI1" s="121"/>
-      <c r="HJ1" s="121"/>
-      <c r="HK1" s="121"/>
-      <c r="HL1" s="121"/>
-      <c r="HM1" s="121"/>
-      <c r="HN1" s="121"/>
-      <c r="HO1" s="121"/>
-      <c r="HP1" s="121"/>
-      <c r="HQ1" s="121"/>
-      <c r="HR1" s="121"/>
-      <c r="HS1" s="121"/>
-      <c r="HT1" s="121"/>
-      <c r="HU1" s="121"/>
-      <c r="HV1" s="121"/>
-      <c r="HW1" s="121"/>
-      <c r="HX1" s="121"/>
-      <c r="HY1" s="121"/>
-      <c r="HZ1" s="121"/>
-      <c r="IA1" s="121"/>
-      <c r="IB1" s="121"/>
-      <c r="IC1" s="121"/>
-      <c r="ID1" s="121"/>
-      <c r="IE1" s="121"/>
-      <c r="IF1" s="121"/>
-      <c r="IG1" s="121"/>
-      <c r="IH1" s="121"/>
-      <c r="II1" s="121"/>
-      <c r="IJ1" s="121"/>
-      <c r="IK1" s="121"/>
-      <c r="IL1" s="121"/>
-      <c r="IM1" s="121"/>
-      <c r="IN1" s="121"/>
-      <c r="IO1" s="121"/>
-      <c r="IP1" s="121"/>
-      <c r="IQ1" s="121"/>
-      <c r="IR1" s="121"/>
-      <c r="IS1" s="121"/>
-      <c r="IT1" s="121"/>
-      <c r="IU1" s="122"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="120"/>
+      <c r="V1" s="120"/>
+      <c r="W1" s="120"/>
+      <c r="X1" s="120"/>
+      <c r="Y1" s="120"/>
+      <c r="Z1" s="120"/>
+      <c r="AA1" s="120"/>
+      <c r="AB1" s="120"/>
+      <c r="AC1" s="120"/>
+      <c r="AD1" s="120"/>
+      <c r="AE1" s="120"/>
+      <c r="AF1" s="120"/>
+      <c r="AG1" s="120"/>
+      <c r="AH1" s="120"/>
+      <c r="AI1" s="120"/>
+      <c r="AJ1" s="120"/>
+      <c r="AK1" s="120"/>
+      <c r="AL1" s="120"/>
+      <c r="AM1" s="120"/>
+      <c r="AN1" s="120"/>
+      <c r="AO1" s="120"/>
+      <c r="AP1" s="120"/>
+      <c r="AQ1" s="120"/>
+      <c r="AR1" s="120"/>
+      <c r="AS1" s="120"/>
+      <c r="AT1" s="120"/>
+      <c r="AU1" s="120"/>
+      <c r="AV1" s="120"/>
+      <c r="AW1" s="120"/>
+      <c r="AX1" s="120"/>
+      <c r="AY1" s="120"/>
+      <c r="AZ1" s="120"/>
+      <c r="BA1" s="120"/>
+      <c r="BB1" s="120"/>
+      <c r="BC1" s="120"/>
+      <c r="BD1" s="120"/>
+      <c r="BE1" s="120"/>
+      <c r="BF1" s="120"/>
+      <c r="BG1" s="120"/>
+      <c r="BH1" s="120"/>
+      <c r="BI1" s="120"/>
+      <c r="BJ1" s="120"/>
+      <c r="BK1" s="120"/>
+      <c r="BL1" s="120"/>
+      <c r="BM1" s="120"/>
+      <c r="BN1" s="120"/>
+      <c r="BO1" s="120"/>
+      <c r="BP1" s="120"/>
+      <c r="BQ1" s="120"/>
+      <c r="BR1" s="120"/>
+      <c r="BS1" s="120"/>
+      <c r="BT1" s="120"/>
+      <c r="BU1" s="120"/>
+      <c r="BV1" s="120"/>
+      <c r="BW1" s="120"/>
+      <c r="BX1" s="120"/>
+      <c r="BY1" s="120"/>
+      <c r="BZ1" s="120"/>
+      <c r="CA1" s="120"/>
+      <c r="CB1" s="120"/>
+      <c r="CC1" s="120"/>
+      <c r="CD1" s="120"/>
+      <c r="CE1" s="120"/>
+      <c r="CF1" s="120"/>
+      <c r="CG1" s="120"/>
+      <c r="CH1" s="120"/>
+      <c r="CI1" s="120"/>
+      <c r="CJ1" s="120"/>
+      <c r="CK1" s="120"/>
+      <c r="CL1" s="120"/>
+      <c r="CM1" s="120"/>
+      <c r="CN1" s="120"/>
+      <c r="CO1" s="120"/>
+      <c r="CP1" s="120"/>
+      <c r="CQ1" s="120"/>
+      <c r="CR1" s="120"/>
+      <c r="CS1" s="120"/>
+      <c r="CT1" s="120"/>
+      <c r="CU1" s="120"/>
+      <c r="CV1" s="120"/>
+      <c r="CW1" s="120"/>
+      <c r="CX1" s="120"/>
+      <c r="CY1" s="120"/>
+      <c r="CZ1" s="120"/>
+      <c r="DA1" s="120"/>
+      <c r="DB1" s="120"/>
+      <c r="DC1" s="120"/>
+      <c r="DD1" s="120"/>
+      <c r="DE1" s="120"/>
+      <c r="DF1" s="120"/>
+      <c r="DG1" s="120"/>
+      <c r="DH1" s="120"/>
+      <c r="DI1" s="120"/>
+      <c r="DJ1" s="120"/>
+      <c r="DK1" s="120"/>
+      <c r="DL1" s="120"/>
+      <c r="DM1" s="120"/>
+      <c r="DN1" s="120"/>
+      <c r="DO1" s="120"/>
+      <c r="DP1" s="120"/>
+      <c r="DQ1" s="120"/>
+      <c r="DR1" s="120"/>
+      <c r="DS1" s="120"/>
+      <c r="DT1" s="120"/>
+      <c r="DU1" s="120"/>
+      <c r="DV1" s="120"/>
+      <c r="DW1" s="120"/>
+      <c r="DX1" s="120"/>
+      <c r="DY1" s="120"/>
+      <c r="DZ1" s="120"/>
+      <c r="EA1" s="120"/>
+      <c r="EB1" s="120"/>
+      <c r="EC1" s="120"/>
+      <c r="ED1" s="120"/>
+      <c r="EE1" s="120"/>
+      <c r="EF1" s="120"/>
+      <c r="EG1" s="120"/>
+      <c r="EH1" s="120"/>
+      <c r="EI1" s="120"/>
+      <c r="EJ1" s="120"/>
+      <c r="EK1" s="120"/>
+      <c r="EL1" s="120"/>
+      <c r="EM1" s="120"/>
+      <c r="EN1" s="120"/>
+      <c r="EO1" s="120"/>
+      <c r="EP1" s="120"/>
+      <c r="EQ1" s="120"/>
+      <c r="ER1" s="120"/>
+      <c r="ES1" s="120"/>
+      <c r="ET1" s="120"/>
+      <c r="EU1" s="120"/>
+      <c r="EV1" s="120"/>
+      <c r="EW1" s="120"/>
+      <c r="EX1" s="120"/>
+      <c r="EY1" s="120"/>
+      <c r="EZ1" s="120"/>
+      <c r="FA1" s="120"/>
+      <c r="FB1" s="120"/>
+      <c r="FC1" s="120"/>
+      <c r="FD1" s="120"/>
+      <c r="FE1" s="120"/>
+      <c r="FF1" s="120"/>
+      <c r="FG1" s="120"/>
+      <c r="FH1" s="120"/>
+      <c r="FI1" s="120"/>
+      <c r="FJ1" s="120"/>
+      <c r="FK1" s="120"/>
+      <c r="FL1" s="120"/>
+      <c r="FM1" s="120"/>
+      <c r="FN1" s="120"/>
+      <c r="FO1" s="120"/>
+      <c r="FP1" s="120"/>
+      <c r="FQ1" s="120"/>
+      <c r="FR1" s="120"/>
+      <c r="FS1" s="120"/>
+      <c r="FT1" s="120"/>
+      <c r="FU1" s="120"/>
+      <c r="FV1" s="120"/>
+      <c r="FW1" s="120"/>
+      <c r="FX1" s="120"/>
+      <c r="FY1" s="120"/>
+      <c r="FZ1" s="120"/>
+      <c r="GA1" s="120"/>
+      <c r="GB1" s="120"/>
+      <c r="GC1" s="120"/>
+      <c r="GD1" s="120"/>
+      <c r="GE1" s="120"/>
+      <c r="GF1" s="120"/>
+      <c r="GG1" s="120"/>
+      <c r="GH1" s="120"/>
+      <c r="GI1" s="120"/>
+      <c r="GJ1" s="120"/>
+      <c r="GK1" s="120"/>
+      <c r="GL1" s="120"/>
+      <c r="GM1" s="120"/>
+      <c r="GN1" s="120"/>
+      <c r="GO1" s="120"/>
+      <c r="GP1" s="120"/>
+      <c r="GQ1" s="120"/>
+      <c r="GR1" s="120"/>
+      <c r="GS1" s="120"/>
+      <c r="GT1" s="120"/>
+      <c r="GU1" s="120"/>
+      <c r="GV1" s="120"/>
+      <c r="GW1" s="120"/>
+      <c r="GX1" s="120"/>
+      <c r="GY1" s="120"/>
+      <c r="GZ1" s="120"/>
+      <c r="HA1" s="120"/>
+      <c r="HB1" s="120"/>
+      <c r="HC1" s="120"/>
+      <c r="HD1" s="120"/>
+      <c r="HE1" s="120"/>
+      <c r="HF1" s="120"/>
+      <c r="HG1" s="120"/>
+      <c r="HH1" s="120"/>
+      <c r="HI1" s="120"/>
+      <c r="HJ1" s="120"/>
+      <c r="HK1" s="120"/>
+      <c r="HL1" s="120"/>
+      <c r="HM1" s="120"/>
+      <c r="HN1" s="120"/>
+      <c r="HO1" s="120"/>
+      <c r="HP1" s="120"/>
+      <c r="HQ1" s="120"/>
+      <c r="HR1" s="120"/>
+      <c r="HS1" s="120"/>
+      <c r="HT1" s="120"/>
+      <c r="HU1" s="120"/>
+      <c r="HV1" s="120"/>
+      <c r="HW1" s="120"/>
+      <c r="HX1" s="120"/>
+      <c r="HY1" s="120"/>
+      <c r="HZ1" s="120"/>
+      <c r="IA1" s="120"/>
+      <c r="IB1" s="120"/>
+      <c r="IC1" s="120"/>
+      <c r="ID1" s="120"/>
+      <c r="IE1" s="120"/>
+      <c r="IF1" s="120"/>
+      <c r="IG1" s="120"/>
+      <c r="IH1" s="120"/>
+      <c r="II1" s="120"/>
+      <c r="IJ1" s="120"/>
+      <c r="IK1" s="120"/>
+      <c r="IL1" s="120"/>
+      <c r="IM1" s="120"/>
+      <c r="IN1" s="120"/>
+      <c r="IO1" s="120"/>
+      <c r="IP1" s="120"/>
+      <c r="IQ1" s="120"/>
+      <c r="IR1" s="120"/>
+      <c r="IS1" s="120"/>
+      <c r="IT1" s="120"/>
+      <c r="IU1" s="121"/>
     </row>
     <row r="2" spans="1:255" ht="28" x14ac:dyDescent="0.15">
-      <c r="A2" s="124"/>
-      <c r="B2" s="124"/>
-      <c r="C2" s="125" t="s">
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="125" t="s">
+      <c r="D2" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="125" t="s">
+      <c r="E2" s="124" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="126" t="s">
+      <c r="F2" s="125" t="s">
         <v>187</v>
       </c>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="127"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="128"/>
-      <c r="R2" s="128"/>
-      <c r="S2" s="128"/>
-      <c r="T2" s="128"/>
-      <c r="U2" s="128"/>
-      <c r="V2" s="128"/>
-      <c r="W2" s="128"/>
-      <c r="X2" s="128"/>
-      <c r="Y2" s="128"/>
-      <c r="Z2" s="128"/>
-      <c r="AA2" s="128"/>
-      <c r="AB2" s="128"/>
-      <c r="AC2" s="128"/>
-      <c r="AD2" s="128"/>
-      <c r="AE2" s="128"/>
-      <c r="AF2" s="128"/>
-      <c r="AG2" s="128"/>
-      <c r="AH2" s="128"/>
-      <c r="AI2" s="128"/>
-      <c r="AJ2" s="128"/>
-      <c r="AK2" s="128"/>
-      <c r="AL2" s="128"/>
-      <c r="AM2" s="128"/>
-      <c r="AN2" s="128"/>
-      <c r="AO2" s="128"/>
-      <c r="AP2" s="128"/>
-      <c r="AQ2" s="128"/>
-      <c r="AR2" s="128"/>
-      <c r="AS2" s="128"/>
-      <c r="AT2" s="128"/>
-      <c r="AU2" s="128"/>
-      <c r="AV2" s="128"/>
-      <c r="AW2" s="128"/>
-      <c r="AX2" s="128"/>
-      <c r="AY2" s="128"/>
-      <c r="AZ2" s="128"/>
-      <c r="BA2" s="128"/>
-      <c r="BB2" s="128"/>
-      <c r="BC2" s="128"/>
-      <c r="BD2" s="128"/>
-      <c r="BE2" s="128"/>
-      <c r="BF2" s="128"/>
-      <c r="BG2" s="128"/>
-      <c r="BH2" s="128"/>
-      <c r="BI2" s="128"/>
-      <c r="BJ2" s="128"/>
-      <c r="BK2" s="128"/>
-      <c r="BL2" s="128"/>
-      <c r="BM2" s="128"/>
-      <c r="BN2" s="128"/>
-      <c r="BO2" s="128"/>
-      <c r="BP2" s="128"/>
-      <c r="BQ2" s="128"/>
-      <c r="BR2" s="128"/>
-      <c r="BS2" s="128"/>
-      <c r="BT2" s="128"/>
-      <c r="BU2" s="128"/>
-      <c r="BV2" s="128"/>
-      <c r="BW2" s="128"/>
-      <c r="BX2" s="128"/>
-      <c r="BY2" s="128"/>
-      <c r="BZ2" s="128"/>
-      <c r="CA2" s="128"/>
-      <c r="CB2" s="128"/>
-      <c r="CC2" s="128"/>
-      <c r="CD2" s="128"/>
-      <c r="CE2" s="128"/>
-      <c r="CF2" s="128"/>
-      <c r="CG2" s="128"/>
-      <c r="CH2" s="128"/>
-      <c r="CI2" s="128"/>
-      <c r="CJ2" s="128"/>
-      <c r="CK2" s="128"/>
-      <c r="CL2" s="128"/>
-      <c r="CM2" s="128"/>
-      <c r="CN2" s="128"/>
-      <c r="CO2" s="128"/>
-      <c r="CP2" s="128"/>
-      <c r="CQ2" s="128"/>
-      <c r="CR2" s="128"/>
-      <c r="CS2" s="128"/>
-      <c r="CT2" s="128"/>
-      <c r="CU2" s="128"/>
-      <c r="CV2" s="128"/>
-      <c r="CW2" s="128"/>
-      <c r="CX2" s="128"/>
-      <c r="CY2" s="128"/>
-      <c r="CZ2" s="128"/>
-      <c r="DA2" s="128"/>
-      <c r="DB2" s="128"/>
-      <c r="DC2" s="128"/>
-      <c r="DD2" s="128"/>
-      <c r="DE2" s="128"/>
-      <c r="DF2" s="128"/>
-      <c r="DG2" s="128"/>
-      <c r="DH2" s="128"/>
-      <c r="DI2" s="128"/>
-      <c r="DJ2" s="128"/>
-      <c r="DK2" s="128"/>
-      <c r="DL2" s="128"/>
-      <c r="DM2" s="128"/>
-      <c r="DN2" s="128"/>
-      <c r="DO2" s="128"/>
-      <c r="DP2" s="128"/>
-      <c r="DQ2" s="128"/>
-      <c r="DR2" s="128"/>
-      <c r="DS2" s="128"/>
-      <c r="DT2" s="128"/>
-      <c r="DU2" s="128"/>
-      <c r="DV2" s="128"/>
-      <c r="DW2" s="128"/>
-      <c r="DX2" s="128"/>
-      <c r="DY2" s="128"/>
-      <c r="DZ2" s="128"/>
-      <c r="EA2" s="128"/>
-      <c r="EB2" s="128"/>
-      <c r="EC2" s="128"/>
-      <c r="ED2" s="128"/>
-      <c r="EE2" s="128"/>
-      <c r="EF2" s="128"/>
-      <c r="EG2" s="128"/>
-      <c r="EH2" s="128"/>
-      <c r="EI2" s="128"/>
-      <c r="EJ2" s="128"/>
-      <c r="EK2" s="128"/>
-      <c r="EL2" s="128"/>
-      <c r="EM2" s="128"/>
-      <c r="EN2" s="128"/>
-      <c r="EO2" s="128"/>
-      <c r="EP2" s="128"/>
-      <c r="EQ2" s="128"/>
-      <c r="ER2" s="128"/>
-      <c r="ES2" s="128"/>
-      <c r="ET2" s="128"/>
-      <c r="EU2" s="128"/>
-      <c r="EV2" s="128"/>
-      <c r="EW2" s="128"/>
-      <c r="EX2" s="128"/>
-      <c r="EY2" s="128"/>
-      <c r="EZ2" s="128"/>
-      <c r="FA2" s="128"/>
-      <c r="FB2" s="128"/>
-      <c r="FC2" s="128"/>
-      <c r="FD2" s="128"/>
-      <c r="FE2" s="128"/>
-      <c r="FF2" s="128"/>
-      <c r="FG2" s="128"/>
-      <c r="FH2" s="128"/>
-      <c r="FI2" s="128"/>
-      <c r="FJ2" s="128"/>
-      <c r="FK2" s="128"/>
-      <c r="FL2" s="128"/>
-      <c r="FM2" s="128"/>
-      <c r="FN2" s="128"/>
-      <c r="FO2" s="128"/>
-      <c r="FP2" s="128"/>
-      <c r="FQ2" s="128"/>
-      <c r="FR2" s="128"/>
-      <c r="FS2" s="128"/>
-      <c r="FT2" s="128"/>
-      <c r="FU2" s="128"/>
-      <c r="FV2" s="128"/>
-      <c r="FW2" s="128"/>
-      <c r="FX2" s="128"/>
-      <c r="FY2" s="128"/>
-      <c r="FZ2" s="128"/>
-      <c r="GA2" s="128"/>
-      <c r="GB2" s="128"/>
-      <c r="GC2" s="128"/>
-      <c r="GD2" s="128"/>
-      <c r="GE2" s="128"/>
-      <c r="GF2" s="128"/>
-      <c r="GG2" s="128"/>
-      <c r="GH2" s="128"/>
-      <c r="GI2" s="128"/>
-      <c r="GJ2" s="128"/>
-      <c r="GK2" s="128"/>
-      <c r="GL2" s="128"/>
-      <c r="GM2" s="128"/>
-      <c r="GN2" s="128"/>
-      <c r="GO2" s="128"/>
-      <c r="GP2" s="128"/>
-      <c r="GQ2" s="128"/>
-      <c r="GR2" s="128"/>
-      <c r="GS2" s="128"/>
-      <c r="GT2" s="128"/>
-      <c r="GU2" s="128"/>
-      <c r="GV2" s="128"/>
-      <c r="GW2" s="128"/>
-      <c r="GX2" s="128"/>
-      <c r="GY2" s="128"/>
-      <c r="GZ2" s="128"/>
-      <c r="HA2" s="128"/>
-      <c r="HB2" s="128"/>
-      <c r="HC2" s="128"/>
-      <c r="HD2" s="128"/>
-      <c r="HE2" s="128"/>
-      <c r="HF2" s="128"/>
-      <c r="HG2" s="128"/>
-      <c r="HH2" s="128"/>
-      <c r="HI2" s="128"/>
-      <c r="HJ2" s="128"/>
-      <c r="HK2" s="128"/>
-      <c r="HL2" s="128"/>
-      <c r="HM2" s="128"/>
-      <c r="HN2" s="128"/>
-      <c r="HO2" s="128"/>
-      <c r="HP2" s="128"/>
-      <c r="HQ2" s="128"/>
-      <c r="HR2" s="128"/>
-      <c r="HS2" s="128"/>
-      <c r="HT2" s="128"/>
-      <c r="HU2" s="128"/>
-      <c r="HV2" s="128"/>
-      <c r="HW2" s="128"/>
-      <c r="HX2" s="128"/>
-      <c r="HY2" s="128"/>
-      <c r="HZ2" s="128"/>
-      <c r="IA2" s="128"/>
-      <c r="IB2" s="128"/>
-      <c r="IC2" s="128"/>
-      <c r="ID2" s="128"/>
-      <c r="IE2" s="128"/>
-      <c r="IF2" s="128"/>
-      <c r="IG2" s="128"/>
-      <c r="IH2" s="128"/>
-      <c r="II2" s="128"/>
-      <c r="IJ2" s="128"/>
-      <c r="IK2" s="128"/>
-      <c r="IL2" s="128"/>
-      <c r="IM2" s="128"/>
-      <c r="IN2" s="128"/>
-      <c r="IO2" s="128"/>
-      <c r="IP2" s="128"/>
-      <c r="IQ2" s="128"/>
-      <c r="IR2" s="128"/>
-      <c r="IS2" s="128"/>
-      <c r="IT2" s="128"/>
-      <c r="IU2" s="129"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="127"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="127"/>
+      <c r="S2" s="127"/>
+      <c r="T2" s="127"/>
+      <c r="U2" s="127"/>
+      <c r="V2" s="127"/>
+      <c r="W2" s="127"/>
+      <c r="X2" s="127"/>
+      <c r="Y2" s="127"/>
+      <c r="Z2" s="127"/>
+      <c r="AA2" s="127"/>
+      <c r="AB2" s="127"/>
+      <c r="AC2" s="127"/>
+      <c r="AD2" s="127"/>
+      <c r="AE2" s="127"/>
+      <c r="AF2" s="127"/>
+      <c r="AG2" s="127"/>
+      <c r="AH2" s="127"/>
+      <c r="AI2" s="127"/>
+      <c r="AJ2" s="127"/>
+      <c r="AK2" s="127"/>
+      <c r="AL2" s="127"/>
+      <c r="AM2" s="127"/>
+      <c r="AN2" s="127"/>
+      <c r="AO2" s="127"/>
+      <c r="AP2" s="127"/>
+      <c r="AQ2" s="127"/>
+      <c r="AR2" s="127"/>
+      <c r="AS2" s="127"/>
+      <c r="AT2" s="127"/>
+      <c r="AU2" s="127"/>
+      <c r="AV2" s="127"/>
+      <c r="AW2" s="127"/>
+      <c r="AX2" s="127"/>
+      <c r="AY2" s="127"/>
+      <c r="AZ2" s="127"/>
+      <c r="BA2" s="127"/>
+      <c r="BB2" s="127"/>
+      <c r="BC2" s="127"/>
+      <c r="BD2" s="127"/>
+      <c r="BE2" s="127"/>
+      <c r="BF2" s="127"/>
+      <c r="BG2" s="127"/>
+      <c r="BH2" s="127"/>
+      <c r="BI2" s="127"/>
+      <c r="BJ2" s="127"/>
+      <c r="BK2" s="127"/>
+      <c r="BL2" s="127"/>
+      <c r="BM2" s="127"/>
+      <c r="BN2" s="127"/>
+      <c r="BO2" s="127"/>
+      <c r="BP2" s="127"/>
+      <c r="BQ2" s="127"/>
+      <c r="BR2" s="127"/>
+      <c r="BS2" s="127"/>
+      <c r="BT2" s="127"/>
+      <c r="BU2" s="127"/>
+      <c r="BV2" s="127"/>
+      <c r="BW2" s="127"/>
+      <c r="BX2" s="127"/>
+      <c r="BY2" s="127"/>
+      <c r="BZ2" s="127"/>
+      <c r="CA2" s="127"/>
+      <c r="CB2" s="127"/>
+      <c r="CC2" s="127"/>
+      <c r="CD2" s="127"/>
+      <c r="CE2" s="127"/>
+      <c r="CF2" s="127"/>
+      <c r="CG2" s="127"/>
+      <c r="CH2" s="127"/>
+      <c r="CI2" s="127"/>
+      <c r="CJ2" s="127"/>
+      <c r="CK2" s="127"/>
+      <c r="CL2" s="127"/>
+      <c r="CM2" s="127"/>
+      <c r="CN2" s="127"/>
+      <c r="CO2" s="127"/>
+      <c r="CP2" s="127"/>
+      <c r="CQ2" s="127"/>
+      <c r="CR2" s="127"/>
+      <c r="CS2" s="127"/>
+      <c r="CT2" s="127"/>
+      <c r="CU2" s="127"/>
+      <c r="CV2" s="127"/>
+      <c r="CW2" s="127"/>
+      <c r="CX2" s="127"/>
+      <c r="CY2" s="127"/>
+      <c r="CZ2" s="127"/>
+      <c r="DA2" s="127"/>
+      <c r="DB2" s="127"/>
+      <c r="DC2" s="127"/>
+      <c r="DD2" s="127"/>
+      <c r="DE2" s="127"/>
+      <c r="DF2" s="127"/>
+      <c r="DG2" s="127"/>
+      <c r="DH2" s="127"/>
+      <c r="DI2" s="127"/>
+      <c r="DJ2" s="127"/>
+      <c r="DK2" s="127"/>
+      <c r="DL2" s="127"/>
+      <c r="DM2" s="127"/>
+      <c r="DN2" s="127"/>
+      <c r="DO2" s="127"/>
+      <c r="DP2" s="127"/>
+      <c r="DQ2" s="127"/>
+      <c r="DR2" s="127"/>
+      <c r="DS2" s="127"/>
+      <c r="DT2" s="127"/>
+      <c r="DU2" s="127"/>
+      <c r="DV2" s="127"/>
+      <c r="DW2" s="127"/>
+      <c r="DX2" s="127"/>
+      <c r="DY2" s="127"/>
+      <c r="DZ2" s="127"/>
+      <c r="EA2" s="127"/>
+      <c r="EB2" s="127"/>
+      <c r="EC2" s="127"/>
+      <c r="ED2" s="127"/>
+      <c r="EE2" s="127"/>
+      <c r="EF2" s="127"/>
+      <c r="EG2" s="127"/>
+      <c r="EH2" s="127"/>
+      <c r="EI2" s="127"/>
+      <c r="EJ2" s="127"/>
+      <c r="EK2" s="127"/>
+      <c r="EL2" s="127"/>
+      <c r="EM2" s="127"/>
+      <c r="EN2" s="127"/>
+      <c r="EO2" s="127"/>
+      <c r="EP2" s="127"/>
+      <c r="EQ2" s="127"/>
+      <c r="ER2" s="127"/>
+      <c r="ES2" s="127"/>
+      <c r="ET2" s="127"/>
+      <c r="EU2" s="127"/>
+      <c r="EV2" s="127"/>
+      <c r="EW2" s="127"/>
+      <c r="EX2" s="127"/>
+      <c r="EY2" s="127"/>
+      <c r="EZ2" s="127"/>
+      <c r="FA2" s="127"/>
+      <c r="FB2" s="127"/>
+      <c r="FC2" s="127"/>
+      <c r="FD2" s="127"/>
+      <c r="FE2" s="127"/>
+      <c r="FF2" s="127"/>
+      <c r="FG2" s="127"/>
+      <c r="FH2" s="127"/>
+      <c r="FI2" s="127"/>
+      <c r="FJ2" s="127"/>
+      <c r="FK2" s="127"/>
+      <c r="FL2" s="127"/>
+      <c r="FM2" s="127"/>
+      <c r="FN2" s="127"/>
+      <c r="FO2" s="127"/>
+      <c r="FP2" s="127"/>
+      <c r="FQ2" s="127"/>
+      <c r="FR2" s="127"/>
+      <c r="FS2" s="127"/>
+      <c r="FT2" s="127"/>
+      <c r="FU2" s="127"/>
+      <c r="FV2" s="127"/>
+      <c r="FW2" s="127"/>
+      <c r="FX2" s="127"/>
+      <c r="FY2" s="127"/>
+      <c r="FZ2" s="127"/>
+      <c r="GA2" s="127"/>
+      <c r="GB2" s="127"/>
+      <c r="GC2" s="127"/>
+      <c r="GD2" s="127"/>
+      <c r="GE2" s="127"/>
+      <c r="GF2" s="127"/>
+      <c r="GG2" s="127"/>
+      <c r="GH2" s="127"/>
+      <c r="GI2" s="127"/>
+      <c r="GJ2" s="127"/>
+      <c r="GK2" s="127"/>
+      <c r="GL2" s="127"/>
+      <c r="GM2" s="127"/>
+      <c r="GN2" s="127"/>
+      <c r="GO2" s="127"/>
+      <c r="GP2" s="127"/>
+      <c r="GQ2" s="127"/>
+      <c r="GR2" s="127"/>
+      <c r="GS2" s="127"/>
+      <c r="GT2" s="127"/>
+      <c r="GU2" s="127"/>
+      <c r="GV2" s="127"/>
+      <c r="GW2" s="127"/>
+      <c r="GX2" s="127"/>
+      <c r="GY2" s="127"/>
+      <c r="GZ2" s="127"/>
+      <c r="HA2" s="127"/>
+      <c r="HB2" s="127"/>
+      <c r="HC2" s="127"/>
+      <c r="HD2" s="127"/>
+      <c r="HE2" s="127"/>
+      <c r="HF2" s="127"/>
+      <c r="HG2" s="127"/>
+      <c r="HH2" s="127"/>
+      <c r="HI2" s="127"/>
+      <c r="HJ2" s="127"/>
+      <c r="HK2" s="127"/>
+      <c r="HL2" s="127"/>
+      <c r="HM2" s="127"/>
+      <c r="HN2" s="127"/>
+      <c r="HO2" s="127"/>
+      <c r="HP2" s="127"/>
+      <c r="HQ2" s="127"/>
+      <c r="HR2" s="127"/>
+      <c r="HS2" s="127"/>
+      <c r="HT2" s="127"/>
+      <c r="HU2" s="127"/>
+      <c r="HV2" s="127"/>
+      <c r="HW2" s="127"/>
+      <c r="HX2" s="127"/>
+      <c r="HY2" s="127"/>
+      <c r="HZ2" s="127"/>
+      <c r="IA2" s="127"/>
+      <c r="IB2" s="127"/>
+      <c r="IC2" s="127"/>
+      <c r="ID2" s="127"/>
+      <c r="IE2" s="127"/>
+      <c r="IF2" s="127"/>
+      <c r="IG2" s="127"/>
+      <c r="IH2" s="127"/>
+      <c r="II2" s="127"/>
+      <c r="IJ2" s="127"/>
+      <c r="IK2" s="127"/>
+      <c r="IL2" s="127"/>
+      <c r="IM2" s="127"/>
+      <c r="IN2" s="127"/>
+      <c r="IO2" s="127"/>
+      <c r="IP2" s="127"/>
+      <c r="IQ2" s="127"/>
+      <c r="IR2" s="127"/>
+      <c r="IS2" s="127"/>
+      <c r="IT2" s="127"/>
+      <c r="IU2" s="128"/>
     </row>
     <row r="3" spans="1:255" x14ac:dyDescent="0.15">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="131" t="s">
+      <c r="C3" s="130" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="131" t="s">
+      <c r="D3" s="130" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="131" t="s">
+      <c r="E3" s="130" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="132" t="s">
+      <c r="F3" s="131" t="s">
         <v>189</v>
       </c>
-      <c r="G3" s="133"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135"/>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="135"/>
-      <c r="X3" s="135"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="135"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="135"/>
-      <c r="AC3" s="135"/>
-      <c r="AD3" s="135"/>
-      <c r="AE3" s="135"/>
-      <c r="AF3" s="135"/>
-      <c r="AG3" s="135"/>
-      <c r="AH3" s="135"/>
-      <c r="AI3" s="135"/>
-      <c r="AJ3" s="135"/>
-      <c r="AK3" s="135"/>
-      <c r="AL3" s="135"/>
-      <c r="AM3" s="135"/>
-      <c r="AN3" s="135"/>
-      <c r="AO3" s="135"/>
-      <c r="AP3" s="135"/>
-      <c r="AQ3" s="135"/>
-      <c r="AR3" s="135"/>
-      <c r="AS3" s="135"/>
-      <c r="AT3" s="135"/>
-      <c r="AU3" s="135"/>
-      <c r="AV3" s="135"/>
-      <c r="AW3" s="135"/>
-      <c r="AX3" s="135"/>
-      <c r="AY3" s="135"/>
-      <c r="AZ3" s="135"/>
-      <c r="BA3" s="135"/>
-      <c r="BB3" s="135"/>
-      <c r="BC3" s="135"/>
-      <c r="BD3" s="135"/>
-      <c r="BE3" s="135"/>
-      <c r="BF3" s="135"/>
-      <c r="BG3" s="135"/>
-      <c r="BH3" s="135"/>
-      <c r="BI3" s="135"/>
-      <c r="BJ3" s="135"/>
-      <c r="BK3" s="135"/>
-      <c r="BL3" s="135"/>
-      <c r="BM3" s="135"/>
-      <c r="BN3" s="135"/>
-      <c r="BO3" s="135"/>
-      <c r="BP3" s="135"/>
-      <c r="BQ3" s="135"/>
-      <c r="BR3" s="135"/>
-      <c r="BS3" s="135"/>
-      <c r="BT3" s="135"/>
-      <c r="BU3" s="135"/>
-      <c r="BV3" s="135"/>
-      <c r="BW3" s="135"/>
-      <c r="BX3" s="135"/>
-      <c r="BY3" s="135"/>
-      <c r="BZ3" s="135"/>
-      <c r="CA3" s="135"/>
-      <c r="CB3" s="135"/>
-      <c r="CC3" s="135"/>
-      <c r="CD3" s="135"/>
-      <c r="CE3" s="135"/>
-      <c r="CF3" s="135"/>
-      <c r="CG3" s="135"/>
-      <c r="CH3" s="135"/>
-      <c r="CI3" s="135"/>
-      <c r="CJ3" s="135"/>
-      <c r="CK3" s="135"/>
-      <c r="CL3" s="135"/>
-      <c r="CM3" s="135"/>
-      <c r="CN3" s="135"/>
-      <c r="CO3" s="135"/>
-      <c r="CP3" s="135"/>
-      <c r="CQ3" s="135"/>
-      <c r="CR3" s="135"/>
-      <c r="CS3" s="135"/>
-      <c r="CT3" s="135"/>
-      <c r="CU3" s="135"/>
-      <c r="CV3" s="135"/>
-      <c r="CW3" s="135"/>
-      <c r="CX3" s="135"/>
-      <c r="CY3" s="135"/>
-      <c r="CZ3" s="135"/>
-      <c r="DA3" s="135"/>
-      <c r="DB3" s="135"/>
-      <c r="DC3" s="135"/>
-      <c r="DD3" s="135"/>
-      <c r="DE3" s="135"/>
-      <c r="DF3" s="135"/>
-      <c r="DG3" s="135"/>
-      <c r="DH3" s="135"/>
-      <c r="DI3" s="135"/>
-      <c r="DJ3" s="135"/>
-      <c r="DK3" s="135"/>
-      <c r="DL3" s="135"/>
-      <c r="DM3" s="135"/>
-      <c r="DN3" s="135"/>
-      <c r="DO3" s="135"/>
-      <c r="DP3" s="135"/>
-      <c r="DQ3" s="135"/>
-      <c r="DR3" s="135"/>
-      <c r="DS3" s="135"/>
-      <c r="DT3" s="135"/>
-      <c r="DU3" s="135"/>
-      <c r="DV3" s="135"/>
-      <c r="DW3" s="135"/>
-      <c r="DX3" s="135"/>
-      <c r="DY3" s="135"/>
-      <c r="DZ3" s="135"/>
-      <c r="EA3" s="135"/>
-      <c r="EB3" s="135"/>
-      <c r="EC3" s="135"/>
-      <c r="ED3" s="135"/>
-      <c r="EE3" s="135"/>
-      <c r="EF3" s="135"/>
-      <c r="EG3" s="135"/>
-      <c r="EH3" s="135"/>
-      <c r="EI3" s="135"/>
-      <c r="EJ3" s="135"/>
-      <c r="EK3" s="135"/>
-      <c r="EL3" s="135"/>
-      <c r="EM3" s="135"/>
-      <c r="EN3" s="135"/>
-      <c r="EO3" s="135"/>
-      <c r="EP3" s="135"/>
-      <c r="EQ3" s="135"/>
-      <c r="ER3" s="135"/>
-      <c r="ES3" s="135"/>
-      <c r="ET3" s="135"/>
-      <c r="EU3" s="135"/>
-      <c r="EV3" s="135"/>
-      <c r="EW3" s="135"/>
-      <c r="EX3" s="135"/>
-      <c r="EY3" s="135"/>
-      <c r="EZ3" s="135"/>
-      <c r="FA3" s="135"/>
-      <c r="FB3" s="135"/>
-      <c r="FC3" s="135"/>
-      <c r="FD3" s="135"/>
-      <c r="FE3" s="135"/>
-      <c r="FF3" s="135"/>
-      <c r="FG3" s="135"/>
-      <c r="FH3" s="135"/>
-      <c r="FI3" s="135"/>
-      <c r="FJ3" s="135"/>
-      <c r="FK3" s="135"/>
-      <c r="FL3" s="135"/>
-      <c r="FM3" s="135"/>
-      <c r="FN3" s="135"/>
-      <c r="FO3" s="135"/>
-      <c r="FP3" s="135"/>
-      <c r="FQ3" s="135"/>
-      <c r="FR3" s="135"/>
-      <c r="FS3" s="135"/>
-      <c r="FT3" s="135"/>
-      <c r="FU3" s="135"/>
-      <c r="FV3" s="135"/>
-      <c r="FW3" s="135"/>
-      <c r="FX3" s="135"/>
-      <c r="FY3" s="135"/>
-      <c r="FZ3" s="135"/>
-      <c r="GA3" s="135"/>
-      <c r="GB3" s="135"/>
-      <c r="GC3" s="135"/>
-      <c r="GD3" s="135"/>
-      <c r="GE3" s="135"/>
-      <c r="GF3" s="135"/>
-      <c r="GG3" s="135"/>
-      <c r="GH3" s="135"/>
-      <c r="GI3" s="135"/>
-      <c r="GJ3" s="135"/>
-      <c r="GK3" s="135"/>
-      <c r="GL3" s="135"/>
-      <c r="GM3" s="135"/>
-      <c r="GN3" s="135"/>
-      <c r="GO3" s="135"/>
-      <c r="GP3" s="135"/>
-      <c r="GQ3" s="135"/>
-      <c r="GR3" s="135"/>
-      <c r="GS3" s="135"/>
-      <c r="GT3" s="135"/>
-      <c r="GU3" s="135"/>
-      <c r="GV3" s="135"/>
-      <c r="GW3" s="135"/>
-      <c r="GX3" s="135"/>
-      <c r="GY3" s="135"/>
-      <c r="GZ3" s="135"/>
-      <c r="HA3" s="135"/>
-      <c r="HB3" s="135"/>
-      <c r="HC3" s="135"/>
-      <c r="HD3" s="135"/>
-      <c r="HE3" s="135"/>
-      <c r="HF3" s="135"/>
-      <c r="HG3" s="135"/>
-      <c r="HH3" s="135"/>
-      <c r="HI3" s="135"/>
-      <c r="HJ3" s="135"/>
-      <c r="HK3" s="135"/>
-      <c r="HL3" s="135"/>
-      <c r="HM3" s="135"/>
-      <c r="HN3" s="135"/>
-      <c r="HO3" s="135"/>
-      <c r="HP3" s="135"/>
-      <c r="HQ3" s="135"/>
-      <c r="HR3" s="135"/>
-      <c r="HS3" s="135"/>
-      <c r="HT3" s="135"/>
-      <c r="HU3" s="135"/>
-      <c r="HV3" s="135"/>
-      <c r="HW3" s="135"/>
-      <c r="HX3" s="135"/>
-      <c r="HY3" s="135"/>
-      <c r="HZ3" s="135"/>
-      <c r="IA3" s="135"/>
-      <c r="IB3" s="135"/>
-      <c r="IC3" s="135"/>
-      <c r="ID3" s="135"/>
-      <c r="IE3" s="135"/>
-      <c r="IF3" s="135"/>
-      <c r="IG3" s="135"/>
-      <c r="IH3" s="135"/>
-      <c r="II3" s="135"/>
-      <c r="IJ3" s="135"/>
-      <c r="IK3" s="135"/>
-      <c r="IL3" s="135"/>
-      <c r="IM3" s="135"/>
-      <c r="IN3" s="135"/>
-      <c r="IO3" s="135"/>
-      <c r="IP3" s="135"/>
-      <c r="IQ3" s="135"/>
-      <c r="IR3" s="135"/>
-      <c r="IS3" s="135"/>
-      <c r="IT3" s="135"/>
-      <c r="IU3" s="136"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="134"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="134"/>
+      <c r="T3" s="134"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="134"/>
+      <c r="X3" s="134"/>
+      <c r="Y3" s="134"/>
+      <c r="Z3" s="134"/>
+      <c r="AA3" s="134"/>
+      <c r="AB3" s="134"/>
+      <c r="AC3" s="134"/>
+      <c r="AD3" s="134"/>
+      <c r="AE3" s="134"/>
+      <c r="AF3" s="134"/>
+      <c r="AG3" s="134"/>
+      <c r="AH3" s="134"/>
+      <c r="AI3" s="134"/>
+      <c r="AJ3" s="134"/>
+      <c r="AK3" s="134"/>
+      <c r="AL3" s="134"/>
+      <c r="AM3" s="134"/>
+      <c r="AN3" s="134"/>
+      <c r="AO3" s="134"/>
+      <c r="AP3" s="134"/>
+      <c r="AQ3" s="134"/>
+      <c r="AR3" s="134"/>
+      <c r="AS3" s="134"/>
+      <c r="AT3" s="134"/>
+      <c r="AU3" s="134"/>
+      <c r="AV3" s="134"/>
+      <c r="AW3" s="134"/>
+      <c r="AX3" s="134"/>
+      <c r="AY3" s="134"/>
+      <c r="AZ3" s="134"/>
+      <c r="BA3" s="134"/>
+      <c r="BB3" s="134"/>
+      <c r="BC3" s="134"/>
+      <c r="BD3" s="134"/>
+      <c r="BE3" s="134"/>
+      <c r="BF3" s="134"/>
+      <c r="BG3" s="134"/>
+      <c r="BH3" s="134"/>
+      <c r="BI3" s="134"/>
+      <c r="BJ3" s="134"/>
+      <c r="BK3" s="134"/>
+      <c r="BL3" s="134"/>
+      <c r="BM3" s="134"/>
+      <c r="BN3" s="134"/>
+      <c r="BO3" s="134"/>
+      <c r="BP3" s="134"/>
+      <c r="BQ3" s="134"/>
+      <c r="BR3" s="134"/>
+      <c r="BS3" s="134"/>
+      <c r="BT3" s="134"/>
+      <c r="BU3" s="134"/>
+      <c r="BV3" s="134"/>
+      <c r="BW3" s="134"/>
+      <c r="BX3" s="134"/>
+      <c r="BY3" s="134"/>
+      <c r="BZ3" s="134"/>
+      <c r="CA3" s="134"/>
+      <c r="CB3" s="134"/>
+      <c r="CC3" s="134"/>
+      <c r="CD3" s="134"/>
+      <c r="CE3" s="134"/>
+      <c r="CF3" s="134"/>
+      <c r="CG3" s="134"/>
+      <c r="CH3" s="134"/>
+      <c r="CI3" s="134"/>
+      <c r="CJ3" s="134"/>
+      <c r="CK3" s="134"/>
+      <c r="CL3" s="134"/>
+      <c r="CM3" s="134"/>
+      <c r="CN3" s="134"/>
+      <c r="CO3" s="134"/>
+      <c r="CP3" s="134"/>
+      <c r="CQ3" s="134"/>
+      <c r="CR3" s="134"/>
+      <c r="CS3" s="134"/>
+      <c r="CT3" s="134"/>
+      <c r="CU3" s="134"/>
+      <c r="CV3" s="134"/>
+      <c r="CW3" s="134"/>
+      <c r="CX3" s="134"/>
+      <c r="CY3" s="134"/>
+      <c r="CZ3" s="134"/>
+      <c r="DA3" s="134"/>
+      <c r="DB3" s="134"/>
+      <c r="DC3" s="134"/>
+      <c r="DD3" s="134"/>
+      <c r="DE3" s="134"/>
+      <c r="DF3" s="134"/>
+      <c r="DG3" s="134"/>
+      <c r="DH3" s="134"/>
+      <c r="DI3" s="134"/>
+      <c r="DJ3" s="134"/>
+      <c r="DK3" s="134"/>
+      <c r="DL3" s="134"/>
+      <c r="DM3" s="134"/>
+      <c r="DN3" s="134"/>
+      <c r="DO3" s="134"/>
+      <c r="DP3" s="134"/>
+      <c r="DQ3" s="134"/>
+      <c r="DR3" s="134"/>
+      <c r="DS3" s="134"/>
+      <c r="DT3" s="134"/>
+      <c r="DU3" s="134"/>
+      <c r="DV3" s="134"/>
+      <c r="DW3" s="134"/>
+      <c r="DX3" s="134"/>
+      <c r="DY3" s="134"/>
+      <c r="DZ3" s="134"/>
+      <c r="EA3" s="134"/>
+      <c r="EB3" s="134"/>
+      <c r="EC3" s="134"/>
+      <c r="ED3" s="134"/>
+      <c r="EE3" s="134"/>
+      <c r="EF3" s="134"/>
+      <c r="EG3" s="134"/>
+      <c r="EH3" s="134"/>
+      <c r="EI3" s="134"/>
+      <c r="EJ3" s="134"/>
+      <c r="EK3" s="134"/>
+      <c r="EL3" s="134"/>
+      <c r="EM3" s="134"/>
+      <c r="EN3" s="134"/>
+      <c r="EO3" s="134"/>
+      <c r="EP3" s="134"/>
+      <c r="EQ3" s="134"/>
+      <c r="ER3" s="134"/>
+      <c r="ES3" s="134"/>
+      <c r="ET3" s="134"/>
+      <c r="EU3" s="134"/>
+      <c r="EV3" s="134"/>
+      <c r="EW3" s="134"/>
+      <c r="EX3" s="134"/>
+      <c r="EY3" s="134"/>
+      <c r="EZ3" s="134"/>
+      <c r="FA3" s="134"/>
+      <c r="FB3" s="134"/>
+      <c r="FC3" s="134"/>
+      <c r="FD3" s="134"/>
+      <c r="FE3" s="134"/>
+      <c r="FF3" s="134"/>
+      <c r="FG3" s="134"/>
+      <c r="FH3" s="134"/>
+      <c r="FI3" s="134"/>
+      <c r="FJ3" s="134"/>
+      <c r="FK3" s="134"/>
+      <c r="FL3" s="134"/>
+      <c r="FM3" s="134"/>
+      <c r="FN3" s="134"/>
+      <c r="FO3" s="134"/>
+      <c r="FP3" s="134"/>
+      <c r="FQ3" s="134"/>
+      <c r="FR3" s="134"/>
+      <c r="FS3" s="134"/>
+      <c r="FT3" s="134"/>
+      <c r="FU3" s="134"/>
+      <c r="FV3" s="134"/>
+      <c r="FW3" s="134"/>
+      <c r="FX3" s="134"/>
+      <c r="FY3" s="134"/>
+      <c r="FZ3" s="134"/>
+      <c r="GA3" s="134"/>
+      <c r="GB3" s="134"/>
+      <c r="GC3" s="134"/>
+      <c r="GD3" s="134"/>
+      <c r="GE3" s="134"/>
+      <c r="GF3" s="134"/>
+      <c r="GG3" s="134"/>
+      <c r="GH3" s="134"/>
+      <c r="GI3" s="134"/>
+      <c r="GJ3" s="134"/>
+      <c r="GK3" s="134"/>
+      <c r="GL3" s="134"/>
+      <c r="GM3" s="134"/>
+      <c r="GN3" s="134"/>
+      <c r="GO3" s="134"/>
+      <c r="GP3" s="134"/>
+      <c r="GQ3" s="134"/>
+      <c r="GR3" s="134"/>
+      <c r="GS3" s="134"/>
+      <c r="GT3" s="134"/>
+      <c r="GU3" s="134"/>
+      <c r="GV3" s="134"/>
+      <c r="GW3" s="134"/>
+      <c r="GX3" s="134"/>
+      <c r="GY3" s="134"/>
+      <c r="GZ3" s="134"/>
+      <c r="HA3" s="134"/>
+      <c r="HB3" s="134"/>
+      <c r="HC3" s="134"/>
+      <c r="HD3" s="134"/>
+      <c r="HE3" s="134"/>
+      <c r="HF3" s="134"/>
+      <c r="HG3" s="134"/>
+      <c r="HH3" s="134"/>
+      <c r="HI3" s="134"/>
+      <c r="HJ3" s="134"/>
+      <c r="HK3" s="134"/>
+      <c r="HL3" s="134"/>
+      <c r="HM3" s="134"/>
+      <c r="HN3" s="134"/>
+      <c r="HO3" s="134"/>
+      <c r="HP3" s="134"/>
+      <c r="HQ3" s="134"/>
+      <c r="HR3" s="134"/>
+      <c r="HS3" s="134"/>
+      <c r="HT3" s="134"/>
+      <c r="HU3" s="134"/>
+      <c r="HV3" s="134"/>
+      <c r="HW3" s="134"/>
+      <c r="HX3" s="134"/>
+      <c r="HY3" s="134"/>
+      <c r="HZ3" s="134"/>
+      <c r="IA3" s="134"/>
+      <c r="IB3" s="134"/>
+      <c r="IC3" s="134"/>
+      <c r="ID3" s="134"/>
+      <c r="IE3" s="134"/>
+      <c r="IF3" s="134"/>
+      <c r="IG3" s="134"/>
+      <c r="IH3" s="134"/>
+      <c r="II3" s="134"/>
+      <c r="IJ3" s="134"/>
+      <c r="IK3" s="134"/>
+      <c r="IL3" s="134"/>
+      <c r="IM3" s="134"/>
+      <c r="IN3" s="134"/>
+      <c r="IO3" s="134"/>
+      <c r="IP3" s="134"/>
+      <c r="IQ3" s="134"/>
+      <c r="IR3" s="134"/>
+      <c r="IS3" s="134"/>
+      <c r="IT3" s="134"/>
+      <c r="IU3" s="135"/>
     </row>
     <row r="4" spans="1:255" x14ac:dyDescent="0.15">
       <c r="A4" s="15">
@@ -8439,13 +8457,13 @@
       <c r="C4" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D4" s="137" t="s">
+      <c r="D4" s="136" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F4" s="138" t="s">
+      <c r="F4" s="137" t="s">
         <v>189</v>
       </c>
     </row>
@@ -8457,13 +8475,13 @@
       <c r="C5" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="139" t="s">
+      <c r="D5" s="138" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F5" s="140" t="s">
+      <c r="F5" s="139" t="s">
         <v>189</v>
       </c>
     </row>
@@ -8475,13 +8493,13 @@
       <c r="C6" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="141" t="s">
+      <c r="D6" s="140" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="F6" s="142" t="s">
+      <c r="F6" s="141" t="s">
         <v>189</v>
       </c>
     </row>
@@ -8655,7 +8673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="114" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -9566,7 +9584,7 @@
       <c r="E6" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="145" t="s">
+      <c r="F6" s="144" t="s">
         <v>215</v>
       </c>
       <c r="H6" s="5"/>
@@ -10508,8 +10526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10718,9 +10736,11 @@
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="49"/>
+      <c r="L4" s="146" t="s">
+        <v>232</v>
+      </c>
       <c r="M4" s="5"/>
-      <c r="N4" s="50"/>
+      <c r="N4" s="49"/>
       <c r="P4" s="5" t="s">
         <v>123</v>
       </c>
@@ -10733,7 +10753,7 @@
       <c r="C5" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="50" t="s">
         <v>124</v>
       </c>
       <c r="E5" t="s">
@@ -10753,9 +10773,11 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="L5" s="146" t="s">
+        <v>233</v>
+      </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="52"/>
+      <c r="N5" s="51"/>
       <c r="P5" s="28" t="s">
         <v>123</v>
       </c>
@@ -10774,7 +10796,7 @@
       <c r="C6" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="52" t="s">
         <v>127</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -10794,9 +10816,11 @@
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="L6" s="146" t="s">
+        <v>234</v>
+      </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="50"/>
+      <c r="N6" s="49"/>
       <c r="P6" s="28" t="s">
         <v>123</v>
       </c>
@@ -10815,7 +10839,7 @@
       <c r="C7" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>129</v>
       </c>
       <c r="E7" t="s">
@@ -10835,9 +10859,11 @@
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="49"/>
+      <c r="L7" s="146" t="s">
+        <v>235</v>
+      </c>
       <c r="M7" s="5"/>
-      <c r="N7" s="50"/>
+      <c r="N7" s="49"/>
       <c r="P7" s="5" t="s">
         <v>123</v>
       </c>
@@ -10856,7 +10882,7 @@
       <c r="C8" t="s">
         <v>196</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="54" t="s">
         <v>131</v>
       </c>
       <c r="E8" t="s">
@@ -10873,6 +10899,9 @@
       </c>
       <c r="I8" s="33" t="s">
         <v>100</v>
+      </c>
+      <c r="L8" s="146" t="s">
+        <v>236</v>
       </c>
       <c r="P8" s="28" t="s">
         <v>123</v>
@@ -10892,7 +10921,7 @@
       <c r="C9" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="143" t="s">
+      <c r="D9" s="142" t="s">
         <v>204</v>
       </c>
       <c r="E9" t="s">
@@ -10909,6 +10938,9 @@
       </c>
       <c r="I9" s="33" t="s">
         <v>206</v>
+      </c>
+      <c r="L9" s="146" t="s">
+        <v>237</v>
       </c>
       <c r="P9" s="28" t="s">
         <v>123</v>
@@ -10935,6 +10967,14 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="L5" r:id="rId1" xr:uid="{C7221064-E99C-094C-855F-47E0524F54FC}"/>
+    <hyperlink ref="L6" r:id="rId2" xr:uid="{8E412379-65C8-8D42-BE7F-B952DDEFDCA6}"/>
+    <hyperlink ref="L7" r:id="rId3" xr:uid="{C1E46905-10B1-C140-AD9D-0672E3035E5A}"/>
+    <hyperlink ref="L8" r:id="rId4" xr:uid="{85EDEC8F-221C-4745-A90B-76559B0FDD0A}"/>
+    <hyperlink ref="L9" r:id="rId5" xr:uid="{DA359530-14B7-5741-95FC-AEE4CE15367D}"/>
+    <hyperlink ref="L4" r:id="rId6" xr:uid="{D7246D58-03AF-0949-A436-B0DE9E8BE389}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
@@ -10949,7 +10989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -10995,7 +11035,7 @@
       <c r="K1"/>
       <c r="M1"/>
     </row>
-    <row r="2" spans="1:28" s="58" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" s="57" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39" t="s">
@@ -11007,7 +11047,7 @@
       <c r="E2" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="55" t="s">
         <v>137</v>
       </c>
       <c r="G2" s="39" t="s">
@@ -11016,13 +11056,13 @@
       <c r="H2" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="56" t="s">
         <v>140</v>
       </c>
       <c r="J2" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="56" t="s">
         <v>137</v>
       </c>
       <c r="L2" s="29" t="s">
@@ -11050,46 +11090,46 @@
       <c r="AB2" s="29"/>
     </row>
     <row r="3" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="61" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="61" t="s">
         <v>147</v>
       </c>
-      <c r="H3" s="62" t="s">
+      <c r="H3" s="61" t="s">
         <v>148</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="I3" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="K3" s="62" t="s">
+      <c r="K3" s="61" t="s">
         <v>151</v>
       </c>
-      <c r="L3" s="62" t="s">
+      <c r="L3" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="M3" s="64" t="s">
+      <c r="M3" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="64" t="s">
         <v>153</v>
       </c>
     </row>
@@ -11104,14 +11144,14 @@
       <c r="D4" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="48">
         <v>1</v>
       </c>
       <c r="G4"/>
-      <c r="H4" s="66" t="s">
+      <c r="H4" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I4" s="48">
@@ -11138,14 +11178,14 @@
       <c r="D5" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="53" t="s">
         <v>45</v>
       </c>
       <c r="F5" s="48">
         <v>2</v>
       </c>
       <c r="G5"/>
-      <c r="H5" s="66" t="s">
+      <c r="H5" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I5" s="48">
@@ -11173,14 +11213,14 @@
       <c r="D6" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="53" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="48">
         <v>3</v>
       </c>
       <c r="G6"/>
-      <c r="H6" s="66" t="s">
+      <c r="H6" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I6" s="48">
@@ -11250,7 +11290,7 @@
         <v>5</v>
       </c>
       <c r="G8"/>
-      <c r="H8" s="66" t="s">
+      <c r="H8" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I8" s="48">
@@ -11285,7 +11325,7 @@
         <v>6</v>
       </c>
       <c r="G9"/>
-      <c r="H9" s="66" t="s">
+      <c r="H9" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I9" s="48">
@@ -11320,7 +11360,7 @@
         <v>7</v>
       </c>
       <c r="G10"/>
-      <c r="H10" s="66" t="s">
+      <c r="H10" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I10" s="48">
@@ -11355,7 +11395,7 @@
         <v>8</v>
       </c>
       <c r="G11"/>
-      <c r="H11" s="66" t="s">
+      <c r="H11" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I11" s="48">
@@ -11390,7 +11430,7 @@
         <v>9</v>
       </c>
       <c r="G12"/>
-      <c r="H12" s="66" t="s">
+      <c r="H12" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I12" s="48">
@@ -11425,7 +11465,7 @@
         <v>10</v>
       </c>
       <c r="G13"/>
-      <c r="H13" s="66" t="s">
+      <c r="H13" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I13" s="48">
@@ -11460,7 +11500,7 @@
         <v>11</v>
       </c>
       <c r="G14"/>
-      <c r="H14" s="66" t="s">
+      <c r="H14" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I14" s="48">
@@ -11495,7 +11535,7 @@
         <v>12</v>
       </c>
       <c r="G15"/>
-      <c r="H15" s="66" t="s">
+      <c r="H15" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I15" s="48">
@@ -11523,14 +11563,14 @@
       <c r="D16" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="66" t="s">
         <v>208</v>
       </c>
       <c r="F16" s="48">
         <v>13</v>
       </c>
       <c r="G16"/>
-      <c r="H16" s="66" t="s">
+      <c r="H16" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I16" s="48">
@@ -11555,10 +11595,10 @@
       <c r="C17" t="s">
         <v>196</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="50" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="48">
@@ -11590,10 +11630,10 @@
       <c r="C18" t="s">
         <v>196</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="51" t="s">
+      <c r="E18" s="50" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="48">
@@ -11625,17 +11665,17 @@
       <c r="C19" t="s">
         <v>196</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="D19" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="68" t="s">
+      <c r="E19" s="67" t="s">
         <v>70</v>
       </c>
       <c r="F19" s="48">
         <v>3</v>
       </c>
       <c r="G19"/>
-      <c r="H19" s="66" t="s">
+      <c r="H19" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I19" s="48">
@@ -11660,17 +11700,17 @@
       <c r="C20" t="s">
         <v>196</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="67" t="s">
         <v>50</v>
       </c>
       <c r="F20" s="48">
         <v>4</v>
       </c>
       <c r="G20"/>
-      <c r="H20" s="66" t="s">
+      <c r="H20" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I20" s="48">
@@ -11695,17 +11735,17 @@
       <c r="C21" t="s">
         <v>196</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="D21" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="67" t="s">
         <v>208</v>
       </c>
       <c r="F21" s="48">
         <v>5</v>
       </c>
       <c r="G21"/>
-      <c r="H21" s="66" t="s">
+      <c r="H21" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I21" s="48">
@@ -11730,10 +11770,10 @@
       <c r="C22" t="s">
         <v>196</v>
       </c>
-      <c r="D22" s="53" t="s">
+      <c r="D22" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="E22" s="53" t="s">
+      <c r="E22" s="52" t="s">
         <v>47</v>
       </c>
       <c r="F22" s="48">
@@ -11765,10 +11805,10 @@
       <c r="C23" t="s">
         <v>196</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D23" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="E23" s="53" t="s">
+      <c r="E23" s="52" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="48">
@@ -11800,10 +11840,10 @@
       <c r="C24" t="s">
         <v>196</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="E24" s="69" t="s">
+      <c r="E24" s="68" t="s">
         <v>208</v>
       </c>
       <c r="F24" s="48">
@@ -11835,10 +11875,10 @@
       <c r="C25" t="s">
         <v>196</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="53" t="s">
         <v>47</v>
       </c>
       <c r="F25" s="48">
@@ -11869,10 +11909,10 @@
       <c r="C26" t="s">
         <v>196</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="53" t="s">
         <v>45</v>
       </c>
       <c r="F26" s="48">
@@ -11904,17 +11944,17 @@
       <c r="C27" t="s">
         <v>196</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="53" t="s">
         <v>70</v>
       </c>
       <c r="F27" s="48">
         <v>3</v>
       </c>
       <c r="G27"/>
-      <c r="H27" s="66" t="s">
+      <c r="H27" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I27" s="48">
@@ -11939,17 +11979,17 @@
       <c r="C28" t="s">
         <v>196</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="53" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="48">
         <v>4</v>
       </c>
       <c r="G28"/>
-      <c r="H28" s="66" t="s">
+      <c r="H28" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I28" s="48">
@@ -11974,17 +12014,17 @@
       <c r="C29" t="s">
         <v>196</v>
       </c>
-      <c r="D29" s="54" t="s">
+      <c r="D29" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="E29" s="67" t="s">
+      <c r="E29" s="66" t="s">
         <v>208</v>
       </c>
       <c r="F29" s="48">
         <v>5</v>
       </c>
       <c r="G29"/>
-      <c r="H29" s="66" t="s">
+      <c r="H29" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I29" s="48">
@@ -12009,10 +12049,10 @@
       <c r="C30" t="s">
         <v>196</v>
       </c>
-      <c r="D30" s="55" t="s">
+      <c r="D30" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="E30" s="70" t="s">
+      <c r="E30" s="69" t="s">
         <v>47</v>
       </c>
       <c r="F30" s="48">
@@ -12039,10 +12079,10 @@
       <c r="C31" t="s">
         <v>196</v>
       </c>
-      <c r="D31" s="55" t="s">
+      <c r="D31" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="70" t="s">
+      <c r="E31" s="69" t="s">
         <v>45</v>
       </c>
       <c r="F31" s="48">
@@ -12069,16 +12109,16 @@
       <c r="C32" t="s">
         <v>196</v>
       </c>
-      <c r="D32" s="55" t="s">
+      <c r="D32" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="E32" s="70" t="s">
+      <c r="E32" s="69" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="48">
         <v>3</v>
       </c>
-      <c r="H32" s="66" t="s">
+      <c r="H32" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I32" s="48">
@@ -12099,16 +12139,16 @@
       <c r="C33" t="s">
         <v>196</v>
       </c>
-      <c r="D33" s="55" t="s">
+      <c r="D33" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="E33" s="71" t="s">
+      <c r="E33" s="70" t="s">
         <v>208</v>
       </c>
       <c r="F33" s="48">
         <v>4</v>
       </c>
-      <c r="H33" s="66" t="s">
+      <c r="H33" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I33" s="48">
@@ -12129,16 +12169,16 @@
       <c r="C34" t="s">
         <v>196</v>
       </c>
-      <c r="D34" s="55" t="s">
+      <c r="D34" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="71" t="s">
+      <c r="E34" s="70" t="s">
         <v>75</v>
       </c>
       <c r="F34" s="48">
         <v>5</v>
       </c>
-      <c r="H34" s="66" t="s">
+      <c r="H34" s="65" t="s">
         <v>154</v>
       </c>
       <c r="I34" s="48">

</xml_diff>

<commit_message>
Update CCD definition with handleEvidence event and evidenceHandled field
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A75DB9-76DD-694D-B4EF-5DC0EB4B969A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3494EC-FC04-6742-929C-1241A2230642}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1340" windowWidth="25600" windowHeight="13040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="239">
   <si>
     <t>Change History</t>
   </si>
@@ -755,6 +755,27 @@
   </si>
   <si>
     <t>Set jurisdiction to BULKSCAN</t>
+  </si>
+  <si>
+    <t>evidenceHandled</t>
+  </si>
+  <si>
+    <t>Supplementary evidence handled</t>
+  </si>
+  <si>
+    <t>YesOrNo</t>
+  </si>
+  <si>
+    <t>handleEvidence</t>
+  </si>
+  <si>
+    <t>Handle supplementary evidence</t>
+  </si>
+  <si>
+    <t>MANDATORY</t>
+  </si>
+  <si>
+    <t>Added evidenceHandled field and handleEvidence event</t>
   </si>
 </sst>
 </file>
@@ -971,7 +992,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1038,8 +1059,14 @@
         <bgColor rgb="FFC2E0AE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFC2E0AE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1267,19 +1294,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1292,7 +1306,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1544,7 +1558,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1554,6 +1567,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -1944,10 +1960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2037,7 +2053,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="146">
+      <c r="A7" s="145">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -2054,7 +2070,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="146">
+      <c r="A8" s="145">
         <v>5</v>
       </c>
       <c r="B8" t="s">
@@ -2071,7 +2087,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="146">
+      <c r="A9" s="145">
         <v>6</v>
       </c>
       <c r="B9" t="s">
@@ -2088,7 +2104,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="146">
+      <c r="A10" s="145">
         <v>7</v>
       </c>
       <c r="B10" t="s">
@@ -2101,6 +2117,23 @@
         <v>43382</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="145">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6">
+        <v>43388</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>224</v>
       </c>
     </row>
@@ -2691,8 +2724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2925,10 +2958,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2937,7 +2970,7 @@
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="51.33203125" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="27" width="7.1640625" customWidth="1"/>
     <col min="28" max="1025" width="8.33203125" customWidth="1"/>
@@ -3176,13 +3209,31 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A8" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B5:B7" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B5:B8" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6398,10 +6449,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6410,7 +6461,7 @@
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
     <col min="8" max="27" width="7.1640625" customWidth="1"/>
@@ -6627,13 +6678,31 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A8" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0D00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0D00-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B5:B7" xr:uid="{00000000-0002-0000-0D00-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B5:B8" xr:uid="{00000000-0002-0000-0D00-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7024,10 +7093,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7374,9 +7443,27 @@
         <v>189</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="97">
+        <v>43101</v>
+      </c>
+      <c r="B19" s="98"/>
+      <c r="C19" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="99" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" s="92" t="s">
+        <v>202</v>
+      </c>
+      <c r="F19" s="100" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7393,10 +7480,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7585,7 +7672,7 @@
       <c r="C9" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="144" t="s">
+      <c r="D9" s="143" t="s">
         <v>204</v>
       </c>
       <c r="E9" s="92" t="s">
@@ -7595,9 +7682,27 @@
         <v>189</v>
       </c>
     </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A10" s="97">
+        <v>43101</v>
+      </c>
+      <c r="B10" s="110"/>
+      <c r="C10" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="147" t="s">
+        <v>235</v>
+      </c>
+      <c r="E10" s="92" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="100" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-1100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-1100-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8475,13 +8580,13 @@
       <c r="C6" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="141" t="s">
+      <c r="D6" s="148" t="s">
         <v>102</v>
       </c>
       <c r="E6" s="92" t="s">
         <v>202</v>
       </c>
-      <c r="F6" s="142" t="s">
+      <c r="F6" s="141" t="s">
         <v>189</v>
       </c>
     </row>
@@ -8827,7 +8932,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9310,16 +9415,38 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="J19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <autoFilter ref="A1:L18" xr:uid="{5CF36EC4-574A-F740-BEC7-9B222789F5DB}"/>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-0300-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B18" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B19" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9566,7 +9693,7 @@
       <c r="E6" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="145" t="s">
+      <c r="F6" s="144" t="s">
         <v>215</v>
       </c>
       <c r="H6" s="5"/>
@@ -10506,10 +10633,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AC9"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10517,7 +10644,7 @@
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="30.5" customWidth="1"/>
     <col min="6" max="6" width="38.1640625" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
@@ -10892,7 +11019,7 @@
       <c r="C9" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="143" t="s">
+      <c r="D9" s="142" t="s">
         <v>204</v>
       </c>
       <c r="E9" t="s">
@@ -10920,17 +11047,53 @@
         <v>126</v>
       </c>
     </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
+      <c r="A10" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="146" t="s">
+        <v>235</v>
+      </c>
+      <c r="E10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G10" s="48">
+        <v>7</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G10" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10947,10 +11110,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB34"/>
+  <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12151,9 +12314,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A35" s="15">
+        <v>43466</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" t="s">
+        <v>196</v>
+      </c>
+      <c r="D35" t="s">
+        <v>235</v>
+      </c>
+      <c r="E35" s="70" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="48">
+        <v>1</v>
+      </c>
+      <c r="H35" s="66" t="s">
+        <v>237</v>
+      </c>
+      <c r="I35" s="48">
+        <v>1</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K35" s="48">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A34" xr:uid="{00000000-0002-0000-0800-000000000000}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A35" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Updated ccd definition to change scannedDate type to DateTime
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3494EC-FC04-6742-929C-1241A2230642}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE3DBAA-0D5B-C04B-AF00-BD046493BA38}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="241">
   <si>
     <t>Change History</t>
   </si>
@@ -776,6 +776,12 @@
   </si>
   <si>
     <t>Added evidenceHandled field and handleEvidence event</t>
+  </si>
+  <si>
+    <t>Changed scannedDate field in ScannedDocument complex type to DateTime type</t>
+  </si>
+  <si>
+    <t>Aliveni Choppa</t>
   </si>
 </sst>
 </file>
@@ -1960,10 +1966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2135,6 +2141,23 @@
       </c>
       <c r="E11" s="2" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="145">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6">
+        <v>43404</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -9466,7 +9489,7 @@
   <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9786,7 +9809,7 @@
         <v>213</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="F9" s="38" t="s">
         <v>218</v>

</xml_diff>

<commit_message>
Updated fields list for handleEvidence event to allow caseworker to change only "evidenceHandled" field
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C0795C-7210-8949-B594-C51AF508AD28}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E5BA9B-031C-F04C-B60D-2AFC3C40E62E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="235">
   <si>
     <t>Change History</t>
   </si>
@@ -773,6 +773,9 @@
   </si>
   <si>
     <t>Case Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated CaseEventToFields list for handleEvidence event </t>
   </si>
 </sst>
 </file>
@@ -1880,9 +1883,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2088,6 +2091,23 @@
         <v>43420</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="115">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6">
+        <v>43430</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>185</v>
       </c>
     </row>
@@ -15257,8 +15277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15652,8 +15672,8 @@
       <c r="D11" s="131" t="s">
         <v>180</v>
       </c>
-      <c r="E11" s="132" t="s">
-        <v>158</v>
+      <c r="E11" s="130" t="s">
+        <v>177</v>
       </c>
       <c r="F11" s="43">
         <v>1</v>

</xml_diff>

<commit_message>
BPS-449 Updated ccd definitions to add subtype to Document complex type tab
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E5BA9B-031C-F04C-B60D-2AFC3C40E62E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0E4B8A-D654-5D4D-AC1B-B8110672CCD8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="238">
   <si>
     <t>Change History</t>
   </si>
@@ -776,6 +776,15 @@
   </si>
   <si>
     <t xml:space="preserve">Updated CaseEventToFields list for handleEvidence event </t>
+  </si>
+  <si>
+    <t>Updated Document complex type tab to include subtype</t>
+  </si>
+  <si>
+    <t>subtype</t>
+  </si>
+  <si>
+    <t>Document Subtype</t>
   </si>
 </sst>
 </file>
@@ -1883,10 +1892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2108,6 +2117,23 @@
         <v>43430</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="115">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6">
+        <v>43481</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>185</v>
       </c>
     </row>
@@ -13710,10 +13736,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" activeCellId="8" sqref="A2:XFD2 A1:XFD1 A3:XFD3 A7:XFD7 A8:XFD8 A9:XFD9 A10:XFD10 A11:XFD11 A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13965,53 +13991,53 @@
       <c r="A8" s="15">
         <v>43101</v>
       </c>
-      <c r="B8" s="13"/>
       <c r="C8" s="33" t="s">
         <v>157</v>
       </c>
       <c r="D8" s="87" t="s">
-        <v>164</v>
+        <v>236</v>
       </c>
       <c r="E8" s="87" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" s="87"/>
       <c r="G8" s="87" t="s">
-        <v>189</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="5"/>
+        <v>237</v>
+      </c>
       <c r="K8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="15">
         <v>43101</v>
       </c>
+      <c r="B9" s="13"/>
       <c r="C9" s="33" t="s">
         <v>157</v>
       </c>
       <c r="D9" s="87" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E9" s="87" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="116"/>
+        <v>48</v>
+      </c>
+      <c r="F9" s="87"/>
       <c r="G9" s="87" t="s">
-        <v>190</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="29" t="s">
         <v>30</v>
       </c>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
@@ -14021,14 +14047,14 @@
         <v>157</v>
       </c>
       <c r="D10" s="87" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E10" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="87"/>
+      <c r="F10" s="116"/>
       <c r="G10" s="87" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K10" s="29" t="s">
         <v>30</v>
@@ -14042,69 +14068,69 @@
         <v>157</v>
       </c>
       <c r="D11" s="87" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E11" s="87" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="87" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K11" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>43101</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="D12" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="5"/>
+      <c r="D12" s="87" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87" t="s">
+        <v>192</v>
+      </c>
       <c r="K12" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>43101</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="D13" s="87" t="s">
-        <v>222</v>
-      </c>
-      <c r="E13" s="87" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87" t="s">
-        <v>217</v>
-      </c>
+      <c r="G13" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="29" t="s">
         <v>30</v>
       </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
@@ -14114,14 +14140,14 @@
         <v>216</v>
       </c>
       <c r="D14" s="87" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E14" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="87"/>
       <c r="G14" s="87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K14" s="29" t="s">
         <v>30</v>
@@ -14135,14 +14161,14 @@
         <v>216</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E15" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="87"/>
       <c r="G15" s="87" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K15" s="29" t="s">
         <v>30</v>
@@ -14156,14 +14182,14 @@
         <v>216</v>
       </c>
       <c r="D16" s="87" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E16" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F16" s="87"/>
       <c r="G16" s="87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K16" s="29" t="s">
         <v>30</v>
@@ -14177,14 +14203,14 @@
         <v>216</v>
       </c>
       <c r="D17" s="87" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E17" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="87"/>
       <c r="G17" s="87" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="K17" s="29" t="s">
         <v>30</v>
@@ -14198,14 +14224,14 @@
         <v>216</v>
       </c>
       <c r="D18" s="87" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E18" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="87"/>
       <c r="G18" s="87" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="K18" s="29" t="s">
         <v>30</v>
@@ -14219,22 +14245,43 @@
         <v>216</v>
       </c>
       <c r="D19" s="87" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E19" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="87"/>
       <c r="G19" s="87" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K19" s="29" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A20" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" s="87" t="s">
+        <v>229</v>
+      </c>
+      <c r="E20" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87" t="s">
+        <v>231</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19" xr:uid="{95848D38-FC25-4E49-AE02-31A0B33A06F2}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20" xr:uid="{95848D38-FC25-4E49-AE02-31A0B33A06F2}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Added custom event history tab to bulkscan ccd definitions
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0E4B8A-D654-5D4D-AC1B-B8110672CCD8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B1E935-BA79-E54F-9A3A-2C5DF0DCD23A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="243">
   <si>
     <t>Change History</t>
   </si>
@@ -785,6 +785,21 @@
   </si>
   <si>
     <t>Document Subtype</t>
+  </si>
+  <si>
+    <t>EventHistory</t>
+  </si>
+  <si>
+    <t>Event History</t>
+  </si>
+  <si>
+    <t>Added Event history tab</t>
+  </si>
+  <si>
+    <t>customHistoryViewer</t>
+  </si>
+  <si>
+    <t>CaseHistoryViewer</t>
   </si>
 </sst>
 </file>
@@ -1892,10 +1907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="K1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2134,6 +2149,23 @@
         <v>43481</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="115">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6">
+        <v>43544</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2154,10 +2186,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:AA1048553"/>
+  <dimension ref="A1:AA1048554"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H8"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2277,16 +2309,16 @@
         <v>118</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>119</v>
+        <v>238</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>109</v>
+        <v>239</v>
       </c>
       <c r="G4" s="59">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>120</v>
+        <v>241</v>
       </c>
       <c r="I4" s="59">
         <v>1</v>
@@ -2310,13 +2342,13 @@
         <v>109</v>
       </c>
       <c r="G5" s="59">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="59">
         <v>1</v>
-      </c>
-      <c r="H5" s="132" t="s">
-        <v>210</v>
-      </c>
-      <c r="I5" s="59">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2337,13 +2369,13 @@
         <v>109</v>
       </c>
       <c r="G6" s="59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="132" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I6" s="59">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2364,13 +2396,13 @@
         <v>109</v>
       </c>
       <c r="G7" s="59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="132" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I7" s="59">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2391,13 +2423,13 @@
         <v>109</v>
       </c>
       <c r="G8" s="59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="132" t="s">
-        <v>177</v>
+        <v>214</v>
       </c>
       <c r="I8" s="59">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2412,30 +2444,57 @@
         <v>118</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G9" s="59">
         <v>2</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="132" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9" s="59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="59">
+        <v>3</v>
+      </c>
+      <c r="H10" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="I9" s="59">
+      <c r="I10" s="59">
         <v>1</v>
       </c>
     </row>
-    <row r="1048552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1048553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1048554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2710,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11919,10 +11978,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12098,9 +12157,26 @@
         <v>142</v>
       </c>
     </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A9" s="79">
+        <v>43101</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="132" t="s">
+        <v>241</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" s="80" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13458,10 +13534,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A2" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13712,14 +13788,35 @@
         <v>30</v>
       </c>
     </row>
+    <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="132" t="s">
+        <v>241</v>
+      </c>
+      <c r="E9" s="132"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="132" t="s">
+        <v>242</v>
+      </c>
+      <c r="H9" s="132"/>
+      <c r="J9" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L3" xr:uid="{5CF36EC4-574A-F740-BEC7-9B222789F5DB}"/>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13738,7 +13835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
renamed CaseEventHistory field id
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B1E935-BA79-E54F-9A3A-2C5DF0DCD23A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FB7D34-0E15-2B40-A2C8-A38065129489}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -793,13 +793,13 @@
     <t>Event History</t>
   </si>
   <si>
-    <t>Added Event history tab</t>
-  </si>
-  <si>
-    <t>customHistoryViewer</t>
-  </si>
-  <si>
     <t>CaseHistoryViewer</t>
+  </si>
+  <si>
+    <t>caseHistory</t>
+  </si>
+  <si>
+    <t>Added custom event history tab</t>
   </si>
 </sst>
 </file>
@@ -1909,9 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2157,7 +2155,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>7</v>
@@ -11980,8 +11978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13537,7 +13535,7 @@
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13802,7 +13800,7 @@
       <c r="E9" s="132"/>
       <c r="F9" s="130"/>
       <c r="G9" s="132" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H9" s="132"/>
       <c r="J9" s="5" t="s">

</xml_diff>

<commit_message>
renamed EventHistory tab id
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FB7D34-0E15-2B40-A2C8-A38065129489}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746604C6-63FE-4F4A-9BEF-23469527E55F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="244">
   <si>
     <t>Change History</t>
   </si>
@@ -787,9 +787,6 @@
     <t>Document Subtype</t>
   </si>
   <si>
-    <t>EventHistory</t>
-  </si>
-  <si>
     <t>Event History</t>
   </si>
   <si>
@@ -800,6 +797,12 @@
   </si>
   <si>
     <t>Added custom event history tab</t>
+  </si>
+  <si>
+    <t>Case History</t>
+  </si>
+  <si>
+    <t>eventHistory</t>
   </si>
 </sst>
 </file>
@@ -1909,7 +1912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2155,7 +2158,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>7</v>
@@ -2307,16 +2310,16 @@
         <v>118</v>
       </c>
       <c r="E4" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>238</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>239</v>
       </c>
       <c r="G4" s="59">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I4" s="59">
         <v>1</v>
@@ -11978,7 +11981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -12163,7 +12166,7 @@
         <v>149</v>
       </c>
       <c r="D9" s="132" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E9" s="77" t="s">
         <v>152</v>
@@ -13795,12 +13798,14 @@
         <v>149</v>
       </c>
       <c r="D9" s="132" t="s">
-        <v>241</v>
-      </c>
-      <c r="E9" s="132"/>
+        <v>240</v>
+      </c>
+      <c r="E9" s="132" t="s">
+        <v>242</v>
+      </c>
       <c r="F9" s="130"/>
       <c r="G9" s="132" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H9" s="132"/>
       <c r="J9" s="5" t="s">

</xml_diff>

<commit_message>
Add 'legacyId' case field and its 'previousServiceCaseReference' alias
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746604C6-63FE-4F4A-9BEF-23469527E55F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28492F2-6F15-0B4E-A0D8-D1887FCC52D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -32,11 +32,12 @@
     <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId18"/>
     <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId19"/>
+    <sheet name="SearchAlias" sheetId="20" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$L$7</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="252">
   <si>
     <t>Change History</t>
   </si>
@@ -803,6 +804,30 @@
   </si>
   <si>
     <t>eventHistory</t>
+  </si>
+  <si>
+    <t>SearchAlias</t>
+  </si>
+  <si>
+    <t>Unique alias id for a case field of a case type</t>
+  </si>
+  <si>
+    <t>This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
+  </si>
+  <si>
+    <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>legacyId</t>
+  </si>
+  <si>
+    <t>previousServiceCaseReference</t>
+  </si>
+  <si>
+    <t>Legacy ID</t>
+  </si>
+  <si>
+    <t>Created SearchAlias tab and added legacyId case field</t>
   </si>
 </sst>
 </file>
@@ -813,7 +838,7 @@
     <numFmt numFmtId="164" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1036,6 +1061,30 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1051,7 +1100,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1255,6 +1304,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1267,7 +1340,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1520,6 +1593,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="30" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -1910,9 +2001,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2168,6 +2261,23 @@
       </c>
       <c r="E16" s="2" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="115">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="6">
+        <v>43598</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -11981,7 +12091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -13362,6 +13472,107 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FE2902-4889-4846-A591-62C4C43C1C14}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="134" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="136" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="137" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="138"/>
+    </row>
+    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A2" s="139"/>
+      <c r="B2" s="140" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="140" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" s="140"/>
+      <c r="E2" s="138"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="141" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="142" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" s="142" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="142"/>
+      <c r="E3" s="138"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="138" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="143" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="144" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" s="145"/>
+      <c r="E4" s="138"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="138"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="138"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="138"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="138"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="147"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="138"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="138"/>
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA4"/>
@@ -13535,10 +13746,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13812,14 +14023,37 @@
         <v>30</v>
       </c>
     </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A10" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="132" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" s="132" t="s">
+        <v>250</v>
+      </c>
+      <c r="F10" s="130"/>
+      <c r="G10" s="132" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="132"/>
+      <c r="J10" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L3" xr:uid="{5CF36EC4-574A-F740-BEC7-9B222789F5DB}"/>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add legacyId to AuthorisationCaseField tab
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28492F2-6F15-0B4E-A0D8-D1887FCC52D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7736FA1D-8B69-8C4C-BC78-C6A35705F214}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="252">
   <si>
     <t>Change History</t>
   </si>
@@ -12089,10 +12089,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12285,9 +12285,26 @@
         <v>142</v>
       </c>
     </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A10" s="79">
+        <v>43101</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="132" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" s="80" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13477,7 +13494,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13748,8 +13765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Include legacyId field in createCase event
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7736FA1D-8B69-8C4C-BC78-C6A35705F214}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC08F1F1-280E-B94C-91C7-C8B534C87CFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="253">
   <si>
     <t>Change History</t>
   </si>
@@ -828,6 +828,9 @@
   </si>
   <si>
     <t>Created SearchAlias tab and added legacyId case field</t>
+  </si>
+  <si>
+    <t>Included legacyId field in createCase event</t>
   </si>
 </sst>
 </file>
@@ -2001,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2277,6 +2280,23 @@
         <v>43598</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="115">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6">
+        <v>43606</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>169</v>
       </c>
     </row>
@@ -12091,8 +12111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15673,10 +15693,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15830,8 +15850,8 @@
       <c r="D4" s="130" t="s">
         <v>208</v>
       </c>
-      <c r="E4" s="132" t="s">
-        <v>210</v>
+      <c r="E4" t="s">
+        <v>248</v>
       </c>
       <c r="F4" s="43">
         <v>1</v>
@@ -15866,7 +15886,7 @@
         <v>208</v>
       </c>
       <c r="E5" s="132" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F5" s="43">
         <v>2</v>
@@ -15901,7 +15921,7 @@
         <v>208</v>
       </c>
       <c r="E6" s="132" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F6" s="43">
         <v>3</v>
@@ -15936,7 +15956,7 @@
         <v>208</v>
       </c>
       <c r="E7" s="132" t="s">
-        <v>158</v>
+        <v>214</v>
       </c>
       <c r="F7" s="43">
         <v>4</v>
@@ -15971,7 +15991,7 @@
         <v>208</v>
       </c>
       <c r="E8" s="132" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="F8" s="43">
         <v>5</v>
@@ -16003,13 +16023,13 @@
         <v>149</v>
       </c>
       <c r="D9" s="130" t="s">
-        <v>154</v>
+        <v>208</v>
       </c>
       <c r="E9" s="132" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="F9" s="43">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G9"/>
       <c r="H9" s="56" t="s">
@@ -16022,7 +16042,7 @@
         <v>109</v>
       </c>
       <c r="K9" s="43">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -16031,7 +16051,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
-        <v>43466</v>
+        <v>43101</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
@@ -16040,14 +16060,15 @@
       <c r="D10" s="130" t="s">
         <v>154</v>
       </c>
-      <c r="E10" s="130" t="s">
-        <v>177</v>
+      <c r="E10" s="132" t="s">
+        <v>158</v>
       </c>
       <c r="F10" s="43">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G10"/>
       <c r="H10" s="56" t="s">
-        <v>182</v>
+        <v>108</v>
       </c>
       <c r="I10" s="43">
         <v>1</v>
@@ -16056,7 +16077,7 @@
         <v>109</v>
       </c>
       <c r="K10" s="43">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.15">
@@ -16067,14 +16088,14 @@
       <c r="C11" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="131" t="s">
-        <v>180</v>
+      <c r="D11" s="130" t="s">
+        <v>154</v>
       </c>
       <c r="E11" s="130" t="s">
         <v>177</v>
       </c>
       <c r="F11" s="43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="56" t="s">
         <v>182</v>
@@ -16086,12 +16107,42 @@
         <v>109</v>
       </c>
       <c r="K11" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A12" s="15">
+        <v>43466</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="131" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" s="130" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="43">
+        <v>1</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="I12" s="43">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="43">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A12 A4:A9" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add deliveryDate field to ScannedDocument in BulkScan ccd definitions
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC08F1F1-280E-B94C-91C7-C8B534C87CFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B11652B-75DF-044B-B7E3-FAE7BBA826F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="256">
   <si>
     <t>Change History</t>
   </si>
@@ -831,6 +831,15 @@
   </si>
   <si>
     <t>Included legacyId field in createCase event</t>
+  </si>
+  <si>
+    <t>Added deliveryDate field to ScannedDocument in complex types tab</t>
+  </si>
+  <si>
+    <t>deliveryDate</t>
+  </si>
+  <si>
+    <t>Delivery Date</t>
   </si>
 </sst>
 </file>
@@ -2004,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2298,6 +2307,23 @@
       </c>
       <c r="E18" s="2" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="115">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>253</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6">
+        <v>43599</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -14107,10 +14133,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14473,56 +14499,56 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>43101</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="D13" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="5"/>
+      <c r="D13" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87" t="s">
+        <v>255</v>
+      </c>
       <c r="K13" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>43101</v>
       </c>
-      <c r="C14" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="D14" s="87" t="s">
-        <v>222</v>
-      </c>
-      <c r="E14" s="87" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87" t="s">
-        <v>217</v>
-      </c>
+      <c r="G14" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="29" t="s">
         <v>30</v>
       </c>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="15">
@@ -14532,14 +14558,14 @@
         <v>216</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E15" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="87"/>
       <c r="G15" s="87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K15" s="29" t="s">
         <v>30</v>
@@ -14553,14 +14579,14 @@
         <v>216</v>
       </c>
       <c r="D16" s="87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E16" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F16" s="87"/>
       <c r="G16" s="87" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K16" s="29" t="s">
         <v>30</v>
@@ -14574,14 +14600,14 @@
         <v>216</v>
       </c>
       <c r="D17" s="87" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E17" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="87"/>
       <c r="G17" s="87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K17" s="29" t="s">
         <v>30</v>
@@ -14595,14 +14621,14 @@
         <v>216</v>
       </c>
       <c r="D18" s="87" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E18" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="87"/>
       <c r="G18" s="87" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="K18" s="29" t="s">
         <v>30</v>
@@ -14616,14 +14642,14 @@
         <v>216</v>
       </c>
       <c r="D19" s="87" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E19" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="87"/>
       <c r="G19" s="87" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="K19" s="29" t="s">
         <v>30</v>
@@ -14637,22 +14663,43 @@
         <v>216</v>
       </c>
       <c r="D20" s="87" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E20" s="87" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="87"/>
       <c r="G20" s="87" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K20" s="29" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A21" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="D21" s="87" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87" t="s">
+        <v>231</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20" xr:uid="{95848D38-FC25-4E49-AE02-31A0B33A06F2}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A21" xr:uid="{95848D38-FC25-4E49-AE02-31A0B33A06F2}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add AuthorisationCaseType tab to bulkscan ccd definitions
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B11652B-75DF-044B-B7E3-FAE7BBA826F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6862B4BE-B4FD-0E4C-8B46-6FEA49854FF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -18,26 +18,27 @@
     <sheet name="CaseType" sheetId="3" r:id="rId3"/>
     <sheet name="CaseField" sheetId="4" r:id="rId4"/>
     <sheet name="ComplexTypes" sheetId="5" r:id="rId5"/>
-    <sheet name="FixedLists" sheetId="6" r:id="rId6"/>
-    <sheet name="State" sheetId="7" r:id="rId7"/>
-    <sheet name="CaseEvent" sheetId="8" r:id="rId8"/>
-    <sheet name="CaseEventToFields" sheetId="9" r:id="rId9"/>
-    <sheet name="CaseTypeTab" sheetId="10" r:id="rId10"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId11"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId12"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId13"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId14"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId15"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId16"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId17"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId18"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId19"/>
-    <sheet name="SearchAlias" sheetId="20" r:id="rId20"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId6"/>
+    <sheet name="FixedLists" sheetId="6" r:id="rId7"/>
+    <sheet name="State" sheetId="7" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="8" r:id="rId9"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId10"/>
+    <sheet name="CaseTypeTab" sheetId="10" r:id="rId11"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId12"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId13"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId14"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId15"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId16"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId17"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId18"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId19"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId20"/>
+    <sheet name="SearchAlias" sheetId="20" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$L$7</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="263">
   <si>
     <t>Change History</t>
   </si>
@@ -840,6 +841,31 @@
   </si>
   <si>
     <t>Delivery Date</t>
+  </si>
+  <si>
+    <t>CRU</t>
+  </si>
+  <si>
+    <t>C - Create, R - Read, U - Update, D - Delete
+MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+MaxLength: 100.</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>Added AuthorisationComplexType tab</t>
   </si>
 </sst>
 </file>
@@ -850,7 +876,7 @@
     <numFmt numFmtId="164" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1097,6 +1123,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1341,7 +1378,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
@@ -1351,8 +1388,10 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1623,8 +1662,25 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1634,6 +1690,8 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="9" xr:uid="{1E974C16-ADD0-5843-899B-4B328845F1AC}"/>
+    <cellStyle name="Normal 2 3" xfId="10" xr:uid="{50BBC938-D2C4-2948-84ED-E190A296233A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2013,10 +2071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2323,6 +2381,23 @@
         <v>43599</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="115">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>43634</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2342,6 +2417,472 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AB12"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13" style="43" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.1640625" customWidth="1"/>
+    <col min="13" max="13" width="25.1640625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="25.5" customWidth="1"/>
+    <col min="15" max="28" width="7.1640625" customWidth="1"/>
+    <col min="29" max="1025" width="8.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="5"/>
+      <c r="K1"/>
+      <c r="M1"/>
+    </row>
+    <row r="2" spans="1:28" s="48" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+    </row>
+    <row r="3" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="N3" s="55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" s="43">
+        <v>1</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="43">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="43">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="132" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="43">
+        <v>2</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="43">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" s="43">
+        <v>2</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="132" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="43">
+        <v>3</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="43">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="43">
+        <v>3</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="43">
+        <v>4</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="43">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="43">
+        <v>4</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="43">
+        <v>5</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="43">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="43">
+        <v>5</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="132" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="43">
+        <v>6</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="43">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="43">
+        <v>6</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A10" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" s="43">
+        <v>1</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="43">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A11" s="15">
+        <v>43466</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="130" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" s="43">
+        <v>2</v>
+      </c>
+      <c r="H11" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="I11" s="43">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K11" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A12" s="15">
+        <v>43466</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="131" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" s="130" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="43">
+        <v>1</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="I12" s="43">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="43">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A12 A4:A9" xr:uid="{00000000-0002-0000-0800-000000000000}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AA1048554"/>
   <sheetViews>
@@ -2666,7 +3207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
@@ -2922,7 +3463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
@@ -3198,7 +3739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMK7"/>
   <sheetViews>
@@ -10491,7 +11032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -11759,7 +12300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
@@ -12034,7 +12575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -12133,7 +12674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
@@ -12365,7 +12906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
@@ -12532,7 +13073,156 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AA4"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" customWidth="1"/>
+    <col min="6" max="27" width="7.1640625" customWidth="1"/>
+    <col min="28" max="1025" width="8.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+    </row>
+    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+    </row>
+    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK4"/>
   <sheetViews>
@@ -13386,156 +14076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA4"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
-    <col min="6" max="27" width="7.1640625" customWidth="1"/>
-    <col min="28" max="1025" width="8.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-    </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13"/>
-    </row>
-    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>42736</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FE2902-4889-4846-A591-62C4C43C1C14}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -14135,7 +14676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -14715,6 +15256,411 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB819C9-5507-5442-ABBF-DB2BA25FD59C}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="148" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="148" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="148" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="148" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="148" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="148" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="148" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="148"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="160" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="159" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="158" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="157" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+    </row>
+    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="A2" s="156"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="155" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="155" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="155" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" s="155" t="s">
+        <v>258</v>
+      </c>
+      <c r="G2" s="155" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="154" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="154" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="153" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="153" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="153" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="152" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="152" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B4" s="149"/>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B5" s="149"/>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B6" s="149"/>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B7" s="149"/>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B8" s="149"/>
+      <c r="C8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" t="s">
+        <v>152</v>
+      </c>
+      <c r="G8" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B9" s="149"/>
+      <c r="C9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B10" s="149"/>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" t="s">
+        <v>254</v>
+      </c>
+      <c r="F10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B11" s="149"/>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B12" s="149"/>
+      <c r="C12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="E12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+      <c r="G12" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B13" s="149"/>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B14" s="149"/>
+      <c r="C14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="E14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B15" s="149"/>
+      <c r="C15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="E15" t="s">
+        <v>225</v>
+      </c>
+      <c r="F15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G15" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B16" s="149"/>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B17" s="149"/>
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="E17" t="s">
+        <v>228</v>
+      </c>
+      <c r="F17" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="150">
+        <v>43101</v>
+      </c>
+      <c r="B18" s="149"/>
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="E18" t="s">
+        <v>229</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G18" s="149" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{FB92365D-369B-0044-A8EE-223BE5F20B8F}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
@@ -15277,7 +16223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
@@ -15420,7 +16366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -15736,470 +16682,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB12"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13" style="43" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" style="24" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.1640625" customWidth="1"/>
-    <col min="13" max="13" width="25.1640625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="25.5" customWidth="1"/>
-    <col min="15" max="28" width="7.1640625" customWidth="1"/>
-    <col min="29" max="1025" width="8.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="5"/>
-      <c r="K1"/>
-      <c r="M1"/>
-    </row>
-    <row r="2" spans="1:28" s="48" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="K2" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-    </row>
-    <row r="3" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="J3" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="K3" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="L3" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="N3" s="55" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="130" t="s">
-        <v>208</v>
-      </c>
-      <c r="E4" t="s">
-        <v>248</v>
-      </c>
-      <c r="F4" s="43">
-        <v>1</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="43">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K4" s="43">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="130" t="s">
-        <v>208</v>
-      </c>
-      <c r="E5" s="132" t="s">
-        <v>210</v>
-      </c>
-      <c r="F5" s="43">
-        <v>2</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="I5" s="43">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K5" s="43">
-        <v>2</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="130" t="s">
-        <v>208</v>
-      </c>
-      <c r="E6" s="132" t="s">
-        <v>212</v>
-      </c>
-      <c r="F6" s="43">
-        <v>3</v>
-      </c>
-      <c r="G6"/>
-      <c r="H6" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" s="43">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K6" s="43">
-        <v>3</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D7" s="130" t="s">
-        <v>208</v>
-      </c>
-      <c r="E7" s="132" t="s">
-        <v>214</v>
-      </c>
-      <c r="F7" s="43">
-        <v>4</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7" s="43">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K7" s="43">
-        <v>4</v>
-      </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D8" s="130" t="s">
-        <v>208</v>
-      </c>
-      <c r="E8" s="132" t="s">
-        <v>158</v>
-      </c>
-      <c r="F8" s="43">
-        <v>5</v>
-      </c>
-      <c r="G8"/>
-      <c r="H8" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" s="43">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K8" s="43">
-        <v>5</v>
-      </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" s="130" t="s">
-        <v>208</v>
-      </c>
-      <c r="E9" s="132" t="s">
-        <v>177</v>
-      </c>
-      <c r="F9" s="43">
-        <v>6</v>
-      </c>
-      <c r="G9"/>
-      <c r="H9" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="I9" s="43">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K9" s="43">
-        <v>6</v>
-      </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A10" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D10" s="130" t="s">
-        <v>154</v>
-      </c>
-      <c r="E10" s="132" t="s">
-        <v>158</v>
-      </c>
-      <c r="F10" s="43">
-        <v>1</v>
-      </c>
-      <c r="G10"/>
-      <c r="H10" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="I10" s="43">
-        <v>1</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K10" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A11" s="15">
-        <v>43466</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D11" s="130" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11" s="130" t="s">
-        <v>177</v>
-      </c>
-      <c r="F11" s="43">
-        <v>2</v>
-      </c>
-      <c r="H11" s="56" t="s">
-        <v>182</v>
-      </c>
-      <c r="I11" s="43">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K11" s="43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A12" s="15">
-        <v>43466</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D12" s="131" t="s">
-        <v>180</v>
-      </c>
-      <c r="E12" s="130" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" s="43">
-        <v>1</v>
-      </c>
-      <c r="H12" s="56" t="s">
-        <v>182</v>
-      </c>
-      <c r="I12" s="43">
-        <v>1</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K12" s="43">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A12 A4:A9" xr:uid="{00000000-0002-0000-0800-000000000000}">
-      <formula1>42736</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated bulkscan ccd definition to add new fields and some mandatory fields
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6862B4BE-B4FD-0E4C-8B46-6FEA49854FF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080A2C5C-6219-E948-AE52-C6EEC11A7B54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="25560" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17240" tabRatio="500" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,26 @@
     <sheet name="CaseType" sheetId="3" r:id="rId3"/>
     <sheet name="CaseField" sheetId="4" r:id="rId4"/>
     <sheet name="ComplexTypes" sheetId="5" r:id="rId5"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId6"/>
-    <sheet name="FixedLists" sheetId="6" r:id="rId7"/>
-    <sheet name="State" sheetId="7" r:id="rId8"/>
-    <sheet name="CaseEvent" sheetId="8" r:id="rId9"/>
-    <sheet name="CaseEventToFields" sheetId="9" r:id="rId10"/>
-    <sheet name="CaseTypeTab" sheetId="10" r:id="rId11"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId12"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId13"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId14"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId15"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId16"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId17"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId18"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId19"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId20"/>
-    <sheet name="SearchAlias" sheetId="20" r:id="rId21"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId6"/>
+    <sheet name="CaseEventToComplexTypes" sheetId="21" r:id="rId7"/>
+    <sheet name="FixedLists" sheetId="6" r:id="rId8"/>
+    <sheet name="State" sheetId="7" r:id="rId9"/>
+    <sheet name="CaseEvent" sheetId="8" r:id="rId10"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId11"/>
+    <sheet name="CaseTypeTab" sheetId="10" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId13"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId14"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId15"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId16"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId17"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId18"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId21"/>
+    <sheet name="SearchAlias" sheetId="20" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$L$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$L$10</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="283">
   <si>
     <t>Change History</t>
   </si>
@@ -843,29 +844,93 @@
     <t>Delivery Date</t>
   </si>
   <si>
-    <t>CRU</t>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>contactNumber</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>PhoneUK</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>Contact Details</t>
+  </si>
+  <si>
+    <t>contactDetails</t>
+  </si>
+  <si>
+    <t>Added new fields to the case to test phase 2 changes</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>FieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>EventHintText</t>
+  </si>
+  <si>
+    <t>EventElementLabel</t>
+  </si>
+  <si>
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+MaxLength: 1000</t>
+  </si>
+  <si>
+    <t>Accepted Values:  for mandatory, readonly and optional data on UI
+MustBe: MANDATORY, READONLY, OPTIONAL</t>
+  </si>
+  <si>
+    <t>The order of the fields on the screen.
+Positive Integer</t>
+  </si>
+  <si>
+    <t>MaxLength:300</t>
+  </si>
+  <si>
+    <t>Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>EventToComplexTypes</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+MaxLength: 100.</t>
   </si>
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
   <si>
-    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
-MaxLength: 100.</t>
-  </si>
-  <si>
-    <t>The Field ID should match an ID in the CaseField Tab
-MaxLength: 70</t>
-  </si>
-  <si>
-    <t>Must match ID on 'CaseType' tab
-MaxLength: 70</t>
-  </si>
-  <si>
-    <t>AuthorisationComplexType</t>
-  </si>
-  <si>
-    <t>Added AuthorisationComplexType tab</t>
+    <t>READONLY</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1443,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
@@ -1388,10 +1453,11 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1662,25 +1728,29 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="9" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1690,8 +1760,9 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="9" xr:uid="{1E974C16-ADD0-5843-899B-4B328845F1AC}"/>
-    <cellStyle name="Normal 2 3" xfId="10" xr:uid="{50BBC938-D2C4-2948-84ED-E190A296233A}"/>
+    <cellStyle name="Normal 2" xfId="11" xr:uid="{68453A2E-9B27-5445-AD1C-3F45F88A9FBF}"/>
+    <cellStyle name="Normal 2 3" xfId="9" xr:uid="{7691E89B-92EC-CA46-80C2-9C309E07083D}"/>
+    <cellStyle name="Normal 3" xfId="10" xr:uid="{8B489D75-9D3B-8C49-A9B3-69099076E245}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2073,7 +2144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -2378,7 +2449,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="6">
-        <v>43599</v>
+        <v>43630</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>185</v>
@@ -2389,13 +2460,13 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="6">
-        <v>43634</v>
+        <v>43636</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>185</v>
@@ -2417,11 +2488,329 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="30.5" customWidth="1"/>
+    <col min="6" max="6" width="38.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="10" max="10" width="26" style="19" customWidth="1"/>
+    <col min="11" max="11" width="28" style="19" customWidth="1"/>
+    <col min="12" max="12" width="27.5" style="19" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="68.5" style="19" customWidth="1"/>
+    <col min="15" max="15" width="25.5" style="19" customWidth="1"/>
+    <col min="16" max="16" width="20.5" customWidth="1"/>
+    <col min="17" max="17" width="27.5" customWidth="1"/>
+    <col min="18" max="19" width="7.1640625" style="2" customWidth="1"/>
+    <col min="20" max="29" width="7.1640625" customWidth="1"/>
+    <col min="30" max="1025" width="8.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+    </row>
+    <row r="2" spans="1:29" ht="98" x14ac:dyDescent="0.15">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="41"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+    </row>
+    <row r="3" spans="1:29" ht="45" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="R3" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="S3" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
+      <c r="A4" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="43">
+        <v>1</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="45"/>
+      <c r="P4" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
+      <c r="A5" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="43">
+        <v>2</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="P5" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
+      <c r="A6" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="130" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="43">
+        <v>3</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="P6" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0700-000000000000}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0700-000001000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G6" xr:uid="{00000000-0002-0000-0700-000002000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AB29"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2618,7 +3007,7 @@
       </c>
       <c r="G5"/>
       <c r="H5" s="56" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="I5" s="43">
         <v>1</v>
@@ -2653,7 +3042,7 @@
       </c>
       <c r="G6"/>
       <c r="H6" s="56" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="I6" s="43">
         <v>1</v>
@@ -2681,14 +3070,14 @@
         <v>208</v>
       </c>
       <c r="E7" s="132" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="F7" s="43">
         <v>4</v>
       </c>
       <c r="G7"/>
       <c r="H7" s="56" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="I7" s="43">
         <v>1</v>
@@ -2716,23 +3105,23 @@
         <v>208</v>
       </c>
       <c r="E8" s="132" t="s">
-        <v>158</v>
+        <v>259</v>
       </c>
       <c r="F8" s="43">
         <v>5</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="56" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="I8" s="43">
+        <v>2</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="K8" s="43">
         <v>1</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K8" s="43">
-        <v>5</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -2751,30 +3140,30 @@
         <v>208</v>
       </c>
       <c r="E9" s="132" t="s">
-        <v>177</v>
+        <v>258</v>
       </c>
       <c r="F9" s="43">
         <v>6</v>
       </c>
       <c r="G9"/>
       <c r="H9" s="56" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="I9" s="43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
       <c r="K9" s="43">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
         <v>43101</v>
       </c>
@@ -2783,91 +3172,229 @@
         <v>149</v>
       </c>
       <c r="D10" s="130" t="s">
-        <v>154</v>
+        <v>208</v>
       </c>
       <c r="E10" s="132" t="s">
-        <v>158</v>
+        <v>214</v>
       </c>
       <c r="F10" s="43">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G10"/>
       <c r="H10" s="56" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="I10" s="43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
       <c r="K10" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
-        <v>43466</v>
+        <v>43101</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
         <v>149</v>
       </c>
       <c r="D11" s="130" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11" s="130" t="s">
-        <v>177</v>
+        <v>208</v>
+      </c>
+      <c r="E11" s="132" t="s">
+        <v>158</v>
       </c>
       <c r="F11" s="43">
+        <v>8</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="43">
         <v>2</v>
       </c>
-      <c r="H11" s="56" t="s">
-        <v>182</v>
-      </c>
-      <c r="I11" s="43">
-        <v>1</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
       <c r="K11" s="43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
-        <v>43466</v>
+        <v>43101</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" t="s">
         <v>149</v>
       </c>
-      <c r="D12" s="131" t="s">
+      <c r="D12" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" s="132" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="43">
+        <v>9</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="43">
+        <v>2</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="K12" s="43">
+        <v>5</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A13" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="43">
+        <v>1</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="43">
+        <v>1</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A14" s="15">
+        <v>43466</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="130" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" s="43">
+        <v>2</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="I14" s="43">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A15" s="15">
+        <v>43466</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="131" t="s">
         <v>180</v>
       </c>
-      <c r="E12" s="130" t="s">
+      <c r="E15" s="130" t="s">
         <v>177</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F15" s="43">
         <v>1</v>
       </c>
-      <c r="H12" s="56" t="s">
+      <c r="H15" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="I12" s="43">
+      <c r="I15" s="43">
         <v>1</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K12" s="43">
+      <c r="J15" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15" s="43">
         <v>1</v>
       </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E19" s="132"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E20" s="132"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E21" s="132"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E22" s="132"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E23" s="132"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E24" s="132"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E25" s="132"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E26" s="132"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E27" s="132"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E28" s="132"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E29" s="132"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A12 A4:A9" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2882,12 +3409,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:AA1048554"/>
+  <dimension ref="A1:AA1048557"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3124,10 +3651,10 @@
         <v>2</v>
       </c>
       <c r="H8" s="132" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="I8" s="59">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3142,19 +3669,19 @@
         <v>118</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>119</v>
+        <v>264</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
       <c r="G9" s="59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9" s="132" t="s">
-        <v>177</v>
+        <v>259</v>
       </c>
       <c r="I9" s="59">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3169,30 +3696,111 @@
         <v>118</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>121</v>
+        <v>264</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>122</v>
+        <v>263</v>
       </c>
       <c r="G10" s="59">
         <v>3</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="132" t="s">
+        <v>258</v>
+      </c>
+      <c r="I10" s="59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="G11" s="59">
+        <v>3</v>
+      </c>
+      <c r="H11" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="I11" s="59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="59">
+        <v>4</v>
+      </c>
+      <c r="H12" s="132" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="59">
+        <v>4</v>
+      </c>
+      <c r="H13" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="I10" s="59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1048553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="I13" s="59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1048556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1048557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A13" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B13" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3207,7 +3815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
@@ -3463,7 +4071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
@@ -3739,7 +4347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMK7"/>
   <sheetViews>
@@ -11032,7 +11640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -12300,7 +12908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
@@ -12575,12 +13183,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12674,12 +13282,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12812,7 +13420,7 @@
         <v>149</v>
       </c>
       <c r="D6" s="132" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="E6" s="77" t="s">
         <v>152</v>
@@ -12822,19 +13430,20 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A7" s="79">
+      <c r="A7" s="75">
         <v>43101</v>
       </c>
+      <c r="B7" s="76"/>
       <c r="C7" s="5" t="s">
         <v>149</v>
       </c>
       <c r="D7" s="132" t="s">
-        <v>158</v>
+        <v>258</v>
       </c>
       <c r="E7" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="F7" s="80" t="s">
+      <c r="F7" s="78" t="s">
         <v>142</v>
       </c>
     </row>
@@ -12846,7 +13455,7 @@
         <v>149</v>
       </c>
       <c r="D8" s="132" t="s">
-        <v>177</v>
+        <v>214</v>
       </c>
       <c r="E8" s="77" t="s">
         <v>152</v>
@@ -12863,7 +13472,7 @@
         <v>149</v>
       </c>
       <c r="D9" s="132" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="E9" s="77" t="s">
         <v>152</v>
@@ -12880,7 +13489,7 @@
         <v>149</v>
       </c>
       <c r="D10" s="132" t="s">
-        <v>248</v>
+        <v>158</v>
       </c>
       <c r="E10" s="77" t="s">
         <v>152</v>
@@ -12889,176 +13498,93 @@
         <v>142</v>
       </c>
     </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A11" s="79">
+        <v>43101</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="132" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" s="80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A12" s="79">
+        <v>43101</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="132" t="s">
+        <v>240</v>
+      </c>
+      <c r="E12" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A13" s="79">
+        <v>43101</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="132" t="s">
+        <v>248</v>
+      </c>
+      <c r="E13" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" s="80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="D16" s="132"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D17" s="132"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D18" s="132"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D19" s="132"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D20" s="132"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D21" s="132"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D22" s="132"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D23" s="132"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D24" s="132"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D25" s="132"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D26" s="132"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-1000-000000000000}">
-      <formula1>42736</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:AA6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.5" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
-    <col min="7" max="1025" width="8.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" s="86" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="83" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="84" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="85" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-    </row>
-    <row r="2" spans="1:27" s="19" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-    </row>
-    <row r="3" spans="1:27" s="56" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="56" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A4" s="75">
-        <v>43101</v>
-      </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="130" t="s">
-        <v>208</v>
-      </c>
-      <c r="E4" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="78" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A5" s="79">
-        <v>43101</v>
-      </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="130" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="80" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A6" s="79">
-        <v>43101</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="130" t="s">
-        <v>180</v>
-      </c>
-      <c r="E6" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="F6" s="88" t="s">
-        <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-1100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A13" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13078,7 +13604,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13223,6 +13749,173 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:AA6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="7" max="1025" width="8.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="86" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A1" s="82" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="85" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:27" s="19" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+    </row>
+    <row r="3" spans="1:27" s="56" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A4" s="75">
+        <v>43101</v>
+      </c>
+      <c r="B4" s="76"/>
+      <c r="C4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="130" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="78" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A5" s="79">
+        <v>43101</v>
+      </c>
+      <c r="B5" s="87"/>
+      <c r="C5" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="A6" s="79">
+        <v>43101</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="130" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="88" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-1100-000000000000}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK4"/>
   <sheetViews>
@@ -14076,12 +14769,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FE2902-4889-4846-A591-62C4C43C1C14}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14182,7 +14875,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14350,7 +15043,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -14542,14 +15235,14 @@
         <v>149</v>
       </c>
       <c r="D6" s="132" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="E6" s="132" t="s">
-        <v>215</v>
+        <v>256</v>
       </c>
       <c r="F6" s="130"/>
       <c r="G6" s="132" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="H6" s="132"/>
       <c r="J6" s="5" t="s">
@@ -14565,18 +15258,16 @@
         <v>149</v>
       </c>
       <c r="D7" s="132" t="s">
-        <v>158</v>
+        <v>258</v>
       </c>
       <c r="E7" s="132" t="s">
-        <v>47</v>
+        <v>257</v>
       </c>
       <c r="F7" s="130"/>
       <c r="G7" s="132" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="132" t="s">
-        <v>157</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="H7" s="132"/>
       <c r="J7" s="5" t="s">
         <v>30</v>
       </c>
@@ -14590,14 +15281,14 @@
         <v>149</v>
       </c>
       <c r="D8" s="132" t="s">
-        <v>177</v>
+        <v>214</v>
       </c>
       <c r="E8" s="132" t="s">
-        <v>178</v>
+        <v>215</v>
       </c>
       <c r="F8" s="130"/>
       <c r="G8" s="132" t="s">
-        <v>179</v>
+        <v>216</v>
       </c>
       <c r="H8" s="132"/>
       <c r="J8" s="5" t="s">
@@ -14613,21 +15304,21 @@
         <v>149</v>
       </c>
       <c r="D9" s="132" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="E9" s="132" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="F9" s="130"/>
       <c r="G9" s="132" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="H9" s="132"/>
       <c r="J9" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
         <v>43101</v>
       </c>
@@ -14636,28 +15327,99 @@
         <v>149</v>
       </c>
       <c r="D10" s="132" t="s">
-        <v>248</v>
+        <v>158</v>
       </c>
       <c r="E10" s="132" t="s">
-        <v>250</v>
+        <v>47</v>
       </c>
       <c r="F10" s="130"/>
       <c r="G10" s="132" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="132" t="s">
+        <v>157</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="132" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="132" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="130"/>
+      <c r="G11" s="132" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="132"/>
+      <c r="J11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="132" t="s">
+        <v>240</v>
+      </c>
+      <c r="E12" s="132" t="s">
+        <v>242</v>
+      </c>
+      <c r="F12" s="130"/>
+      <c r="G12" s="132" t="s">
+        <v>239</v>
+      </c>
+      <c r="H12" s="132"/>
+      <c r="J12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A13" s="15">
+        <v>43101</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="132" t="s">
+        <v>248</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>250</v>
+      </c>
+      <c r="F13" s="130"/>
+      <c r="G13" s="132" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="132"/>
-      <c r="J10" s="5" t="s">
+      <c r="H13" s="132"/>
+      <c r="J13" s="5" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L3" xr:uid="{5CF36EC4-574A-F740-BEC7-9B222789F5DB}"/>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A13" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B13" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -14677,7 +15439,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G8" sqref="A1:R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15256,397 +16018,397 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB819C9-5507-5442-ABBF-DB2BA25FD59C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB4E5300-4FA0-3842-8A40-CF2A51B4EA3C}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" style="148" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="148" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="148" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="148" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="148" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="148" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="148" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="148"/>
+    <col min="1" max="1" width="33.1640625" style="160" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="160" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="160" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="160" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="160" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="160" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="160" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="160"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="160" t="s">
-        <v>261</v>
-      </c>
-      <c r="B1" s="159" t="s">
+      <c r="A1" s="159" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="158" t="s">
+      <c r="C1" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="157" t="s">
+      <c r="D1" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
     </row>
     <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A2" s="156"/>
-      <c r="B2" s="156"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="155" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="D2" s="155" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="E2" s="155" t="s">
         <v>196</v>
       </c>
       <c r="F2" s="155" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="G2" s="155" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="153" t="s">
+      <c r="C3" s="152" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="153" t="s">
+      <c r="D3" s="152" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="153" t="s">
+      <c r="E3" s="152" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="152" t="s">
+      <c r="F3" s="162" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="152" t="s">
+      <c r="G3" s="162" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="150">
+      <c r="A4" s="15">
         <v>43101</v>
       </c>
-      <c r="B4" s="149"/>
+      <c r="B4" s="148"/>
       <c r="C4" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="151" t="s">
+      <c r="D4" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="87" t="s">
         <v>162</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="149" t="s">
-        <v>256</v>
+      <c r="G4" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="150">
+      <c r="A5" s="15">
         <v>43101</v>
       </c>
-      <c r="B5" s="149"/>
+      <c r="B5" s="148"/>
       <c r="C5" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="151" t="s">
+      <c r="D5" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="87" t="s">
         <v>236</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="149" t="s">
-        <v>256</v>
+      <c r="G5" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="150">
+      <c r="A6" s="15">
         <v>43101</v>
       </c>
-      <c r="B6" s="149"/>
+      <c r="B6" s="148"/>
       <c r="C6" t="s">
         <v>149</v>
       </c>
-      <c r="D6" s="151" t="s">
+      <c r="D6" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="149" t="s">
-        <v>256</v>
+      <c r="G6" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="150">
+      <c r="A7" s="15">
         <v>43101</v>
       </c>
-      <c r="B7" s="149"/>
+      <c r="B7" s="148"/>
       <c r="C7" t="s">
         <v>149</v>
       </c>
-      <c r="D7" s="151" t="s">
+      <c r="D7" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="149" t="s">
-        <v>256</v>
+      <c r="G7" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="150">
+      <c r="A8" s="15">
         <v>43101</v>
       </c>
-      <c r="B8" s="149"/>
+      <c r="B8" s="148"/>
       <c r="C8" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="151" t="s">
+      <c r="D8" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="87" t="s">
         <v>161</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="149" t="s">
-        <v>256</v>
+      <c r="G8" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="150">
+      <c r="A9" s="15">
         <v>43101</v>
       </c>
-      <c r="B9" s="149"/>
+      <c r="B9" s="148"/>
       <c r="C9" t="s">
         <v>149</v>
       </c>
-      <c r="D9" s="151" t="s">
+      <c r="D9" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="149" t="s">
-        <v>256</v>
+      <c r="G9" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="150">
+      <c r="A10" s="15">
         <v>43101</v>
       </c>
-      <c r="B10" s="149"/>
+      <c r="B10" s="148"/>
       <c r="C10" t="s">
         <v>149</v>
       </c>
-      <c r="D10" s="151" t="s">
+      <c r="D10" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="87" t="s">
         <v>254</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G10" s="149" t="s">
-        <v>256</v>
+      <c r="G10" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="150">
+      <c r="A11" s="15">
         <v>43101</v>
       </c>
-      <c r="B11" s="149"/>
+      <c r="B11" s="148"/>
       <c r="C11" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="151" t="s">
+      <c r="D11" s="150" t="s">
         <v>158</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="149" t="s">
-        <v>256</v>
+      <c r="G11" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="150">
+      <c r="A12" s="15">
         <v>43101</v>
       </c>
-      <c r="B12" s="149"/>
+      <c r="B12" s="148"/>
       <c r="C12" t="s">
         <v>149</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="132" t="s">
         <v>214</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="87" t="s">
         <v>222</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G12" s="149" t="s">
-        <v>256</v>
+      <c r="G12" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="150">
+      <c r="A13" s="15">
         <v>43101</v>
       </c>
-      <c r="B13" s="149"/>
+      <c r="B13" s="148"/>
       <c r="C13" t="s">
         <v>149</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="132" t="s">
         <v>214</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="87" t="s">
         <v>223</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="149" t="s">
-        <v>256</v>
+      <c r="G13" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="150">
+      <c r="A14" s="15">
         <v>43101</v>
       </c>
-      <c r="B14" s="149"/>
+      <c r="B14" s="148"/>
       <c r="C14" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="132" t="s">
         <v>214</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="87" t="s">
         <v>224</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="149" t="s">
-        <v>256</v>
+      <c r="G14" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="150">
+      <c r="A15" s="15">
         <v>43101</v>
       </c>
-      <c r="B15" s="149"/>
+      <c r="B15" s="148"/>
       <c r="C15" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="132" t="s">
         <v>214</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="87" t="s">
         <v>225</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="149" t="s">
-        <v>256</v>
+      <c r="G15" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="150">
+      <c r="A16" s="15">
         <v>43101</v>
       </c>
-      <c r="B16" s="149"/>
+      <c r="B16" s="148"/>
       <c r="C16" t="s">
         <v>149</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="132" t="s">
         <v>214</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="87" t="s">
         <v>227</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="149" t="s">
-        <v>256</v>
+      <c r="G16" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="150">
+      <c r="A17" s="15">
         <v>43101</v>
       </c>
-      <c r="B17" s="149"/>
+      <c r="B17" s="148"/>
       <c r="C17" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="132" t="s">
         <v>214</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="87" t="s">
         <v>228</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G17" s="149" t="s">
-        <v>256</v>
+      <c r="G17" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="150">
+      <c r="A18" s="15">
         <v>43101</v>
       </c>
-      <c r="B18" s="149"/>
+      <c r="B18" s="148"/>
       <c r="C18" t="s">
         <v>149</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="132" t="s">
         <v>214</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="87" t="s">
         <v>229</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G18" s="149" t="s">
-        <v>256</v>
+      <c r="G18" s="148" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -15661,6 +16423,746 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFC173F-8B90-4E46-9FB4-78E7E15983D2}">
+  <dimension ref="A1:X1048569"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" style="148" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="148" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="148" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="148" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="148" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="148" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" style="148" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="148" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" style="148" customWidth="1"/>
+    <col min="10" max="10" width="22.5" style="148" customWidth="1"/>
+    <col min="11" max="11" width="22" style="148" customWidth="1"/>
+    <col min="12" max="1021" width="8.83203125" style="148" customWidth="1"/>
+    <col min="1022" max="16384" width="8.83203125" style="148"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="159" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="158" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="156" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="153" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="A2" s="154" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="155" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="155" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" s="155" t="s">
+        <v>274</v>
+      </c>
+      <c r="E2" s="155" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="155" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="155" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="155" t="s">
+        <v>273</v>
+      </c>
+      <c r="I2" s="155" t="s">
+        <v>272</v>
+      </c>
+      <c r="J2" s="155" t="s">
+        <v>271</v>
+      </c>
+      <c r="K2" s="154" t="s">
+        <v>270</v>
+      </c>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
+      <c r="R2" s="154"/>
+      <c r="S2" s="154"/>
+      <c r="T2" s="154"/>
+      <c r="U2" s="154"/>
+      <c r="V2" s="154"/>
+      <c r="W2" s="154"/>
+      <c r="X2" s="154"/>
+    </row>
+    <row r="3" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="151" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="151" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="152" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="152" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="152" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="152" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="151" t="s">
+        <v>269</v>
+      </c>
+      <c r="H3" s="151" t="s">
+        <v>268</v>
+      </c>
+      <c r="I3" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="J3" s="151" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="151" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A4" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C4" s="132" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="87" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="87" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" s="148">
+        <v>1</v>
+      </c>
+      <c r="J4" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A5" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C5" s="132" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" s="87" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" s="87" t="s">
+        <v>218</v>
+      </c>
+      <c r="I5" s="148">
+        <v>2</v>
+      </c>
+      <c r="J5" s="148" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A6" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C6" s="132" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" s="87" t="s">
+        <v>224</v>
+      </c>
+      <c r="G6" s="87" t="s">
+        <v>219</v>
+      </c>
+      <c r="I6" s="148">
+        <v>3</v>
+      </c>
+      <c r="J6" s="148" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A7" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C7" s="132" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="87" t="s">
+        <v>225</v>
+      </c>
+      <c r="G7" s="87" t="s">
+        <v>220</v>
+      </c>
+      <c r="I7" s="148">
+        <v>4</v>
+      </c>
+      <c r="J7" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A8" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C8" s="132" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" s="148" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" s="87" t="s">
+        <v>227</v>
+      </c>
+      <c r="G8" s="87" t="s">
+        <v>226</v>
+      </c>
+      <c r="I8" s="148">
+        <v>5</v>
+      </c>
+      <c r="J8" s="148" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A9" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C9" s="132" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="148" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" s="87" t="s">
+        <v>228</v>
+      </c>
+      <c r="G9" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="I9" s="148">
+        <v>6</v>
+      </c>
+      <c r="J9" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A10" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C10" s="132" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" s="148" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="132" t="s">
+        <v>214</v>
+      </c>
+      <c r="F10" s="87" t="s">
+        <v>229</v>
+      </c>
+      <c r="G10" s="87" t="s">
+        <v>231</v>
+      </c>
+      <c r="I10" s="148">
+        <v>7</v>
+      </c>
+      <c r="J10" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A11" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E11" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="87" t="s">
+        <v>188</v>
+      </c>
+      <c r="I11" s="148">
+        <v>1</v>
+      </c>
+      <c r="J11" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A12" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="87" t="s">
+        <v>236</v>
+      </c>
+      <c r="G12" s="87" t="s">
+        <v>237</v>
+      </c>
+      <c r="I12" s="148">
+        <v>2</v>
+      </c>
+      <c r="J12" s="148" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A13" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="87" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13" s="87" t="s">
+        <v>189</v>
+      </c>
+      <c r="I13" s="148">
+        <v>3</v>
+      </c>
+      <c r="J13" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A14" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="87" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="87" t="s">
+        <v>190</v>
+      </c>
+      <c r="I14" s="148">
+        <v>4</v>
+      </c>
+      <c r="J14" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A15" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E15" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="87" t="s">
+        <v>161</v>
+      </c>
+      <c r="G15" s="87" t="s">
+        <v>191</v>
+      </c>
+      <c r="I15" s="148">
+        <v>5</v>
+      </c>
+      <c r="J15" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A16" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E16" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="87" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" s="87" t="s">
+        <v>192</v>
+      </c>
+      <c r="I16" s="148">
+        <v>6</v>
+      </c>
+      <c r="J16" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A17" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E17" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="G17" s="87" t="s">
+        <v>255</v>
+      </c>
+      <c r="I17" s="148">
+        <v>7</v>
+      </c>
+      <c r="J17" s="148" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A18" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="E18" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="I18" s="148">
+        <v>8</v>
+      </c>
+      <c r="J18" s="148" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A19" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="87" t="s">
+        <v>188</v>
+      </c>
+      <c r="I19" s="148">
+        <v>1</v>
+      </c>
+      <c r="J19" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A20" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" s="87" t="s">
+        <v>236</v>
+      </c>
+      <c r="G20" s="87" t="s">
+        <v>237</v>
+      </c>
+      <c r="I20" s="148">
+        <v>2</v>
+      </c>
+      <c r="J20" s="148" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A21" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" s="87" t="s">
+        <v>164</v>
+      </c>
+      <c r="G21" s="87" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21" s="148">
+        <v>3</v>
+      </c>
+      <c r="J21" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A22" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="87" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" s="87" t="s">
+        <v>190</v>
+      </c>
+      <c r="I22" s="148">
+        <v>4</v>
+      </c>
+      <c r="J22" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A23" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E23" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="87" t="s">
+        <v>161</v>
+      </c>
+      <c r="G23" s="87" t="s">
+        <v>191</v>
+      </c>
+      <c r="I23" s="148">
+        <v>5</v>
+      </c>
+      <c r="J23" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A24" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="87" t="s">
+        <v>163</v>
+      </c>
+      <c r="G24" s="87" t="s">
+        <v>192</v>
+      </c>
+      <c r="I24" s="148">
+        <v>6</v>
+      </c>
+      <c r="J24" s="148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A25" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="G25" s="87" t="s">
+        <v>255</v>
+      </c>
+      <c r="I25" s="148">
+        <v>7</v>
+      </c>
+      <c r="J25" s="148" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" s="15">
+        <v>43101</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="I26" s="148">
+        <v>8</v>
+      </c>
+      <c r="J26" s="148" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="1048569" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C1048569" s="148" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A26" xr:uid="{01F787D3-6455-7E4C-BD23-8A98F4ABA42E}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
@@ -16223,7 +17725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
@@ -16364,322 +17866,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AC6"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="30.5" customWidth="1"/>
-    <col min="6" max="6" width="38.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" customWidth="1"/>
-    <col min="9" max="9" width="29" customWidth="1"/>
-    <col min="10" max="10" width="26" style="19" customWidth="1"/>
-    <col min="11" max="11" width="28" style="19" customWidth="1"/>
-    <col min="12" max="12" width="27.5" style="19" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" style="19" customWidth="1"/>
-    <col min="14" max="14" width="68.5" style="19" customWidth="1"/>
-    <col min="15" max="15" width="25.5" style="19" customWidth="1"/>
-    <col min="16" max="16" width="20.5" customWidth="1"/>
-    <col min="17" max="17" width="27.5" customWidth="1"/>
-    <col min="18" max="19" width="7.1640625" style="2" customWidth="1"/>
-    <col min="20" max="29" width="7.1640625" customWidth="1"/>
-    <col min="30" max="1025" width="8.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-    </row>
-    <row r="2" spans="1:29" ht="98" x14ac:dyDescent="0.15">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="R2" s="41"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-    </row>
-    <row r="3" spans="1:29" ht="45" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="R3" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="S3" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="13"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
-      <c r="A4" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="130" t="s">
-        <v>208</v>
-      </c>
-      <c r="E4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G4" s="43">
-        <v>1</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="45"/>
-      <c r="P4" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
-      <c r="A5" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B5" s="39"/>
-      <c r="C5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="130" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G5" s="43">
-        <v>2</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="P5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
-      <c r="A6" s="15">
-        <v>43101</v>
-      </c>
-      <c r="B6" s="39"/>
-      <c r="C6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="130" t="s">
-        <v>180</v>
-      </c>
-      <c r="E6" t="s">
-        <v>181</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="G6" s="43">
-        <v>3</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0700-000000000000}">
-      <formula1>42736</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0700-000001000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G6" xr:uid="{00000000-0002-0000-0700-000002000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fields dateOfBirth, contactNumber, email and address are optional now
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitinprabhu/hmcts/platform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED8D925-8E4F-D340-8BB9-F824E074C6EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D9418C-D58C-4549-BEA2-DA35DB1937B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17240" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$L$10</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="272">
   <si>
     <t>Change History</t>
   </si>
@@ -890,6 +890,9 @@
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>Update CaseEventToFields tab. Fields dateOfBirth, contactNumber, email and address are optional now.</t>
   </si>
 </sst>
 </file>
@@ -2096,16 +2099,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="50.5" customWidth="1"/>
+    <col min="2" max="2" width="83" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -2425,6 +2428,32 @@
       <c r="E20" s="2" t="s">
         <v>185</v>
       </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="115">
+        <v>18</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6">
+        <v>43691</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B23" s="29"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B24" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -2445,8 +2474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2454,7 +2483,7 @@
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="13" style="43" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" style="24" customWidth="1"/>
@@ -2712,8 +2741,8 @@
         <v>4</v>
       </c>
       <c r="G7"/>
-      <c r="H7" s="56" t="s">
-        <v>182</v>
+      <c r="H7" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="I7" s="43">
         <v>1</v>
@@ -2747,8 +2776,8 @@
         <v>5</v>
       </c>
       <c r="G8"/>
-      <c r="H8" s="56" t="s">
-        <v>182</v>
+      <c r="H8" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="I8" s="43">
         <v>2</v>
@@ -2782,8 +2811,8 @@
         <v>6</v>
       </c>
       <c r="G9"/>
-      <c r="H9" s="56" t="s">
-        <v>182</v>
+      <c r="H9" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="I9" s="43">
         <v>2</v>
@@ -2817,8 +2846,8 @@
         <v>7</v>
       </c>
       <c r="G10"/>
-      <c r="H10" s="56" t="s">
-        <v>182</v>
+      <c r="H10" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="I10" s="43">
         <v>2</v>
@@ -16062,7 +16091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add coversheet and form to ScannedDocumentType fixed list
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_BULK_SCAN.template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitinprabhu/hmcts/platform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D9418C-D58C-4549-BEA2-DA35DB1937B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4630051-BC69-9242-9911-D2635C17B03E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$L$10</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="277">
   <si>
     <t>Change History</t>
   </si>
@@ -893,6 +893,21 @@
   </si>
   <si>
     <t>Update CaseEventToFields tab. Fields dateOfBirth, contactNumber, email and address are optional now.</t>
+  </si>
+  <si>
+    <t>Add coversheet and form to ScannedDocumentType</t>
+  </si>
+  <si>
+    <t>coversheet</t>
+  </si>
+  <si>
+    <t>Coversheet</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>Form</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1434,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1706,6 +1721,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="11"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="9" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -2101,8 +2117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A3" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2447,7 +2463,21 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B22" s="29"/>
+      <c r="A22" s="115">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="6">
+        <v>43721</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B23" s="29"/>
@@ -16091,8 +16121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16254,11 +16284,19 @@
       <c r="R5" s="5"/>
     </row>
     <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15"/>
+      <c r="A6" s="160">
+        <v>43101</v>
+      </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="34"/>
+      <c r="C6" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E6" t="s">
+        <v>274</v>
+      </c>
       <c r="F6" s="29"/>
       <c r="H6" s="5"/>
       <c r="I6" s="29"/>
@@ -16273,11 +16311,19 @@
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15"/>
+      <c r="A7" s="160">
+        <v>43101</v>
+      </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="34"/>
+      <c r="C7" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E7" t="s">
+        <v>276</v>
+      </c>
       <c r="F7" s="29"/>
       <c r="H7" s="5"/>
       <c r="I7" s="29"/>

</xml_diff>